<commit_message>
finished a) b) c) d)
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218E4E22-4A59-479C-95CD-84EFC89628E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0803E527-C54D-4051-B797-E0BA981A2987}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t xml:space="preserve">Liste der zu zeichnenden Zeigerdiagramme </t>
   </si>
@@ -168,13 +168,16 @@
   </si>
   <si>
     <t>müsste komplettes Bild mit Sin/Cos-Schwingung erstellt werden (selbe wie Nr.  1)</t>
+  </si>
+  <si>
+    <t>a) - d) wurden zu einem tikzpicture zusammengefasst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +216,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -537,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -592,6 +602,30 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -601,15 +635,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -622,22 +647,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -954,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -972,13 +983,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
       <c r="J2" s="12" t="s">
         <v>42</v>
       </c>
@@ -993,10 +1004,10 @@
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
@@ -1015,11 +1026,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="25"/>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="26" t="s">
         <v>3</v>
       </c>
@@ -1034,11 +1045,11 @@
       <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="22"/>
       <c r="H7" s="23" t="s">
         <v>11</v>
@@ -1051,11 +1062,11 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="33"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="5"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
@@ -1068,11 +1079,11 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="5"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
@@ -1083,11 +1094,11 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="5"/>
       <c r="H10" s="7" t="s">
         <v>12</v>
@@ -1098,25 +1109,27 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="43"/>
-      <c r="H11" s="15"/>
+      <c r="H11" s="15" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="5"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
@@ -1124,12 +1137,12 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="5"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="44"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
@@ -1137,12 +1150,12 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="5"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="44"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -1150,11 +1163,11 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="5"/>
       <c r="H15" s="15"/>
     </row>
@@ -1165,11 +1178,11 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="5"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1180,11 +1193,11 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38"/>
       <c r="G17" s="5"/>
       <c r="H17" s="15"/>
     </row>
@@ -1193,11 +1206,11 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="5"/>
       <c r="H18" s="7"/>
     </row>
@@ -1206,11 +1219,11 @@
         <v>13</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="30"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="38"/>
       <c r="G19" s="5"/>
       <c r="H19" s="15"/>
     </row>
@@ -1219,11 +1232,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="33"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
       <c r="G20" s="5"/>
       <c r="H20" s="7"/>
     </row>
@@ -1232,11 +1245,11 @@
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="38"/>
       <c r="G21" s="5"/>
       <c r="H21" s="15"/>
     </row>
@@ -1245,11 +1258,11 @@
         <v>16</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
       <c r="G22" s="5"/>
       <c r="H22" s="7"/>
     </row>
@@ -1258,11 +1271,11 @@
         <v>17</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="30"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
       <c r="G23" s="5"/>
       <c r="H23" s="15"/>
     </row>
@@ -1271,11 +1284,11 @@
         <v>18</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="31" t="s">
+      <c r="D24" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="32"/>
-      <c r="F24" s="33"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="5"/>
       <c r="H24" s="7"/>
     </row>
@@ -1284,11 +1297,11 @@
         <v>19</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="30"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38"/>
       <c r="G25" s="5"/>
       <c r="H25" s="15"/>
     </row>
@@ -1297,11 +1310,11 @@
         <v>20</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
       <c r="G26" s="5"/>
       <c r="H26" s="7"/>
     </row>
@@ -1310,11 +1323,11 @@
         <v>21</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="30"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="38"/>
       <c r="G27" s="5"/>
       <c r="H27" s="15"/>
     </row>
@@ -1323,11 +1336,11 @@
         <v>22</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="31" t="s">
+      <c r="D28" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="32"/>
-      <c r="F28" s="33"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="5"/>
       <c r="H28" s="7"/>
     </row>
@@ -1338,11 +1351,11 @@
       <c r="C29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="30"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="38"/>
       <c r="G29" s="5"/>
       <c r="H29" s="15" t="s">
         <v>45</v>
@@ -1355,11 +1368,11 @@
       <c r="C30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
       <c r="G30" s="5"/>
       <c r="H30" s="7" t="s">
         <v>11</v>
@@ -1370,11 +1383,11 @@
         <v>25</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
       <c r="G31" s="5"/>
       <c r="H31" s="15"/>
     </row>
@@ -1383,11 +1396,11 @@
         <v>26</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30"/>
       <c r="G32" s="5"/>
       <c r="H32" s="7"/>
     </row>
@@ -1396,11 +1409,11 @@
         <v>27</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="30"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="38"/>
       <c r="G33" s="5"/>
       <c r="H33" s="15"/>
     </row>
@@ -1409,11 +1422,11 @@
         <v>28</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="31" t="s">
+      <c r="D34" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="32"/>
-      <c r="F34" s="33"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="30"/>
       <c r="G34" s="5"/>
       <c r="H34" s="7"/>
     </row>
@@ -1422,11 +1435,11 @@
         <v>29</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="38"/>
       <c r="G35" s="5"/>
       <c r="H35" s="15"/>
     </row>
@@ -1435,11 +1448,11 @@
         <v>30</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
       <c r="G36" s="5"/>
       <c r="H36" s="7"/>
     </row>
@@ -1448,34 +1461,16 @@
         <v>31</v>
       </c>
       <c r="C37" s="17"/>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="18"/>
       <c r="H37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="D37:F37"/>
@@ -1492,6 +1487,24 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update status list, typo befehlsliste
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0803E527-C54D-4051-B797-E0BA981A2987}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B5465F8-120F-4EB3-8DB8-5D7EDA21E776}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -602,6 +602,17 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -611,6 +622,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -626,29 +649,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -966,7 +966,7 @@
   <dimension ref="B2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,13 +983,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="J2" s="12" t="s">
         <v>42</v>
       </c>
@@ -1004,10 +1004,10 @@
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
@@ -1026,11 +1026,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="25"/>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="26" t="s">
         <v>3</v>
       </c>
@@ -1045,11 +1045,11 @@
       <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="44"/>
       <c r="G7" s="22"/>
       <c r="H7" s="23" t="s">
         <v>11</v>
@@ -1062,11 +1062,11 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="5"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
@@ -1079,11 +1079,11 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="5"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
@@ -1094,11 +1094,11 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="5"/>
       <c r="H10" s="7" t="s">
         <v>12</v>
@@ -1109,12 +1109,12 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="43"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="15" t="s">
         <v>46</v>
       </c>
@@ -1124,11 +1124,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
@@ -1137,12 +1137,12 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="44"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
@@ -1150,12 +1150,12 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="44"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="29"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -1163,12 +1163,12 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="5"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="10"/>
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -1178,11 +1178,11 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="5"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1193,11 +1193,11 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
       <c r="G17" s="5"/>
       <c r="H17" s="15"/>
     </row>
@@ -1206,11 +1206,11 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="5"/>
       <c r="H18" s="7"/>
     </row>
@@ -1219,11 +1219,11 @@
         <v>13</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="36" t="s">
+      <c r="D19" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="38"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="5"/>
       <c r="H19" s="15"/>
     </row>
@@ -1232,11 +1232,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="30"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
       <c r="G20" s="5"/>
       <c r="H20" s="7"/>
     </row>
@@ -1245,11 +1245,11 @@
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="36" t="s">
+      <c r="D21" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="38"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
       <c r="G21" s="5"/>
       <c r="H21" s="15"/>
     </row>
@@ -1258,11 +1258,11 @@
         <v>16</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
       <c r="G22" s="5"/>
       <c r="H22" s="7"/>
     </row>
@@ -1271,11 +1271,11 @@
         <v>17</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="38"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
       <c r="G23" s="5"/>
       <c r="H23" s="15"/>
     </row>
@@ -1284,11 +1284,11 @@
         <v>18</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="35"/>
       <c r="G24" s="5"/>
       <c r="H24" s="7"/>
     </row>
@@ -1297,11 +1297,11 @@
         <v>19</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="37"/>
-      <c r="F25" s="38"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
       <c r="G25" s="5"/>
       <c r="H25" s="15"/>
     </row>
@@ -1310,11 +1310,11 @@
         <v>20</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
       <c r="G26" s="5"/>
       <c r="H26" s="7"/>
     </row>
@@ -1323,11 +1323,11 @@
         <v>21</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="37"/>
-      <c r="F27" s="38"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="5"/>
       <c r="H27" s="15"/>
     </row>
@@ -1336,11 +1336,11 @@
         <v>22</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="30"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
       <c r="G28" s="5"/>
       <c r="H28" s="7"/>
     </row>
@@ -1351,11 +1351,11 @@
       <c r="C29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="37"/>
-      <c r="F29" s="38"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
       <c r="G29" s="5"/>
       <c r="H29" s="15" t="s">
         <v>45</v>
@@ -1368,11 +1368,11 @@
       <c r="C30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="30"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="35"/>
       <c r="G30" s="5"/>
       <c r="H30" s="7" t="s">
         <v>11</v>
@@ -1383,11 +1383,11 @@
         <v>25</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="37"/>
-      <c r="F31" s="38"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="5"/>
       <c r="H31" s="15"/>
     </row>
@@ -1396,11 +1396,11 @@
         <v>26</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="35"/>
       <c r="G32" s="5"/>
       <c r="H32" s="7"/>
     </row>
@@ -1409,11 +1409,11 @@
         <v>27</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="37"/>
-      <c r="F33" s="38"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="5"/>
       <c r="H33" s="15"/>
     </row>
@@ -1422,11 +1422,11 @@
         <v>28</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="35"/>
       <c r="G34" s="5"/>
       <c r="H34" s="7"/>
     </row>
@@ -1435,11 +1435,11 @@
         <v>29</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="36" t="s">
+      <c r="D35" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="37"/>
-      <c r="F35" s="38"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="5"/>
       <c r="H35" s="15"/>
     </row>
@@ -1448,11 +1448,11 @@
         <v>30</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="30"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="35"/>
       <c r="G36" s="5"/>
       <c r="H36" s="7"/>
     </row>
@@ -1461,16 +1461,34 @@
         <v>31</v>
       </c>
       <c r="C37" s="17"/>
-      <c r="D37" s="39" t="s">
+      <c r="D37" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="40"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="18"/>
       <c r="H37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="D37:F37"/>
@@ -1487,24 +1505,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished Zeigerdiagramm II a)
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9659B6-FD3C-4CAB-9594-62466A4FE949}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE0CA50-8427-4A93-B6D4-4A577395016F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -604,6 +604,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -613,6 +622,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -626,27 +647,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,13 +983,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
       <c r="J2" s="12" t="s">
         <v>42</v>
       </c>
@@ -1004,10 +1004,10 @@
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
@@ -1026,11 +1026,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="25"/>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="26" t="s">
         <v>3</v>
       </c>
@@ -1045,11 +1045,11 @@
       <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="44"/>
       <c r="G7" s="22"/>
       <c r="H7" s="23" t="s">
         <v>11</v>
@@ -1062,11 +1062,11 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="35"/>
       <c r="G8" s="5"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
@@ -1079,12 +1079,12 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="10"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="11"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
       </c>
@@ -1094,12 +1094,12 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="5"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="35"/>
+      <c r="G10" s="10"/>
       <c r="H10" s="7" t="s">
         <v>12</v>
       </c>
@@ -1109,11 +1109,11 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="28"/>
       <c r="H11" s="15" t="s">
         <v>46</v>
@@ -1124,11 +1124,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="35"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
@@ -1137,11 +1137,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="38" t="s">
+      <c r="D13" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="39"/>
-      <c r="F13" s="40"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="32"/>
       <c r="G13" s="29"/>
       <c r="H13" s="15"/>
     </row>
@@ -1150,11 +1150,11 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
       <c r="G14" s="29"/>
       <c r="H14" s="7"/>
     </row>
@@ -1163,11 +1163,11 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="38" t="s">
+      <c r="D15" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="39"/>
-      <c r="F15" s="40"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="32"/>
       <c r="G15" s="29"/>
       <c r="H15" s="15"/>
     </row>
@@ -1178,11 +1178,11 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="5"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1193,11 +1193,11 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="39"/>
-      <c r="F17" s="40"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
       <c r="G17" s="5"/>
       <c r="H17" s="15"/>
     </row>
@@ -1206,11 +1206,11 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="35"/>
       <c r="G18" s="5"/>
       <c r="H18" s="7"/>
     </row>
@@ -1219,11 +1219,11 @@
         <v>13</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="5"/>
       <c r="H19" s="15"/>
     </row>
@@ -1232,11 +1232,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="35"/>
       <c r="G20" s="5"/>
       <c r="H20" s="7"/>
     </row>
@@ -1245,11 +1245,11 @@
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
       <c r="G21" s="5"/>
       <c r="H21" s="15"/>
     </row>
@@ -1258,11 +1258,11 @@
         <v>16</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
       <c r="G22" s="5"/>
       <c r="H22" s="7"/>
     </row>
@@ -1271,11 +1271,11 @@
         <v>17</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="32"/>
       <c r="G23" s="5"/>
       <c r="H23" s="15"/>
     </row>
@@ -1284,11 +1284,11 @@
         <v>18</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="35"/>
       <c r="G24" s="5"/>
       <c r="H24" s="7"/>
     </row>
@@ -1297,11 +1297,11 @@
         <v>19</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="32"/>
       <c r="G25" s="5"/>
       <c r="H25" s="15"/>
     </row>
@@ -1310,11 +1310,11 @@
         <v>20</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="35"/>
       <c r="G26" s="5"/>
       <c r="H26" s="7"/>
     </row>
@@ -1323,11 +1323,11 @@
         <v>21</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="5"/>
       <c r="H27" s="15"/>
     </row>
@@ -1336,11 +1336,11 @@
         <v>22</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="35"/>
       <c r="G28" s="5"/>
       <c r="H28" s="7"/>
     </row>
@@ -1351,11 +1351,11 @@
       <c r="C29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="40"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="32"/>
       <c r="G29" s="5"/>
       <c r="H29" s="15" t="s">
         <v>45</v>
@@ -1368,11 +1368,11 @@
       <c r="C30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="32"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="35"/>
       <c r="G30" s="5"/>
       <c r="H30" s="7" t="s">
         <v>11</v>
@@ -1383,11 +1383,11 @@
         <v>25</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="40"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="5"/>
       <c r="H31" s="15"/>
     </row>
@@ -1396,11 +1396,11 @@
         <v>26</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="32"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="35"/>
       <c r="G32" s="5"/>
       <c r="H32" s="7"/>
     </row>
@@ -1409,11 +1409,11 @@
         <v>27</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="40"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="5"/>
       <c r="H33" s="15"/>
     </row>
@@ -1422,11 +1422,11 @@
         <v>28</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="35"/>
       <c r="G34" s="5"/>
       <c r="H34" s="7"/>
     </row>
@@ -1435,11 +1435,11 @@
         <v>29</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="40"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="5"/>
       <c r="H35" s="15"/>
     </row>
@@ -1448,11 +1448,11 @@
         <v>30</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="35"/>
       <c r="G36" s="5"/>
       <c r="H36" s="7"/>
     </row>
@@ -1461,16 +1461,34 @@
         <v>31</v>
       </c>
       <c r="C37" s="17"/>
-      <c r="D37" s="41" t="s">
+      <c r="D37" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="E37" s="42"/>
-      <c r="F37" s="43"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="38"/>
       <c r="G37" s="18"/>
       <c r="H37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="D37:F37"/>
@@ -1487,24 +1505,6 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished Zeigerdiagramm II b)
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE0CA50-8427-4A93-B6D4-4A577395016F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6319EE5-DDD7-4EF0-9B99-74C359C05C5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -68,9 +68,6 @@
     <t>müsste komplettes Bild mit Sin/Cos-Schwingung erstellt werden</t>
   </si>
   <si>
-    <t>ohne Sin/Cos-Schwingung</t>
-  </si>
-  <si>
     <t>Zeigerdiagramm II b)</t>
   </si>
   <si>
@@ -171,23 +168,19 @@
   </si>
   <si>
     <t>a) - d) wurden zu einem tikzpicture zusammengefasst</t>
+  </si>
+  <si>
+    <t>mit Sin/Cos-Schwingung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -547,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -570,8 +563,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -592,18 +585,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -613,15 +629,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -631,22 +638,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -966,7 +958,7 @@
   <dimension ref="B2:K37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -983,58 +975,58 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="J2" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="J3" s="9"/>
       <c r="K3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="C4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J5" s="11"/>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="41" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="26" t="s">
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="26" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1045,13 +1037,13 @@
       <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="42" t="s">
+      <c r="D7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="23" t="s">
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="22" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1062,11 +1054,11 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="35"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="5"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
@@ -1079,11 +1071,11 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="11"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
@@ -1094,14 +1086,14 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="10"/>
+      <c r="D10" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="11"/>
       <c r="H10" s="7" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
@@ -1109,14 +1101,14 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="28"/>
+      <c r="D11" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
@@ -1124,11 +1116,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
+      <c r="D12" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
@@ -1137,12 +1129,12 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="29"/>
+      <c r="D13" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
@@ -1150,12 +1142,12 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="34"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="29"/>
+      <c r="D14" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -1163,12 +1155,12 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="29"/>
+      <c r="D15" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -1178,11 +1170,11 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="35"/>
+      <c r="D16" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
       <c r="G16" s="5"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1193,11 +1185,11 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
+      <c r="D17" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="38"/>
+      <c r="F17" s="39"/>
       <c r="G17" s="5"/>
       <c r="H17" s="15"/>
     </row>
@@ -1206,11 +1198,11 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
+      <c r="D18" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="5"/>
       <c r="H18" s="7"/>
     </row>
@@ -1219,11 +1211,11 @@
         <v>13</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="32"/>
+      <c r="D19" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="38"/>
+      <c r="F19" s="39"/>
       <c r="G19" s="5"/>
       <c r="H19" s="15"/>
     </row>
@@ -1232,11 +1224,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="35"/>
+      <c r="D20" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="5"/>
       <c r="H20" s="7"/>
     </row>
@@ -1245,11 +1237,11 @@
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
+      <c r="D21" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="38"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="5"/>
       <c r="H21" s="15"/>
     </row>
@@ -1258,11 +1250,11 @@
         <v>16</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
+      <c r="D22" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="5"/>
       <c r="H22" s="7"/>
     </row>
@@ -1271,11 +1263,11 @@
         <v>17</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
+      <c r="D23" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="5"/>
       <c r="H23" s="15"/>
     </row>
@@ -1284,11 +1276,11 @@
         <v>18</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
+      <c r="D24" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="5"/>
       <c r="H24" s="7"/>
     </row>
@@ -1297,11 +1289,11 @@
         <v>19</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
+      <c r="D25" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="38"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="5"/>
       <c r="H25" s="15"/>
     </row>
@@ -1310,11 +1302,11 @@
         <v>20</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
+      <c r="D26" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="30"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="5"/>
       <c r="H26" s="7"/>
     </row>
@@ -1323,11 +1315,11 @@
         <v>21</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
+      <c r="D27" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="E27" s="38"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="5"/>
       <c r="H27" s="15"/>
     </row>
@@ -1336,11 +1328,11 @@
         <v>22</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
+      <c r="D28" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="5"/>
       <c r="H28" s="7"/>
     </row>
@@ -1351,14 +1343,14 @@
       <c r="C29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
+      <c r="D29" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="38"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="5"/>
       <c r="H29" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -1368,11 +1360,11 @@
       <c r="C30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E30" s="34"/>
-      <c r="F30" s="35"/>
+      <c r="D30" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="30"/>
+      <c r="F30" s="31"/>
       <c r="G30" s="5"/>
       <c r="H30" s="7" t="s">
         <v>11</v>
@@ -1383,11 +1375,11 @@
         <v>25</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="32"/>
+      <c r="D31" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" s="38"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="5"/>
       <c r="H31" s="15"/>
     </row>
@@ -1396,11 +1388,11 @@
         <v>26</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="35"/>
+      <c r="D32" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="30"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="5"/>
       <c r="H32" s="7"/>
     </row>
@@ -1409,11 +1401,11 @@
         <v>27</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="32"/>
+      <c r="D33" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="38"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="5"/>
       <c r="H33" s="15"/>
     </row>
@@ -1422,11 +1414,11 @@
         <v>28</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="34"/>
-      <c r="F34" s="35"/>
+      <c r="D34" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="30"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="5"/>
       <c r="H34" s="7"/>
     </row>
@@ -1435,11 +1427,11 @@
         <v>29</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="32"/>
+      <c r="D35" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="38"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="5"/>
       <c r="H35" s="15"/>
     </row>
@@ -1448,11 +1440,11 @@
         <v>30</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="35"/>
+      <c r="D36" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="30"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="5"/>
       <c r="H36" s="7"/>
     </row>
@@ -1461,34 +1453,16 @@
         <v>31</v>
       </c>
       <c r="C37" s="17"/>
-      <c r="D37" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" s="37"/>
-      <c r="F37" s="38"/>
+      <c r="D37" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="E37" s="41"/>
+      <c r="F37" s="42"/>
       <c r="G37" s="18"/>
       <c r="H37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="D37:F37"/>
@@ -1505,6 +1479,24 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished IV a), b) - Started IV c)
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21841958-BA92-45BB-8065-F2D4E731634A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDF486D-60B4-4EBE-B087-25A446CE3834}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -596,6 +596,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -605,15 +629,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -624,21 +639,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,13 +975,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="J2" s="12" t="s">
         <v>41</v>
       </c>
@@ -996,10 +996,10 @@
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="39"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
@@ -1018,11 +1018,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="24"/>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="25" t="s">
         <v>3</v>
       </c>
@@ -1037,11 +1037,11 @@
       <c r="C7" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="43"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="27"/>
       <c r="H7" s="22" t="s">
         <v>11</v>
@@ -1054,11 +1054,11 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
       <c r="G8" s="27"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
@@ -1071,11 +1071,11 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="11"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
@@ -1086,12 +1086,12 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="11"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1101,11 +1101,11 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="27"/>
       <c r="H11" s="15" t="s">
         <v>45</v>
@@ -1116,11 +1116,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="33"/>
-      <c r="F12" s="34"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
@@ -1129,11 +1129,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="39"/>
       <c r="G13" s="28"/>
       <c r="H13" s="15"/>
     </row>
@@ -1142,11 +1142,11 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="33"/>
-      <c r="F14" s="34"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
       <c r="G14" s="28"/>
       <c r="H14" s="7"/>
     </row>
@@ -1155,11 +1155,11 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
       <c r="G15" s="28"/>
       <c r="H15" s="15"/>
     </row>
@@ -1170,12 +1170,12 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="5"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
       </c>
@@ -1185,12 +1185,12 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="5"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="28"/>
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -1198,12 +1198,12 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="5"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="10"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
@@ -1211,11 +1211,11 @@
         <v>13</v>
       </c>
       <c r="C19" s="8"/>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="39"/>
       <c r="G19" s="5"/>
       <c r="H19" s="15"/>
     </row>
@@ -1224,11 +1224,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="32" t="s">
+      <c r="D20" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="5"/>
       <c r="H20" s="7"/>
     </row>
@@ -1237,11 +1237,11 @@
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="5"/>
       <c r="H21" s="15"/>
     </row>
@@ -1250,11 +1250,11 @@
         <v>16</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="5"/>
       <c r="H22" s="7"/>
     </row>
@@ -1263,11 +1263,11 @@
         <v>17</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="5"/>
       <c r="H23" s="15"/>
     </row>
@@ -1276,11 +1276,11 @@
         <v>18</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="5"/>
       <c r="H24" s="7"/>
     </row>
@@ -1289,11 +1289,11 @@
         <v>19</v>
       </c>
       <c r="C25" s="8"/>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="39"/>
       <c r="G25" s="5"/>
       <c r="H25" s="15"/>
     </row>
@@ -1302,11 +1302,11 @@
         <v>20</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="5"/>
       <c r="H26" s="7"/>
     </row>
@@ -1315,11 +1315,11 @@
         <v>21</v>
       </c>
       <c r="C27" s="8"/>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="5"/>
       <c r="H27" s="15"/>
     </row>
@@ -1328,11 +1328,11 @@
         <v>22</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="32" t="s">
+      <c r="D28" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="5"/>
       <c r="H28" s="7"/>
     </row>
@@ -1343,11 +1343,11 @@
       <c r="C29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="5"/>
       <c r="H29" s="15" t="s">
         <v>44</v>
@@ -1360,11 +1360,11 @@
       <c r="C30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="31"/>
       <c r="G30" s="5"/>
       <c r="H30" s="7" t="s">
         <v>11</v>
@@ -1375,11 +1375,11 @@
         <v>25</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="31"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="39"/>
       <c r="G31" s="5"/>
       <c r="H31" s="15"/>
     </row>
@@ -1388,11 +1388,11 @@
         <v>26</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="33"/>
-      <c r="F32" s="34"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="5"/>
       <c r="H32" s="7"/>
     </row>
@@ -1401,11 +1401,11 @@
         <v>27</v>
       </c>
       <c r="C33" s="8"/>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="5"/>
       <c r="H33" s="15"/>
     </row>
@@ -1414,11 +1414,11 @@
         <v>28</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="32" t="s">
+      <c r="D34" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="5"/>
       <c r="H34" s="7"/>
     </row>
@@ -1427,11 +1427,11 @@
         <v>29</v>
       </c>
       <c r="C35" s="8"/>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="30"/>
-      <c r="F35" s="31"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="5"/>
       <c r="H35" s="15"/>
     </row>
@@ -1440,11 +1440,11 @@
         <v>30</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="32" t="s">
+      <c r="D36" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="33"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="5"/>
       <c r="H36" s="7"/>
     </row>
@@ -1453,34 +1453,16 @@
         <v>31</v>
       </c>
       <c r="C37" s="17"/>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="37"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="42"/>
       <c r="G37" s="18"/>
       <c r="H37" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
     <mergeCell ref="D35:F35"/>
     <mergeCell ref="D36:F36"/>
     <mergeCell ref="D37:F37"/>
@@ -1497,6 +1479,24 @@
     <mergeCell ref="D26:F26"/>
     <mergeCell ref="D27:F27"/>
     <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished IV c), Widerst b) & c)
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDF486D-60B4-4EBE-B087-25A446CE3834}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E146EA-E884-4ABD-855C-9621B9852BBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t xml:space="preserve">Liste der zu zeichnenden Zeigerdiagramme </t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>mit Sin/Cos-Schwingung</t>
+  </si>
+  <si>
+    <t>Widertsand im Wechselstromkreis b)</t>
   </si>
 </sst>
 </file>
@@ -249,7 +252,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -371,21 +374,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -540,7 +528,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,30 +560,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -605,10 +599,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -618,27 +624,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -955,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
-  <dimension ref="B2:K37"/>
+  <dimension ref="B2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -975,13 +960,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="J2" s="12" t="s">
         <v>41</v>
       </c>
@@ -996,10 +981,10 @@
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
@@ -1014,36 +999,36 @@
       </c>
     </row>
     <row r="6" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="33" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="25" t="s">
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <v>1</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="22" t="s">
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="21" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1054,12 +1039,12 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="27"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
       </c>
@@ -1071,11 +1056,11 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="11"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
@@ -1086,12 +1071,12 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="28"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="7" t="s">
         <v>46</v>
       </c>
@@ -1101,12 +1086,12 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="27"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="15" t="s">
         <v>45</v>
       </c>
@@ -1116,11 +1101,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
@@ -1129,12 +1114,12 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="28"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="15"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
@@ -1142,12 +1127,12 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="29" t="s">
+      <c r="D14" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="28"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
@@ -1155,12 +1140,12 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="28"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="15"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
@@ -1170,12 +1155,12 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="28"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
       </c>
@@ -1185,12 +1170,12 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="15"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
@@ -1198,288 +1183,291 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="29" t="s">
+      <c r="D18" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="10"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="27"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="14">
+      <c r="B19" s="6">
         <v>13</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="15"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="6">
         <v>14</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="29" t="s">
+      <c r="C20" s="8"/>
+      <c r="D20" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="6">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="30"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="7"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="14">
-        <v>15</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="15"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <v>16</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="29" t="s">
+      <c r="C22" s="8"/>
+      <c r="D22" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="6">
+        <v>17</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="14">
-        <v>17</v>
-      </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="37" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="39"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="15"/>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="6">
         <v>18</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="29" t="s">
+      <c r="C24" s="8"/>
+      <c r="D24" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="29"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="15"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="6">
+        <v>19</v>
+      </c>
+      <c r="C25" s="4"/>
+      <c r="D25" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="7"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="14">
-        <v>19</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="37" t="s">
-        <v>27</v>
-      </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="15"/>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="6">
         <v>20</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="29" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="15"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="6">
+        <v>21</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="14">
-        <v>21</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="39"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="15"/>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="6">
         <v>22</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="29" t="s">
+      <c r="C28" s="8"/>
+      <c r="D28" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="6">
+        <v>23</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="14">
-        <v>23</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
       <c r="G29" s="5"/>
-      <c r="H29" s="15" t="s">
-        <v>44</v>
-      </c>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="6">
         <v>24</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="29" t="s">
+      <c r="D30" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="6">
+        <v>25</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E30" s="30"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="7" t="s">
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="14">
-        <v>25</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31" s="38"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>26</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="29" t="s">
+      <c r="C32" s="8"/>
+      <c r="D32" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="15"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="6">
+        <v>27</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E32" s="30"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="7"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="14">
-        <v>27</v>
-      </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="39"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
       <c r="G33" s="5"/>
-      <c r="H33" s="15"/>
+      <c r="H33" s="7"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>28</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="29" t="s">
+      <c r="C34" s="8"/>
+      <c r="D34" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="29"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="15"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="6">
+        <v>29</v>
+      </c>
+      <c r="C35" s="4"/>
+      <c r="D35" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="7"/>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="14">
-        <v>29</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="E35" s="38"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
       <c r="G35" s="5"/>
-      <c r="H35" s="15"/>
+      <c r="H35" s="7"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
         <v>30</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="29" t="s">
+      <c r="C36" s="8"/>
+      <c r="D36" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="15"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="6">
+        <v>31</v>
+      </c>
+      <c r="C37" s="4"/>
+      <c r="D37" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="30"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="7"/>
-    </row>
-    <row r="37" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="16">
-        <v>31</v>
-      </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="40" t="s">
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="7"/>
+    </row>
+    <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="6">
+        <v>32</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="19"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
+  <mergeCells count="35">
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
     <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D22:F22"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
@@ -1488,15 +1476,26 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished up to Konstruktion...b)
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E146EA-E884-4ABD-855C-9621B9852BBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D241ECA-CFD0-47DE-B797-FBB89BD7100F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="50">
   <si>
     <t xml:space="preserve">Liste der zu zeichnenden Zeigerdiagramme </t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>Widertsand im Wechselstromkreis b)</t>
+  </si>
+  <si>
+    <t>Induktivität im Wechselstromkreis b)</t>
+  </si>
+  <si>
+    <t>Kondensator im Wechselstromkreis b)</t>
   </si>
 </sst>
 </file>
@@ -581,6 +587,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -590,15 +620,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -609,21 +630,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -940,10 +946,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
-  <dimension ref="B2:K38"/>
+  <dimension ref="B2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,13 +966,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
       <c r="J2" s="12" t="s">
         <v>41</v>
       </c>
@@ -981,10 +987,10 @@
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
@@ -1003,11 +1009,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="23"/>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="24" t="s">
         <v>3</v>
       </c>
@@ -1022,11 +1028,11 @@
       <c r="C7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="26"/>
       <c r="H7" s="21" t="s">
         <v>11</v>
@@ -1039,11 +1045,11 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="33"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="26"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
@@ -1056,11 +1062,11 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="11"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
@@ -1071,11 +1077,11 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="27"/>
       <c r="H10" s="7" t="s">
         <v>46</v>
@@ -1086,11 +1092,11 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="26"/>
       <c r="H11" s="15" t="s">
         <v>45</v>
@@ -1101,11 +1107,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
@@ -1114,11 +1120,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
       <c r="G13" s="27"/>
       <c r="H13" s="15"/>
     </row>
@@ -1127,11 +1133,11 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="27"/>
       <c r="H14" s="7"/>
     </row>
@@ -1140,11 +1146,11 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="27"/>
       <c r="H15" s="15"/>
     </row>
@@ -1155,11 +1161,11 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="27"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1170,11 +1176,11 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38"/>
       <c r="G17" s="27"/>
       <c r="H17" s="15"/>
     </row>
@@ -1183,11 +1189,11 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="27"/>
       <c r="H18" s="7"/>
     </row>
@@ -1196,11 +1202,11 @@
         <v>13</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="27"/>
       <c r="H19" s="7"/>
     </row>
@@ -1209,11 +1215,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="30"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
       <c r="G20" s="27"/>
       <c r="H20" s="15"/>
     </row>
@@ -1221,39 +1227,39 @@
       <c r="B21" s="6">
         <v>15</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="15"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="6">
         <v>16</v>
       </c>
-      <c r="C22" s="8"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E22" s="29"/>
       <c r="F22" s="30"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="15"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="6">
         <v>17</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="5"/>
+      <c r="D23" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="7"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
@@ -1261,12 +1267,12 @@
         <v>18</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="5"/>
+      <c r="D24" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="37"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="15"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
@@ -1274,12 +1280,12 @@
         <v>19</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="5"/>
+      <c r="D25" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="7"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
@@ -1287,11 +1293,11 @@
         <v>20</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30"/>
+      <c r="D26" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
       <c r="G26" s="5"/>
       <c r="H26" s="15"/>
     </row>
@@ -1300,11 +1306,11 @@
         <v>21</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
+      <c r="D27" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="29"/>
+      <c r="F27" s="30"/>
       <c r="G27" s="5"/>
       <c r="H27" s="7"/>
     </row>
@@ -1313,11 +1319,11 @@
         <v>22</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="30"/>
+      <c r="D28" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="37"/>
+      <c r="F28" s="38"/>
       <c r="G28" s="5"/>
       <c r="H28" s="15"/>
     </row>
@@ -1326,11 +1332,11 @@
         <v>23</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
+      <c r="D29" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="29"/>
+      <c r="F29" s="30"/>
       <c r="G29" s="5"/>
       <c r="H29" s="7"/>
     </row>
@@ -1338,72 +1344,72 @@
       <c r="B30" s="6">
         <v>24</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="30"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
       <c r="G30" s="5"/>
-      <c r="H30" s="15" t="s">
-        <v>44</v>
-      </c>
+      <c r="H30" s="15"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="6">
         <v>25</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="E31" s="29"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="H31" s="7"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="6">
         <v>26</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30"/>
+      <c r="C32" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="5"/>
-      <c r="H32" s="15"/>
+      <c r="H32" s="15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="6">
         <v>27</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
+      <c r="C33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="29"/>
+      <c r="F33" s="30"/>
       <c r="G33" s="5"/>
-      <c r="H33" s="7"/>
+      <c r="H33" s="7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="6">
         <v>28</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30"/>
+      <c r="D34" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E34" s="37"/>
+      <c r="F34" s="38"/>
       <c r="G34" s="5"/>
       <c r="H34" s="15"/>
     </row>
@@ -1412,11 +1418,11 @@
         <v>29</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
+      <c r="D35" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="29"/>
+      <c r="F35" s="30"/>
       <c r="G35" s="5"/>
       <c r="H35" s="7"/>
     </row>
@@ -1425,11 +1431,11 @@
         <v>30</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="30"/>
+      <c r="D36" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="E36" s="37"/>
+      <c r="F36" s="38"/>
       <c r="G36" s="5"/>
       <c r="H36" s="15"/>
     </row>
@@ -1438,36 +1444,72 @@
         <v>31</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
+      <c r="D37" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="29"/>
+      <c r="F37" s="30"/>
       <c r="G37" s="5"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="6">
         <v>32</v>
       </c>
-      <c r="C38" s="16"/>
-      <c r="D38" s="34" t="s">
+      <c r="C38" s="8"/>
+      <c r="D38" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="37"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="15"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="6">
+        <v>33</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E39" s="29"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="6">
+        <v>34</v>
+      </c>
+      <c r="C40" s="16"/>
+      <c r="D40" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="18"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D23:F23"/>
+  <mergeCells count="37">
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D40:F40"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D25:F25"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="D13:F13"/>
@@ -1477,25 +1519,17 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D19:F19"/>
     <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished up to Rechenop...d)
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D241ECA-CFD0-47DE-B797-FBB89BD7100F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2F1D83-CFB1-4336-BC42-6EC34DC6DD74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t xml:space="preserve">Liste der zu zeichnenden Zeigerdiagramme </t>
   </si>
@@ -587,6 +587,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -596,6 +605,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,27 +630,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,13 +966,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="J2" s="12" t="s">
         <v>41</v>
       </c>
@@ -987,10 +987,10 @@
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
@@ -1009,11 +1009,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="23"/>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="24" t="s">
         <v>3</v>
       </c>
@@ -1028,11 +1028,11 @@
       <c r="C7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="26"/>
       <c r="H7" s="21" t="s">
         <v>11</v>
@@ -1045,11 +1045,11 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="26"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
@@ -1062,11 +1062,11 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="11"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
@@ -1077,11 +1077,11 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="27"/>
       <c r="H10" s="7" t="s">
         <v>46</v>
@@ -1092,11 +1092,11 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="26"/>
       <c r="H11" s="15" t="s">
         <v>45</v>
@@ -1107,11 +1107,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
@@ -1120,11 +1120,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="27"/>
       <c r="H13" s="15"/>
     </row>
@@ -1133,11 +1133,11 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
       <c r="G14" s="27"/>
       <c r="H14" s="7"/>
     </row>
@@ -1146,11 +1146,11 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="27"/>
       <c r="H15" s="15"/>
     </row>
@@ -1161,11 +1161,11 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="27"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1176,11 +1176,11 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="27"/>
       <c r="H17" s="15"/>
     </row>
@@ -1189,11 +1189,11 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="27"/>
       <c r="H18" s="7"/>
     </row>
@@ -1202,11 +1202,11 @@
         <v>13</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="30"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
       <c r="G19" s="27"/>
       <c r="H19" s="7"/>
     </row>
@@ -1215,11 +1215,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
       <c r="G20" s="27"/>
       <c r="H20" s="15"/>
     </row>
@@ -1228,11 +1228,11 @@
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="27"/>
       <c r="H21" s="15"/>
     </row>
@@ -1241,11 +1241,11 @@
         <v>16</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
       <c r="G22" s="27"/>
       <c r="H22" s="7"/>
     </row>
@@ -1254,11 +1254,11 @@
         <v>17</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="38"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="27"/>
       <c r="H23" s="7"/>
     </row>
@@ -1267,11 +1267,11 @@
         <v>18</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="38"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="27"/>
       <c r="H24" s="15"/>
     </row>
@@ -1280,11 +1280,11 @@
         <v>19</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="30"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="27"/>
       <c r="H25" s="7"/>
     </row>
@@ -1293,12 +1293,12 @@
         <v>20</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="5"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="27"/>
       <c r="H26" s="15"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
@@ -1306,12 +1306,12 @@
         <v>21</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="5"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
@@ -1319,12 +1319,12 @@
         <v>22</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="5"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="27"/>
       <c r="H28" s="15"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
@@ -1332,12 +1332,12 @@
         <v>23</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="5"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="27"/>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
@@ -1345,12 +1345,12 @@
         <v>24</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="36" t="s">
+      <c r="D30" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="37"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="5"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="10"/>
       <c r="H30" s="15"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
@@ -1358,11 +1358,11 @@
         <v>25</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="5"/>
       <c r="H31" s="7"/>
     </row>
@@ -1373,11 +1373,11 @@
       <c r="C32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="37"/>
-      <c r="F32" s="38"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30"/>
       <c r="G32" s="5"/>
       <c r="H32" s="15" t="s">
         <v>44</v>
@@ -1390,11 +1390,11 @@
       <c r="C33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="30"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
       <c r="G33" s="5"/>
       <c r="H33" s="7" t="s">
         <v>11</v>
@@ -1405,11 +1405,11 @@
         <v>28</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="36" t="s">
+      <c r="D34" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="37"/>
-      <c r="F34" s="38"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="30"/>
       <c r="G34" s="5"/>
       <c r="H34" s="15"/>
     </row>
@@ -1418,11 +1418,11 @@
         <v>29</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
       <c r="G35" s="5"/>
       <c r="H35" s="7"/>
     </row>
@@ -1431,11 +1431,11 @@
         <v>30</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="37"/>
-      <c r="F36" s="38"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
       <c r="G36" s="5"/>
       <c r="H36" s="15"/>
     </row>
@@ -1444,11 +1444,11 @@
         <v>31</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="30"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="5"/>
       <c r="H37" s="7"/>
     </row>
@@ -1457,11 +1457,11 @@
         <v>32</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="37"/>
-      <c r="F38" s="38"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="30"/>
       <c r="G38" s="5"/>
       <c r="H38" s="15"/>
     </row>
@@ -1470,11 +1470,11 @@
         <v>33</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="28" t="s">
+      <c r="D39" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="30"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
       <c r="G39" s="5"/>
       <c r="H39" s="7"/>
     </row>
@@ -1483,16 +1483,37 @@
         <v>34</v>
       </c>
       <c r="C40" s="16"/>
-      <c r="D40" s="39" t="s">
+      <c r="D40" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="36"/>
       <c r="G40" s="17"/>
       <c r="H40" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D23:F23"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="D40:F40"/>
@@ -1509,27 +1530,6 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finisched up to Komplex... a)
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2F1D83-CFB1-4336-BC42-6EC34DC6DD74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD30DD2-FA3A-4FCA-AB02-23D3D97547D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -587,6 +587,30 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -596,15 +620,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -615,21 +630,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,13 +966,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
       <c r="J2" s="12" t="s">
         <v>41</v>
       </c>
@@ -987,10 +987,10 @@
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
@@ -1009,11 +1009,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="23"/>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="24" t="s">
         <v>3</v>
       </c>
@@ -1028,11 +1028,11 @@
       <c r="C7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="41"/>
-      <c r="F7" s="42"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="26"/>
       <c r="H7" s="21" t="s">
         <v>11</v>
@@ -1045,11 +1045,11 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="33"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="26"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
@@ -1062,11 +1062,11 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="D9" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="30"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
       <c r="G9" s="11"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
@@ -1077,11 +1077,11 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="33"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="27"/>
       <c r="H10" s="7" t="s">
         <v>46</v>
@@ -1092,11 +1092,11 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="26"/>
       <c r="H11" s="15" t="s">
         <v>45</v>
@@ -1107,11 +1107,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="31" t="s">
+      <c r="D12" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="33"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
@@ -1120,11 +1120,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="38"/>
       <c r="G13" s="27"/>
       <c r="H13" s="15"/>
     </row>
@@ -1133,11 +1133,11 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="33"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="27"/>
       <c r="H14" s="7"/>
     </row>
@@ -1146,11 +1146,11 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
       <c r="G15" s="27"/>
       <c r="H15" s="15"/>
     </row>
@@ -1161,11 +1161,11 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="33"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="27"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1176,11 +1176,11 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="38"/>
       <c r="G17" s="27"/>
       <c r="H17" s="15"/>
     </row>
@@ -1189,11 +1189,11 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="31" t="s">
+      <c r="D18" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="33"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="27"/>
       <c r="H18" s="7"/>
     </row>
@@ -1202,11 +1202,11 @@
         <v>13</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
       <c r="G19" s="27"/>
       <c r="H19" s="7"/>
     </row>
@@ -1215,11 +1215,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="30"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="38"/>
       <c r="G20" s="27"/>
       <c r="H20" s="15"/>
     </row>
@@ -1228,11 +1228,11 @@
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="30"/>
       <c r="G21" s="27"/>
       <c r="H21" s="15"/>
     </row>
@@ -1241,11 +1241,11 @@
         <v>16</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
       <c r="G22" s="27"/>
       <c r="H22" s="7"/>
     </row>
@@ -1254,11 +1254,11 @@
         <v>17</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="30"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
       <c r="G23" s="27"/>
       <c r="H23" s="7"/>
     </row>
@@ -1267,11 +1267,11 @@
         <v>18</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="38"/>
       <c r="G24" s="27"/>
       <c r="H24" s="15"/>
     </row>
@@ -1280,11 +1280,11 @@
         <v>19</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="30"/>
       <c r="G25" s="27"/>
       <c r="H25" s="7"/>
     </row>
@@ -1293,11 +1293,11 @@
         <v>20</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="28" t="s">
+      <c r="D26" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="29"/>
-      <c r="F26" s="30"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
       <c r="G26" s="27"/>
       <c r="H26" s="15"/>
     </row>
@@ -1306,11 +1306,11 @@
         <v>21</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="30"/>
       <c r="G27" s="27"/>
       <c r="H27" s="7"/>
     </row>
@@ -1319,11 +1319,11 @@
         <v>22</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="29"/>
-      <c r="F28" s="30"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="38"/>
       <c r="G28" s="27"/>
       <c r="H28" s="15"/>
     </row>
@@ -1332,11 +1332,11 @@
         <v>23</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="30"/>
       <c r="G29" s="27"/>
       <c r="H29" s="7"/>
     </row>
@@ -1345,12 +1345,12 @@
         <v>24</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="29"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="10"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="27"/>
       <c r="H30" s="15"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
@@ -1358,12 +1358,12 @@
         <v>25</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="5"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="27"/>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
@@ -1373,11 +1373,11 @@
       <c r="C32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="30"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="38"/>
       <c r="G32" s="5"/>
       <c r="H32" s="15" t="s">
         <v>44</v>
@@ -1390,11 +1390,11 @@
       <c r="C33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="30"/>
       <c r="G33" s="5"/>
       <c r="H33" s="7" t="s">
         <v>11</v>
@@ -1405,11 +1405,11 @@
         <v>28</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="28" t="s">
+      <c r="D34" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30"/>
+      <c r="E34" s="37"/>
+      <c r="F34" s="38"/>
       <c r="G34" s="5"/>
       <c r="H34" s="15"/>
     </row>
@@ -1418,11 +1418,11 @@
         <v>29</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="30"/>
       <c r="G35" s="5"/>
       <c r="H35" s="7"/>
     </row>
@@ -1431,11 +1431,11 @@
         <v>30</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="28" t="s">
+      <c r="D36" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="30"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="38"/>
       <c r="G36" s="5"/>
       <c r="H36" s="15"/>
     </row>
@@ -1444,11 +1444,11 @@
         <v>31</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="30"/>
       <c r="G37" s="5"/>
       <c r="H37" s="7"/>
     </row>
@@ -1457,11 +1457,11 @@
         <v>32</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="30"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="5"/>
       <c r="H38" s="15"/>
     </row>
@@ -1470,11 +1470,11 @@
         <v>33</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="5"/>
       <c r="H39" s="7"/>
     </row>
@@ -1483,37 +1483,16 @@
         <v>34</v>
       </c>
       <c r="C40" s="16"/>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="41"/>
       <c r="G40" s="17"/>
       <c r="H40" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D23:F23"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="D40:F40"/>
@@ -1530,6 +1509,27 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished all up to Storm.. Indukt. a)
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD30DD2-FA3A-4FCA-AB02-23D3D97547D9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128AB1AB-7FD7-4A59-85BF-487BB1CE00AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -587,6 +588,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -596,6 +606,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -609,27 +631,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -948,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,13 +967,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="J2" s="12" t="s">
         <v>41</v>
       </c>
@@ -987,10 +988,10 @@
       <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="10"/>
@@ -1009,11 +1010,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="23"/>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="24" t="s">
         <v>3</v>
       </c>
@@ -1028,11 +1029,11 @@
       <c r="C7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="26"/>
       <c r="H7" s="21" t="s">
         <v>11</v>
@@ -1045,11 +1046,11 @@
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33"/>
       <c r="G8" s="26"/>
       <c r="H8" s="7" t="s">
         <v>11</v>
@@ -1062,11 +1063,11 @@
       <c r="C9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
       <c r="G9" s="11"/>
       <c r="H9" s="15" t="s">
         <v>11</v>
@@ -1077,11 +1078,11 @@
         <v>4</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
       <c r="G10" s="27"/>
       <c r="H10" s="7" t="s">
         <v>46</v>
@@ -1092,11 +1093,11 @@
         <v>5</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="38"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
       <c r="G11" s="26"/>
       <c r="H11" s="15" t="s">
         <v>45</v>
@@ -1107,11 +1108,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
       <c r="G12" s="11"/>
       <c r="H12" s="7"/>
     </row>
@@ -1120,11 +1121,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="8"/>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="38"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="27"/>
       <c r="H13" s="15"/>
     </row>
@@ -1133,11 +1134,11 @@
         <v>8</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
       <c r="G14" s="27"/>
       <c r="H14" s="7"/>
     </row>
@@ -1146,11 +1147,11 @@
         <v>9</v>
       </c>
       <c r="C15" s="8"/>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="27"/>
       <c r="H15" s="15"/>
     </row>
@@ -1161,11 +1162,11 @@
       <c r="C16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="27"/>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1176,11 +1177,11 @@
         <v>11</v>
       </c>
       <c r="C17" s="8"/>
-      <c r="D17" s="36" t="s">
+      <c r="D17" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="38"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="27"/>
       <c r="H17" s="15"/>
     </row>
@@ -1189,11 +1190,11 @@
         <v>12</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="30"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="27"/>
       <c r="H18" s="7"/>
     </row>
@@ -1202,11 +1203,11 @@
         <v>13</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="30"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
       <c r="G19" s="27"/>
       <c r="H19" s="7"/>
     </row>
@@ -1215,11 +1216,11 @@
         <v>14</v>
       </c>
       <c r="C20" s="8"/>
-      <c r="D20" s="36" t="s">
+      <c r="D20" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="38"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
       <c r="G20" s="27"/>
       <c r="H20" s="15"/>
     </row>
@@ -1228,11 +1229,11 @@
         <v>15</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="30"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="27"/>
       <c r="H21" s="15"/>
     </row>
@@ -1241,11 +1242,11 @@
         <v>16</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="33"/>
       <c r="G22" s="27"/>
       <c r="H22" s="7"/>
     </row>
@@ -1254,11 +1255,11 @@
         <v>17</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="37"/>
-      <c r="F23" s="38"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="30"/>
       <c r="G23" s="27"/>
       <c r="H23" s="7"/>
     </row>
@@ -1267,11 +1268,11 @@
         <v>18</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="37"/>
-      <c r="F24" s="38"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="27"/>
       <c r="H24" s="15"/>
     </row>
@@ -1280,11 +1281,11 @@
         <v>19</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="28" t="s">
+      <c r="D25" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E25" s="29"/>
-      <c r="F25" s="30"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="27"/>
       <c r="H25" s="7"/>
     </row>
@@ -1293,11 +1294,11 @@
         <v>20</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="38"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
       <c r="G26" s="27"/>
       <c r="H26" s="15"/>
     </row>
@@ -1306,11 +1307,11 @@
         <v>21</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="29"/>
-      <c r="F27" s="30"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
       <c r="G27" s="27"/>
       <c r="H27" s="7"/>
     </row>
@@ -1319,11 +1320,11 @@
         <v>22</v>
       </c>
       <c r="C28" s="8"/>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
       <c r="G28" s="27"/>
       <c r="H28" s="15"/>
     </row>
@@ -1332,11 +1333,11 @@
         <v>23</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="29"/>
-      <c r="F29" s="30"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
       <c r="G29" s="27"/>
       <c r="H29" s="7"/>
     </row>
@@ -1345,11 +1346,11 @@
         <v>24</v>
       </c>
       <c r="C30" s="8"/>
-      <c r="D30" s="36" t="s">
+      <c r="D30" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="37"/>
-      <c r="F30" s="38"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
       <c r="G30" s="27"/>
       <c r="H30" s="15"/>
     </row>
@@ -1358,11 +1359,11 @@
         <v>25</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="27"/>
       <c r="H31" s="7"/>
     </row>
@@ -1373,12 +1374,12 @@
       <c r="C32" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="37"/>
-      <c r="F32" s="38"/>
-      <c r="G32" s="5"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="27"/>
       <c r="H32" s="15" t="s">
         <v>44</v>
       </c>
@@ -1390,12 +1391,12 @@
       <c r="C33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="29"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="5"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="27"/>
       <c r="H33" s="7" t="s">
         <v>11</v>
       </c>
@@ -1405,12 +1406,12 @@
         <v>28</v>
       </c>
       <c r="C34" s="8"/>
-      <c r="D34" s="36" t="s">
+      <c r="D34" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="37"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="5"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="27"/>
       <c r="H34" s="15"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
@@ -1418,12 +1419,12 @@
         <v>29</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="5"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="7"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.3">
@@ -1431,11 +1432,11 @@
         <v>30</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="36" t="s">
+      <c r="D36" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="37"/>
-      <c r="F36" s="38"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
       <c r="G36" s="5"/>
       <c r="H36" s="15"/>
     </row>
@@ -1444,11 +1445,11 @@
         <v>31</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="30"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="5"/>
       <c r="H37" s="7"/>
     </row>
@@ -1457,11 +1458,11 @@
         <v>32</v>
       </c>
       <c r="C38" s="8"/>
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="E38" s="37"/>
-      <c r="F38" s="38"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="30"/>
       <c r="G38" s="5"/>
       <c r="H38" s="15"/>
     </row>
@@ -1470,11 +1471,11 @@
         <v>33</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="28" t="s">
+      <c r="D39" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="30"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
       <c r="G39" s="5"/>
       <c r="H39" s="7"/>
     </row>
@@ -1483,16 +1484,37 @@
         <v>34</v>
       </c>
       <c r="C40" s="16"/>
-      <c r="D40" s="39" t="s">
+      <c r="D40" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="E40" s="40"/>
-      <c r="F40" s="41"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="36"/>
       <c r="G40" s="17"/>
       <c r="H40" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D23:F23"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="D40:F40"/>
@@ -1509,27 +1531,6 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished up to schleife plots
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1155E9C1-956D-4175-AE39-7F1C370AFFCF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF24099B-3596-4B25-AB91-7FD49885A388}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="105">
   <si>
     <t xml:space="preserve">Liste der zu zeichnenden Zeigerdiagramme </t>
   </si>
@@ -343,6 +343,9 @@
   </si>
   <si>
     <t>RL-Schaltung mit gleichgerichteter Spannung II c)</t>
+  </si>
+  <si>
+    <t>Layout an RLC-Serienschwingkreis anpassen</t>
   </si>
 </sst>
 </file>
@@ -763,51 +766,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -815,6 +773,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1131,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K115" sqref="K115"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1150,13 +1153,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
       <c r="J2" s="11" t="s">
         <v>41</v>
       </c>
@@ -1171,10 +1174,10 @@
       <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="29"/>
+      <c r="D4" s="31"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="9"/>
@@ -1187,11 +1190,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="21"/>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="22" t="s">
         <v>3</v>
       </c>
@@ -1208,16 +1211,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="24"/>
       <c r="H6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="28" t="s">
         <v>7</v>
       </c>
       <c r="K6" t="s">
@@ -1229,11 +1232,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="28"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="24"/>
       <c r="H7" s="6" t="s">
         <v>11</v>
@@ -1244,11 +1247,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="10"/>
       <c r="H8" s="14" t="s">
         <v>11</v>
@@ -1259,11 +1262,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="25"/>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -1274,11 +1277,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="24"/>
       <c r="H10" s="14" t="s">
         <v>45</v>
@@ -1289,11 +1292,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="10"/>
       <c r="H11" s="6"/>
     </row>
@@ -1302,11 +1305,11 @@
         <v>7</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="25"/>
       <c r="H12" s="14"/>
     </row>
@@ -1315,11 +1318,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="25"/>
       <c r="H13" s="6"/>
     </row>
@@ -1328,11 +1331,11 @@
         <v>9</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="25"/>
       <c r="H14" s="14"/>
     </row>
@@ -1341,11 +1344,11 @@
         <v>10</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="28"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="25"/>
       <c r="H15" s="6" t="s">
         <v>11</v>
@@ -1356,11 +1359,11 @@
         <v>11</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
       <c r="G16" s="25"/>
       <c r="H16" s="14"/>
     </row>
@@ -1369,11 +1372,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="25"/>
       <c r="H17" s="6"/>
     </row>
@@ -1382,11 +1385,11 @@
         <v>13</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="25"/>
       <c r="H18" s="6"/>
     </row>
@@ -1395,11 +1398,11 @@
         <v>14</v>
       </c>
       <c r="C19" s="7"/>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="36"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="40"/>
       <c r="G19" s="25"/>
       <c r="H19" s="14"/>
     </row>
@@ -1408,11 +1411,11 @@
         <v>15</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="28"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="25"/>
       <c r="H20" s="14"/>
     </row>
@@ -1421,11 +1424,11 @@
         <v>16</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="28"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="25"/>
       <c r="H21" s="6"/>
     </row>
@@ -1434,11 +1437,11 @@
         <v>17</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40"/>
       <c r="G22" s="25"/>
       <c r="H22" s="6"/>
     </row>
@@ -1447,11 +1450,11 @@
         <v>18</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="36"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="40"/>
       <c r="G23" s="25"/>
       <c r="H23" s="14"/>
     </row>
@@ -1460,11 +1463,11 @@
         <v>19</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="28"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
       <c r="G24" s="25"/>
       <c r="H24" s="6"/>
     </row>
@@ -1473,11 +1476,11 @@
         <v>20</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="35"/>
-      <c r="F25" s="36"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="40"/>
       <c r="G25" s="25"/>
       <c r="H25" s="14"/>
     </row>
@@ -1486,11 +1489,11 @@
         <v>21</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="28"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="25"/>
       <c r="H26" s="6"/>
     </row>
@@ -1499,11 +1502,11 @@
         <v>22</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="35"/>
-      <c r="F27" s="36"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="40"/>
       <c r="G27" s="25"/>
       <c r="H27" s="14"/>
     </row>
@@ -1512,11 +1515,11 @@
         <v>23</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="27"/>
-      <c r="F28" s="28"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="37"/>
       <c r="G28" s="25"/>
       <c r="H28" s="6"/>
     </row>
@@ -1525,11 +1528,11 @@
         <v>24</v>
       </c>
       <c r="C29" s="7"/>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="35"/>
-      <c r="F29" s="36"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="40"/>
       <c r="G29" s="25"/>
       <c r="H29" s="14"/>
     </row>
@@ -1538,11 +1541,11 @@
         <v>25</v>
       </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="27"/>
-      <c r="F30" s="28"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="37"/>
       <c r="G30" s="25"/>
       <c r="H30" s="6"/>
     </row>
@@ -1551,11 +1554,11 @@
         <v>26</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="40"/>
       <c r="G31" s="25"/>
       <c r="H31" s="14" t="s">
         <v>44</v>
@@ -1566,11 +1569,11 @@
         <v>27</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="27"/>
-      <c r="F32" s="28"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="25"/>
       <c r="H32" s="6" t="s">
         <v>11</v>
@@ -1581,11 +1584,11 @@
         <v>28</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="35"/>
-      <c r="F33" s="36"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="40"/>
       <c r="G33" s="25"/>
       <c r="H33" s="14"/>
     </row>
@@ -1594,11 +1597,11 @@
         <v>29</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="27"/>
-      <c r="F34" s="28"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="37"/>
       <c r="G34" s="25"/>
       <c r="H34" s="6"/>
     </row>
@@ -1607,11 +1610,11 @@
         <v>30</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="35"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="40"/>
       <c r="G35" s="25"/>
       <c r="H35" s="14"/>
     </row>
@@ -1620,11 +1623,11 @@
         <v>31</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="27"/>
-      <c r="F36" s="28"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="37"/>
       <c r="G36" s="25"/>
       <c r="H36" s="6"/>
     </row>
@@ -1633,11 +1636,11 @@
         <v>32</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="40"/>
       <c r="G37" s="25"/>
       <c r="H37" s="14"/>
     </row>
@@ -1646,11 +1649,11 @@
         <v>33</v>
       </c>
       <c r="C38" s="4"/>
-      <c r="D38" s="26" t="s">
+      <c r="D38" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="27"/>
-      <c r="F38" s="28"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="37"/>
       <c r="G38" s="25"/>
       <c r="H38" s="6"/>
     </row>
@@ -1659,11 +1662,11 @@
         <v>34</v>
       </c>
       <c r="C39" s="15"/>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="39"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="44"/>
       <c r="G39" s="25"/>
       <c r="H39" s="16"/>
     </row>
@@ -1671,10 +1674,10 @@
       <c r="B42" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="29"/>
+      <c r="D42" s="31"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
@@ -1683,11 +1686,11 @@
         <v>1</v>
       </c>
       <c r="C43" s="21"/>
-      <c r="D43" s="30" t="s">
+      <c r="D43" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="30"/>
-      <c r="F43" s="30"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="41"/>
       <c r="G43" s="22" t="s">
         <v>3</v>
       </c>
@@ -1700,12 +1703,12 @@
         <v>1</v>
       </c>
       <c r="C44" s="18"/>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="32"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="41"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="25"/>
       <c r="H44" s="19"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
@@ -1713,12 +1716,12 @@
         <v>2</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="26" t="s">
+      <c r="D45" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="27"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="42"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="25"/>
       <c r="H45" s="6"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
@@ -1726,12 +1729,12 @@
         <v>3</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="42"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="25"/>
       <c r="H46" s="14"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
@@ -1739,25 +1742,27 @@
         <v>4</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="26" t="s">
+      <c r="D47" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="27"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="6"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="6" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="17">
         <v>5</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="35"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="42"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="25"/>
       <c r="H48" s="14"/>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
@@ -1765,12 +1770,12 @@
         <v>6</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="26" t="s">
+      <c r="D49" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="27"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="42"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="25"/>
       <c r="H49" s="6"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
@@ -1778,12 +1783,12 @@
         <v>7</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="35"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="42"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="27"/>
       <c r="H50" s="14" t="s">
         <v>58</v>
       </c>
@@ -1792,10 +1797,10 @@
       <c r="B53" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="29"/>
+      <c r="D53" s="31"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
@@ -1804,11 +1809,11 @@
         <v>1</v>
       </c>
       <c r="C54" s="21"/>
-      <c r="D54" s="30" t="s">
+      <c r="D54" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
+      <c r="E54" s="41"/>
+      <c r="F54" s="41"/>
       <c r="G54" s="22" t="s">
         <v>3</v>
       </c>
@@ -1821,12 +1826,12 @@
         <v>1</v>
       </c>
       <c r="C55" s="18"/>
-      <c r="D55" s="31" t="s">
+      <c r="D55" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="32"/>
-      <c r="F55" s="33"/>
-      <c r="G55" s="41"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="26"/>
       <c r="H55" s="19"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
@@ -1834,12 +1839,12 @@
         <v>2</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="26" t="s">
+      <c r="D56" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="27"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="42"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="27"/>
       <c r="H56" s="6"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
@@ -1847,12 +1852,12 @@
         <v>3</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="D57" s="34" t="s">
+      <c r="D57" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="35"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="42"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="27"/>
       <c r="H57" s="14"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
@@ -1860,12 +1865,12 @@
         <v>4</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="26" t="s">
+      <c r="D58" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="27"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="42"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="27"/>
       <c r="H58" s="6"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.3">
@@ -1873,12 +1878,12 @@
         <v>5</v>
       </c>
       <c r="C59" s="7"/>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="35"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="42"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="27"/>
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.3">
@@ -1886,12 +1891,12 @@
         <v>6</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="26" t="s">
+      <c r="D60" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="27"/>
-      <c r="F60" s="28"/>
-      <c r="G60" s="42"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="27"/>
       <c r="H60" s="6"/>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.3">
@@ -1899,12 +1904,12 @@
         <v>7</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="34" t="s">
+      <c r="D61" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="35"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="42"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="27"/>
       <c r="H61" s="14"/>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.3">
@@ -1912,12 +1917,12 @@
         <v>8</v>
       </c>
       <c r="C62" s="7"/>
-      <c r="D62" s="34" t="s">
+      <c r="D62" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="35"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="42"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="27"/>
       <c r="H62" s="14"/>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.3">
@@ -1925,12 +1930,12 @@
         <v>9</v>
       </c>
       <c r="C63" s="7"/>
-      <c r="D63" s="34" t="s">
+      <c r="D63" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="35"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="42"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="40"/>
+      <c r="G63" s="27"/>
       <c r="H63" s="14"/>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.3">
@@ -1940,12 +1945,12 @@
       <c r="C64" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="34" t="s">
+      <c r="D64" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="35"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="42"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="27"/>
       <c r="H64" s="14"/>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.3">
@@ -1955,22 +1960,22 @@
       <c r="C65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="34" t="s">
+      <c r="D65" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="35"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="42"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="27"/>
       <c r="H65" s="14"/>
     </row>
     <row r="68" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B68" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="29" t="s">
+      <c r="C68" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="29"/>
+      <c r="D68" s="31"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
@@ -1979,11 +1984,11 @@
         <v>1</v>
       </c>
       <c r="C69" s="21"/>
-      <c r="D69" s="30" t="s">
+      <c r="D69" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="30"/>
-      <c r="F69" s="30"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="41"/>
       <c r="G69" s="22" t="s">
         <v>3</v>
       </c>
@@ -1996,20 +2001,20 @@
         <v>1</v>
       </c>
       <c r="C70" s="18"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="44"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="34"/>
+      <c r="G70" s="29"/>
       <c r="H70" s="19"/>
     </row>
     <row r="73" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B73" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="29" t="s">
+      <c r="C73" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="D73" s="29"/>
+      <c r="D73" s="31"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
     </row>
@@ -2018,11 +2023,11 @@
         <v>1</v>
       </c>
       <c r="C74" s="21"/>
-      <c r="D74" s="30" t="s">
+      <c r="D74" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E74" s="30"/>
-      <c r="F74" s="30"/>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
       <c r="G74" s="22" t="s">
         <v>3</v>
       </c>
@@ -2035,12 +2040,12 @@
         <v>1</v>
       </c>
       <c r="C75" s="18"/>
-      <c r="D75" s="31" t="s">
+      <c r="D75" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="E75" s="32"/>
-      <c r="F75" s="33"/>
-      <c r="G75" s="41"/>
+      <c r="E75" s="33"/>
+      <c r="F75" s="34"/>
+      <c r="G75" s="26"/>
       <c r="H75" s="19"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.3">
@@ -2048,12 +2053,12 @@
         <v>2</v>
       </c>
       <c r="C76" s="4"/>
-      <c r="D76" s="26" t="s">
+      <c r="D76" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="E76" s="27"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="42"/>
+      <c r="E76" s="36"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="27"/>
       <c r="H76" s="6"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.3">
@@ -2061,12 +2066,12 @@
         <v>3</v>
       </c>
       <c r="C77" s="7"/>
-      <c r="D77" s="34" t="s">
+      <c r="D77" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E77" s="35"/>
-      <c r="F77" s="36"/>
-      <c r="G77" s="42"/>
+      <c r="E77" s="39"/>
+      <c r="F77" s="40"/>
+      <c r="G77" s="27"/>
       <c r="H77" s="14"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.3">
@@ -2074,12 +2079,12 @@
         <v>4</v>
       </c>
       <c r="C78" s="4"/>
-      <c r="D78" s="26" t="s">
+      <c r="D78" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="E78" s="27"/>
-      <c r="F78" s="28"/>
-      <c r="G78" s="42"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="27"/>
       <c r="H78" s="6"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.3">
@@ -2087,22 +2092,22 @@
         <v>5</v>
       </c>
       <c r="C79" s="7"/>
-      <c r="D79" s="34" t="s">
+      <c r="D79" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="E79" s="35"/>
-      <c r="F79" s="36"/>
-      <c r="G79" s="42"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="40"/>
+      <c r="G79" s="27"/>
       <c r="H79" s="14"/>
     </row>
     <row r="82" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B82" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C82" s="29" t="s">
+      <c r="C82" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="29"/>
+      <c r="D82" s="31"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
     </row>
@@ -2111,11 +2116,11 @@
         <v>1</v>
       </c>
       <c r="C83" s="21"/>
-      <c r="D83" s="30" t="s">
+      <c r="D83" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E83" s="30"/>
-      <c r="F83" s="30"/>
+      <c r="E83" s="41"/>
+      <c r="F83" s="41"/>
       <c r="G83" s="22" t="s">
         <v>3</v>
       </c>
@@ -2128,12 +2133,12 @@
         <v>1</v>
       </c>
       <c r="C84" s="18"/>
-      <c r="D84" s="31" t="s">
+      <c r="D84" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="E84" s="32"/>
-      <c r="F84" s="33"/>
-      <c r="G84" s="41"/>
+      <c r="E84" s="33"/>
+      <c r="F84" s="34"/>
+      <c r="G84" s="26"/>
       <c r="H84" s="19"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.3">
@@ -2141,12 +2146,12 @@
         <v>2</v>
       </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="26" t="s">
+      <c r="D85" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="E85" s="27"/>
-      <c r="F85" s="28"/>
-      <c r="G85" s="42"/>
+      <c r="E85" s="36"/>
+      <c r="F85" s="37"/>
+      <c r="G85" s="27"/>
       <c r="H85" s="6"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.3">
@@ -2154,12 +2159,12 @@
         <v>3</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="34" t="s">
+      <c r="D86" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="E86" s="35"/>
-      <c r="F86" s="36"/>
-      <c r="G86" s="42"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="40"/>
+      <c r="G86" s="27"/>
       <c r="H86" s="14"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
@@ -2167,12 +2172,12 @@
         <v>4</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="D87" s="26" t="s">
+      <c r="D87" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="E87" s="27"/>
-      <c r="F87" s="28"/>
-      <c r="G87" s="42"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="27"/>
       <c r="H87" s="6"/>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
@@ -2180,12 +2185,12 @@
         <v>5</v>
       </c>
       <c r="C88" s="7"/>
-      <c r="D88" s="34" t="s">
+      <c r="D88" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="E88" s="35"/>
-      <c r="F88" s="36"/>
-      <c r="G88" s="42"/>
+      <c r="E88" s="39"/>
+      <c r="F88" s="40"/>
+      <c r="G88" s="27"/>
       <c r="H88" s="14"/>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
@@ -2193,12 +2198,12 @@
         <v>6</v>
       </c>
       <c r="C89" s="7"/>
-      <c r="D89" s="34" t="s">
+      <c r="D89" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="E89" s="35"/>
-      <c r="F89" s="36"/>
-      <c r="G89" s="42"/>
+      <c r="E89" s="39"/>
+      <c r="F89" s="40"/>
+      <c r="G89" s="27"/>
       <c r="H89" s="14"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.3">
@@ -2206,12 +2211,12 @@
         <v>7</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="34" t="s">
+      <c r="D90" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="E90" s="35"/>
-      <c r="F90" s="36"/>
-      <c r="G90" s="42"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="40"/>
+      <c r="G90" s="27"/>
       <c r="H90" s="14"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.3">
@@ -2219,12 +2224,12 @@
         <v>8</v>
       </c>
       <c r="C91" s="7"/>
-      <c r="D91" s="34" t="s">
+      <c r="D91" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="E91" s="35"/>
-      <c r="F91" s="36"/>
-      <c r="G91" s="42"/>
+      <c r="E91" s="39"/>
+      <c r="F91" s="40"/>
+      <c r="G91" s="27"/>
       <c r="H91" s="14"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.3">
@@ -2232,12 +2237,12 @@
         <v>9</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="34" t="s">
+      <c r="D92" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="E92" s="35"/>
-      <c r="F92" s="36"/>
-      <c r="G92" s="42"/>
+      <c r="E92" s="39"/>
+      <c r="F92" s="40"/>
+      <c r="G92" s="27"/>
       <c r="H92" s="14"/>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.3">
@@ -2245,12 +2250,12 @@
         <v>10</v>
       </c>
       <c r="C93" s="7"/>
-      <c r="D93" s="34" t="s">
+      <c r="D93" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="E93" s="35"/>
-      <c r="F93" s="36"/>
-      <c r="G93" s="42"/>
+      <c r="E93" s="39"/>
+      <c r="F93" s="40"/>
+      <c r="G93" s="27"/>
       <c r="H93" s="14"/>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.3">
@@ -2258,12 +2263,12 @@
         <v>11</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="34" t="s">
+      <c r="D94" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E94" s="35"/>
-      <c r="F94" s="36"/>
-      <c r="G94" s="42"/>
+      <c r="E94" s="39"/>
+      <c r="F94" s="40"/>
+      <c r="G94" s="27"/>
       <c r="H94" s="14"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.3">
@@ -2271,12 +2276,12 @@
         <v>12</v>
       </c>
       <c r="C95" s="7"/>
-      <c r="D95" s="34" t="s">
+      <c r="D95" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="E95" s="35"/>
-      <c r="F95" s="36"/>
-      <c r="G95" s="42"/>
+      <c r="E95" s="39"/>
+      <c r="F95" s="40"/>
+      <c r="G95" s="27"/>
       <c r="H95" s="14"/>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.3">
@@ -2284,12 +2289,12 @@
         <v>13</v>
       </c>
       <c r="C96" s="7"/>
-      <c r="D96" s="34" t="s">
+      <c r="D96" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="E96" s="35"/>
-      <c r="F96" s="36"/>
-      <c r="G96" s="42"/>
+      <c r="E96" s="39"/>
+      <c r="F96" s="40"/>
+      <c r="G96" s="27"/>
       <c r="H96" s="14"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.3">
@@ -2297,22 +2302,22 @@
         <v>14</v>
       </c>
       <c r="C97" s="7"/>
-      <c r="D97" s="34" t="s">
+      <c r="D97" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="E97" s="35"/>
-      <c r="F97" s="36"/>
-      <c r="G97" s="42"/>
+      <c r="E97" s="39"/>
+      <c r="F97" s="40"/>
+      <c r="G97" s="27"/>
       <c r="H97" s="14"/>
     </row>
     <row r="100" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B100" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C100" s="29" t="s">
+      <c r="C100" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D100" s="29"/>
+      <c r="D100" s="31"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
     </row>
@@ -2321,11 +2326,11 @@
         <v>1</v>
       </c>
       <c r="C101" s="21"/>
-      <c r="D101" s="30" t="s">
+      <c r="D101" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E101" s="30"/>
-      <c r="F101" s="30"/>
+      <c r="E101" s="41"/>
+      <c r="F101" s="41"/>
       <c r="G101" s="22" t="s">
         <v>3</v>
       </c>
@@ -2338,22 +2343,22 @@
         <v>1</v>
       </c>
       <c r="C102" s="18"/>
-      <c r="D102" s="31" t="s">
+      <c r="D102" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="E102" s="32"/>
-      <c r="F102" s="33"/>
-      <c r="G102" s="41"/>
+      <c r="E102" s="33"/>
+      <c r="F102" s="34"/>
+      <c r="G102" s="26"/>
       <c r="H102" s="19"/>
     </row>
     <row r="105" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B105" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C105" s="29" t="s">
+      <c r="C105" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="D105" s="29"/>
+      <c r="D105" s="31"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
     </row>
@@ -2362,11 +2367,11 @@
         <v>1</v>
       </c>
       <c r="C106" s="21"/>
-      <c r="D106" s="30" t="s">
+      <c r="D106" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E106" s="30"/>
-      <c r="F106" s="30"/>
+      <c r="E106" s="41"/>
+      <c r="F106" s="41"/>
       <c r="G106" s="22" t="s">
         <v>3</v>
       </c>
@@ -2379,22 +2384,22 @@
         <v>1</v>
       </c>
       <c r="C107" s="18"/>
-      <c r="D107" s="31" t="s">
+      <c r="D107" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="E107" s="32"/>
-      <c r="F107" s="33"/>
-      <c r="G107" s="41"/>
+      <c r="E107" s="33"/>
+      <c r="F107" s="34"/>
+      <c r="G107" s="26"/>
       <c r="H107" s="19"/>
     </row>
     <row r="110" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B110" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C110" s="29" t="s">
+      <c r="C110" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="D110" s="29"/>
+      <c r="D110" s="31"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
     </row>
@@ -2403,11 +2408,11 @@
         <v>1</v>
       </c>
       <c r="C111" s="21"/>
-      <c r="D111" s="30" t="s">
+      <c r="D111" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E111" s="30"/>
-      <c r="F111" s="30"/>
+      <c r="E111" s="41"/>
+      <c r="F111" s="41"/>
       <c r="G111" s="22" t="s">
         <v>3</v>
       </c>
@@ -2420,20 +2425,20 @@
         <v>1</v>
       </c>
       <c r="C112" s="18"/>
-      <c r="D112" s="31"/>
-      <c r="E112" s="32"/>
-      <c r="F112" s="33"/>
-      <c r="G112" s="45"/>
+      <c r="D112" s="32"/>
+      <c r="E112" s="33"/>
+      <c r="F112" s="34"/>
+      <c r="G112" s="30"/>
       <c r="H112" s="19"/>
     </row>
     <row r="115" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C115" s="29" t="s">
+      <c r="C115" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="D115" s="29"/>
+      <c r="D115" s="31"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
     </row>
@@ -2442,11 +2447,11 @@
         <v>1</v>
       </c>
       <c r="C116" s="21"/>
-      <c r="D116" s="30" t="s">
+      <c r="D116" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="E116" s="30"/>
-      <c r="F116" s="30"/>
+      <c r="E116" s="41"/>
+      <c r="F116" s="41"/>
       <c r="G116" s="22" t="s">
         <v>3</v>
       </c>
@@ -2459,12 +2464,12 @@
         <v>1</v>
       </c>
       <c r="C117" s="18"/>
-      <c r="D117" s="31" t="s">
+      <c r="D117" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="E117" s="32"/>
-      <c r="F117" s="33"/>
-      <c r="G117" s="41"/>
+      <c r="E117" s="33"/>
+      <c r="F117" s="34"/>
+      <c r="G117" s="26"/>
       <c r="H117" s="19"/>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.3">
@@ -2472,12 +2477,12 @@
         <v>2</v>
       </c>
       <c r="C118" s="4"/>
-      <c r="D118" s="26" t="s">
+      <c r="D118" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="E118" s="27"/>
-      <c r="F118" s="28"/>
-      <c r="G118" s="42"/>
+      <c r="E118" s="36"/>
+      <c r="F118" s="37"/>
+      <c r="G118" s="27"/>
       <c r="H118" s="6"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.3">
@@ -2485,12 +2490,12 @@
         <v>3</v>
       </c>
       <c r="C119" s="7"/>
-      <c r="D119" s="34" t="s">
+      <c r="D119" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="E119" s="35"/>
-      <c r="F119" s="36"/>
-      <c r="G119" s="42"/>
+      <c r="E119" s="39"/>
+      <c r="F119" s="40"/>
+      <c r="G119" s="27"/>
       <c r="H119" s="14"/>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.3">
@@ -2498,79 +2503,37 @@
         <v>4</v>
       </c>
       <c r="C120" s="4"/>
-      <c r="D120" s="26" t="s">
+      <c r="D120" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="E120" s="27"/>
-      <c r="F120" s="28"/>
-      <c r="G120" s="42"/>
+      <c r="E120" s="36"/>
+      <c r="F120" s="37"/>
+      <c r="G120" s="27"/>
       <c r="H120" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="D119:F119"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D102:F102"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D97:F97"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="D76:F76"/>
-    <mergeCell ref="D77:F77"/>
-    <mergeCell ref="D78:F78"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
     <mergeCell ref="D37:F37"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="D39:F39"/>
@@ -2587,27 +2550,69 @@
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="D78:F78"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="D102:F102"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D97:F97"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D116:F116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished up to Admittanz
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF24099B-3596-4B25-AB91-7FD49885A388}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496D2BA4-7E38-4B5F-A7A0-89A525BAC2DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="106">
   <si>
     <t xml:space="preserve">Liste der zu zeichnenden Zeigerdiagramme </t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>Layout an RLC-Serienschwingkreis anpassen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Als letztes allenfalls noch machen </t>
   </si>
 </sst>
 </file>
@@ -773,9 +776,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -785,15 +800,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -801,9 +807,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1134,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1174,10 +1177,10 @@
       <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="31"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="9"/>
@@ -1190,11 +1193,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="21"/>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="22" t="s">
         <v>3</v>
       </c>
@@ -1211,11 +1214,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="18"/>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="24"/>
       <c r="H6" s="19" t="s">
         <v>11</v>
@@ -1232,11 +1235,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="24"/>
       <c r="H7" s="6" t="s">
         <v>11</v>
@@ -1247,11 +1250,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="39"/>
-      <c r="F8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="10"/>
       <c r="H8" s="14" t="s">
         <v>11</v>
@@ -1262,11 +1265,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="37"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="25"/>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -1277,11 +1280,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="24"/>
       <c r="H10" s="14" t="s">
         <v>45</v>
@@ -1292,11 +1295,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="10"/>
       <c r="H11" s="6"/>
     </row>
@@ -1305,11 +1308,11 @@
         <v>7</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="38" t="s">
+      <c r="D12" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="39"/>
-      <c r="F12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
       <c r="G12" s="25"/>
       <c r="H12" s="14"/>
     </row>
@@ -1318,11 +1321,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="25"/>
       <c r="H13" s="6"/>
     </row>
@@ -1331,11 +1334,11 @@
         <v>9</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="39"/>
-      <c r="F14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="41"/>
       <c r="G14" s="25"/>
       <c r="H14" s="14"/>
     </row>
@@ -1344,11 +1347,11 @@
         <v>10</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
       <c r="G15" s="25"/>
       <c r="H15" s="6" t="s">
         <v>11</v>
@@ -1359,11 +1362,11 @@
         <v>11</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="38" t="s">
+      <c r="D16" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="41"/>
       <c r="G16" s="25"/>
       <c r="H16" s="14"/>
     </row>
@@ -1372,11 +1375,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="25"/>
       <c r="H17" s="6"/>
     </row>
@@ -1385,11 +1388,11 @@
         <v>13</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="37"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
       <c r="G18" s="25"/>
       <c r="H18" s="6"/>
     </row>
@@ -1398,11 +1401,11 @@
         <v>14</v>
       </c>
       <c r="C19" s="7"/>
-      <c r="D19" s="38" t="s">
+      <c r="D19" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="41"/>
       <c r="G19" s="25"/>
       <c r="H19" s="14"/>
     </row>
@@ -1411,11 +1414,11 @@
         <v>15</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33"/>
       <c r="G20" s="25"/>
       <c r="H20" s="14"/>
     </row>
@@ -1424,11 +1427,11 @@
         <v>16</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="36"/>
-      <c r="F21" s="37"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="25"/>
       <c r="H21" s="6"/>
     </row>
@@ -1437,11 +1440,11 @@
         <v>17</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="41"/>
       <c r="G22" s="25"/>
       <c r="H22" s="6"/>
     </row>
@@ -1450,11 +1453,11 @@
         <v>18</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="38" t="s">
+      <c r="D23" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="39"/>
-      <c r="F23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="41"/>
       <c r="G23" s="25"/>
       <c r="H23" s="14"/>
     </row>
@@ -1463,11 +1466,11 @@
         <v>19</v>
       </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="33"/>
       <c r="G24" s="25"/>
       <c r="H24" s="6"/>
     </row>
@@ -1476,11 +1479,11 @@
         <v>20</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="38" t="s">
+      <c r="D25" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="39"/>
-      <c r="F25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="41"/>
       <c r="G25" s="25"/>
       <c r="H25" s="14"/>
     </row>
@@ -1489,11 +1492,11 @@
         <v>21</v>
       </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="33"/>
       <c r="G26" s="25"/>
       <c r="H26" s="6"/>
     </row>
@@ -1502,11 +1505,11 @@
         <v>22</v>
       </c>
       <c r="C27" s="7"/>
-      <c r="D27" s="38" t="s">
+      <c r="D27" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="25"/>
       <c r="H27" s="14"/>
     </row>
@@ -1515,11 +1518,11 @@
         <v>23</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="37"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="33"/>
       <c r="G28" s="25"/>
       <c r="H28" s="6"/>
     </row>
@@ -1528,11 +1531,11 @@
         <v>24</v>
       </c>
       <c r="C29" s="7"/>
-      <c r="D29" s="38" t="s">
+      <c r="D29" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="39"/>
-      <c r="F29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="25"/>
       <c r="H29" s="14"/>
     </row>
@@ -1541,11 +1544,11 @@
         <v>25</v>
       </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="33"/>
       <c r="G30" s="25"/>
       <c r="H30" s="6"/>
     </row>
@@ -1554,11 +1557,11 @@
         <v>26</v>
       </c>
       <c r="C31" s="7"/>
-      <c r="D31" s="38" t="s">
+      <c r="D31" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="39"/>
-      <c r="F31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="25"/>
       <c r="H31" s="14" t="s">
         <v>44</v>
@@ -1569,11 +1572,11 @@
         <v>27</v>
       </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="37"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="25"/>
       <c r="H32" s="6" t="s">
         <v>11</v>
@@ -1584,11 +1587,11 @@
         <v>28</v>
       </c>
       <c r="C33" s="7"/>
-      <c r="D33" s="38" t="s">
+      <c r="D33" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="39"/>
-      <c r="F33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="25"/>
       <c r="H33" s="14"/>
     </row>
@@ -1597,11 +1600,11 @@
         <v>29</v>
       </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="37"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="33"/>
       <c r="G34" s="25"/>
       <c r="H34" s="6"/>
     </row>
@@ -1610,11 +1613,11 @@
         <v>30</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="25"/>
       <c r="H35" s="14"/>
     </row>
@@ -1623,11 +1626,11 @@
         <v>31</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="37"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
       <c r="G36" s="25"/>
       <c r="H36" s="6"/>
     </row>
@@ -1636,11 +1639,11 @@
         <v>32</v>
       </c>
       <c r="C37" s="7"/>
-      <c r="D37" s="38" t="s">
+      <c r="D37" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="25"/>
       <c r="H37" s="14"/>
     </row>
@@ -1649,11 +1652,11 @@
         <v>33</v>
       </c>
       <c r="C38" s="4"/>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="36"/>
-      <c r="F38" s="37"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="33"/>
       <c r="G38" s="25"/>
       <c r="H38" s="6"/>
     </row>
@@ -1674,10 +1677,10 @@
       <c r="B42" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="C42" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="31"/>
+      <c r="D42" s="34"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
@@ -1686,11 +1689,11 @@
         <v>1</v>
       </c>
       <c r="C43" s="21"/>
-      <c r="D43" s="41" t="s">
+      <c r="D43" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
       <c r="G43" s="22" t="s">
         <v>3</v>
       </c>
@@ -1703,11 +1706,11 @@
         <v>1</v>
       </c>
       <c r="C44" s="18"/>
-      <c r="D44" s="32" t="s">
+      <c r="D44" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="33"/>
-      <c r="F44" s="34"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="38"/>
       <c r="G44" s="25"/>
       <c r="H44" s="19"/>
     </row>
@@ -1716,11 +1719,11 @@
         <v>2</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="35" t="s">
+      <c r="D45" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="36"/>
-      <c r="F45" s="37"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
       <c r="G45" s="25"/>
       <c r="H45" s="6"/>
     </row>
@@ -1729,11 +1732,11 @@
         <v>3</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="38" t="s">
+      <c r="D46" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="39"/>
-      <c r="F46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="41"/>
       <c r="G46" s="25"/>
       <c r="H46" s="14"/>
     </row>
@@ -1742,11 +1745,11 @@
         <v>4</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="35" t="s">
+      <c r="D47" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="36"/>
-      <c r="F47" s="37"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
       <c r="G47" s="25"/>
       <c r="H47" s="6" t="s">
         <v>104</v>
@@ -1757,11 +1760,11 @@
         <v>5</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="38" t="s">
+      <c r="D48" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="39"/>
-      <c r="F48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="41"/>
       <c r="G48" s="25"/>
       <c r="H48" s="14"/>
     </row>
@@ -1770,11 +1773,11 @@
         <v>6</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="35" t="s">
+      <c r="D49" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="37"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
       <c r="G49" s="25"/>
       <c r="H49" s="6"/>
     </row>
@@ -1783,12 +1786,12 @@
         <v>7</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="38" t="s">
+      <c r="D50" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="39"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="27"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="25"/>
       <c r="H50" s="14" t="s">
         <v>58</v>
       </c>
@@ -1797,10 +1800,10 @@
       <c r="B53" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="31" t="s">
+      <c r="C53" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="31"/>
+      <c r="D53" s="34"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
@@ -1809,11 +1812,11 @@
         <v>1</v>
       </c>
       <c r="C54" s="21"/>
-      <c r="D54" s="41" t="s">
+      <c r="D54" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
       <c r="G54" s="22" t="s">
         <v>3</v>
       </c>
@@ -1826,12 +1829,12 @@
         <v>1</v>
       </c>
       <c r="C55" s="18"/>
-      <c r="D55" s="32" t="s">
+      <c r="D55" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="33"/>
-      <c r="F55" s="34"/>
-      <c r="G55" s="26"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="25"/>
       <c r="H55" s="19"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
@@ -1839,12 +1842,12 @@
         <v>2</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="35" t="s">
+      <c r="D56" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="36"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="27"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="25"/>
       <c r="H56" s="6"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
@@ -1852,12 +1855,12 @@
         <v>3</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="D57" s="38" t="s">
+      <c r="D57" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="39"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="27"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="25"/>
       <c r="H57" s="14"/>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
@@ -1865,12 +1868,12 @@
         <v>4</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="35" t="s">
+      <c r="D58" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="36"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="27"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="25"/>
       <c r="H58" s="6"/>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.3">
@@ -1878,12 +1881,12 @@
         <v>5</v>
       </c>
       <c r="C59" s="7"/>
-      <c r="D59" s="38" t="s">
+      <c r="D59" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="39"/>
-      <c r="F59" s="40"/>
-      <c r="G59" s="27"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="25"/>
       <c r="H59" s="14"/>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.3">
@@ -1891,11 +1894,11 @@
         <v>6</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="35" t="s">
+      <c r="D60" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="36"/>
-      <c r="F60" s="37"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="33"/>
       <c r="G60" s="27"/>
       <c r="H60" s="6"/>
     </row>
@@ -1904,11 +1907,11 @@
         <v>7</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="38" t="s">
+      <c r="D61" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="39"/>
-      <c r="F61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="41"/>
       <c r="G61" s="27"/>
       <c r="H61" s="14"/>
     </row>
@@ -1917,11 +1920,11 @@
         <v>8</v>
       </c>
       <c r="C62" s="7"/>
-      <c r="D62" s="38" t="s">
+      <c r="D62" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="39"/>
-      <c r="F62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="41"/>
       <c r="G62" s="27"/>
       <c r="H62" s="14"/>
     </row>
@@ -1930,11 +1933,11 @@
         <v>9</v>
       </c>
       <c r="C63" s="7"/>
-      <c r="D63" s="38" t="s">
+      <c r="D63" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="39"/>
-      <c r="F63" s="40"/>
+      <c r="E63" s="40"/>
+      <c r="F63" s="41"/>
       <c r="G63" s="27"/>
       <c r="H63" s="14"/>
     </row>
@@ -1942,14 +1945,12 @@
       <c r="B64" s="17">
         <v>10</v>
       </c>
-      <c r="C64" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D64" s="38" t="s">
+      <c r="C64" s="7"/>
+      <c r="D64" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="39"/>
-      <c r="F64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="41"/>
       <c r="G64" s="27"/>
       <c r="H64" s="14"/>
     </row>
@@ -1960,22 +1961,24 @@
       <c r="C65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="38" t="s">
+      <c r="D65" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="39"/>
-      <c r="F65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="41"/>
       <c r="G65" s="27"/>
-      <c r="H65" s="14"/>
+      <c r="H65" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="68" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B68" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="31" t="s">
+      <c r="C68" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="31"/>
+      <c r="D68" s="34"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
@@ -1984,11 +1987,11 @@
         <v>1</v>
       </c>
       <c r="C69" s="21"/>
-      <c r="D69" s="41" t="s">
+      <c r="D69" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="41"/>
-      <c r="F69" s="41"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="35"/>
       <c r="G69" s="22" t="s">
         <v>3</v>
       </c>
@@ -2001,9 +2004,9 @@
         <v>1</v>
       </c>
       <c r="C70" s="18"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="34"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="38"/>
       <c r="G70" s="29"/>
       <c r="H70" s="19"/>
     </row>
@@ -2011,10 +2014,10 @@
       <c r="B73" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C73" s="31" t="s">
+      <c r="C73" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="D73" s="31"/>
+      <c r="D73" s="34"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
     </row>
@@ -2023,11 +2026,11 @@
         <v>1</v>
       </c>
       <c r="C74" s="21"/>
-      <c r="D74" s="41" t="s">
+      <c r="D74" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E74" s="41"/>
-      <c r="F74" s="41"/>
+      <c r="E74" s="35"/>
+      <c r="F74" s="35"/>
       <c r="G74" s="22" t="s">
         <v>3</v>
       </c>
@@ -2040,11 +2043,11 @@
         <v>1</v>
       </c>
       <c r="C75" s="18"/>
-      <c r="D75" s="32" t="s">
+      <c r="D75" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="E75" s="33"/>
-      <c r="F75" s="34"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="38"/>
       <c r="G75" s="26"/>
       <c r="H75" s="19"/>
     </row>
@@ -2053,11 +2056,11 @@
         <v>2</v>
       </c>
       <c r="C76" s="4"/>
-      <c r="D76" s="35" t="s">
+      <c r="D76" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="E76" s="36"/>
-      <c r="F76" s="37"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="33"/>
       <c r="G76" s="27"/>
       <c r="H76" s="6"/>
     </row>
@@ -2066,11 +2069,11 @@
         <v>3</v>
       </c>
       <c r="C77" s="7"/>
-      <c r="D77" s="38" t="s">
+      <c r="D77" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="E77" s="39"/>
-      <c r="F77" s="40"/>
+      <c r="E77" s="40"/>
+      <c r="F77" s="41"/>
       <c r="G77" s="27"/>
       <c r="H77" s="14"/>
     </row>
@@ -2079,11 +2082,11 @@
         <v>4</v>
       </c>
       <c r="C78" s="4"/>
-      <c r="D78" s="35" t="s">
+      <c r="D78" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="E78" s="36"/>
-      <c r="F78" s="37"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="33"/>
       <c r="G78" s="27"/>
       <c r="H78" s="6"/>
     </row>
@@ -2092,11 +2095,11 @@
         <v>5</v>
       </c>
       <c r="C79" s="7"/>
-      <c r="D79" s="38" t="s">
+      <c r="D79" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="E79" s="39"/>
-      <c r="F79" s="40"/>
+      <c r="E79" s="40"/>
+      <c r="F79" s="41"/>
       <c r="G79" s="27"/>
       <c r="H79" s="14"/>
     </row>
@@ -2104,10 +2107,10 @@
       <c r="B82" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C82" s="31" t="s">
+      <c r="C82" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D82" s="31"/>
+      <c r="D82" s="34"/>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
     </row>
@@ -2116,11 +2119,11 @@
         <v>1</v>
       </c>
       <c r="C83" s="21"/>
-      <c r="D83" s="41" t="s">
+      <c r="D83" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E83" s="41"/>
-      <c r="F83" s="41"/>
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
       <c r="G83" s="22" t="s">
         <v>3</v>
       </c>
@@ -2133,11 +2136,11 @@
         <v>1</v>
       </c>
       <c r="C84" s="18"/>
-      <c r="D84" s="32" t="s">
+      <c r="D84" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="E84" s="33"/>
-      <c r="F84" s="34"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="38"/>
       <c r="G84" s="26"/>
       <c r="H84" s="19"/>
     </row>
@@ -2146,11 +2149,11 @@
         <v>2</v>
       </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="35" t="s">
+      <c r="D85" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="E85" s="36"/>
-      <c r="F85" s="37"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="33"/>
       <c r="G85" s="27"/>
       <c r="H85" s="6"/>
     </row>
@@ -2159,11 +2162,11 @@
         <v>3</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="38" t="s">
+      <c r="D86" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E86" s="39"/>
-      <c r="F86" s="40"/>
+      <c r="E86" s="40"/>
+      <c r="F86" s="41"/>
       <c r="G86" s="27"/>
       <c r="H86" s="14"/>
     </row>
@@ -2172,11 +2175,11 @@
         <v>4</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="D87" s="35" t="s">
+      <c r="D87" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="E87" s="36"/>
-      <c r="F87" s="37"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="33"/>
       <c r="G87" s="27"/>
       <c r="H87" s="6"/>
     </row>
@@ -2185,11 +2188,11 @@
         <v>5</v>
       </c>
       <c r="C88" s="7"/>
-      <c r="D88" s="38" t="s">
+      <c r="D88" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="E88" s="39"/>
-      <c r="F88" s="40"/>
+      <c r="E88" s="40"/>
+      <c r="F88" s="41"/>
       <c r="G88" s="27"/>
       <c r="H88" s="14"/>
     </row>
@@ -2198,11 +2201,11 @@
         <v>6</v>
       </c>
       <c r="C89" s="7"/>
-      <c r="D89" s="38" t="s">
+      <c r="D89" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="E89" s="39"/>
-      <c r="F89" s="40"/>
+      <c r="E89" s="40"/>
+      <c r="F89" s="41"/>
       <c r="G89" s="27"/>
       <c r="H89" s="14"/>
     </row>
@@ -2211,11 +2214,11 @@
         <v>7</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="38" t="s">
+      <c r="D90" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="E90" s="39"/>
-      <c r="F90" s="40"/>
+      <c r="E90" s="40"/>
+      <c r="F90" s="41"/>
       <c r="G90" s="27"/>
       <c r="H90" s="14"/>
     </row>
@@ -2224,11 +2227,11 @@
         <v>8</v>
       </c>
       <c r="C91" s="7"/>
-      <c r="D91" s="38" t="s">
+      <c r="D91" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="E91" s="39"/>
-      <c r="F91" s="40"/>
+      <c r="E91" s="40"/>
+      <c r="F91" s="41"/>
       <c r="G91" s="27"/>
       <c r="H91" s="14"/>
     </row>
@@ -2237,11 +2240,11 @@
         <v>9</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="38" t="s">
+      <c r="D92" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="E92" s="39"/>
-      <c r="F92" s="40"/>
+      <c r="E92" s="40"/>
+      <c r="F92" s="41"/>
       <c r="G92" s="27"/>
       <c r="H92" s="14"/>
     </row>
@@ -2250,11 +2253,11 @@
         <v>10</v>
       </c>
       <c r="C93" s="7"/>
-      <c r="D93" s="38" t="s">
+      <c r="D93" s="39" t="s">
         <v>89</v>
       </c>
-      <c r="E93" s="39"/>
-      <c r="F93" s="40"/>
+      <c r="E93" s="40"/>
+      <c r="F93" s="41"/>
       <c r="G93" s="27"/>
       <c r="H93" s="14"/>
     </row>
@@ -2263,11 +2266,11 @@
         <v>11</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="38" t="s">
+      <c r="D94" s="39" t="s">
         <v>90</v>
       </c>
-      <c r="E94" s="39"/>
-      <c r="F94" s="40"/>
+      <c r="E94" s="40"/>
+      <c r="F94" s="41"/>
       <c r="G94" s="27"/>
       <c r="H94" s="14"/>
     </row>
@@ -2276,11 +2279,11 @@
         <v>12</v>
       </c>
       <c r="C95" s="7"/>
-      <c r="D95" s="38" t="s">
+      <c r="D95" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="E95" s="39"/>
-      <c r="F95" s="40"/>
+      <c r="E95" s="40"/>
+      <c r="F95" s="41"/>
       <c r="G95" s="27"/>
       <c r="H95" s="14"/>
     </row>
@@ -2289,11 +2292,11 @@
         <v>13</v>
       </c>
       <c r="C96" s="7"/>
-      <c r="D96" s="38" t="s">
+      <c r="D96" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="E96" s="39"/>
-      <c r="F96" s="40"/>
+      <c r="E96" s="40"/>
+      <c r="F96" s="41"/>
       <c r="G96" s="27"/>
       <c r="H96" s="14"/>
     </row>
@@ -2302,11 +2305,11 @@
         <v>14</v>
       </c>
       <c r="C97" s="7"/>
-      <c r="D97" s="38" t="s">
+      <c r="D97" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="E97" s="39"/>
-      <c r="F97" s="40"/>
+      <c r="E97" s="40"/>
+      <c r="F97" s="41"/>
       <c r="G97" s="27"/>
       <c r="H97" s="14"/>
     </row>
@@ -2314,10 +2317,10 @@
       <c r="B100" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C100" s="31" t="s">
+      <c r="C100" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="D100" s="31"/>
+      <c r="D100" s="34"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
     </row>
@@ -2326,11 +2329,11 @@
         <v>1</v>
       </c>
       <c r="C101" s="21"/>
-      <c r="D101" s="41" t="s">
+      <c r="D101" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E101" s="41"/>
-      <c r="F101" s="41"/>
+      <c r="E101" s="35"/>
+      <c r="F101" s="35"/>
       <c r="G101" s="22" t="s">
         <v>3</v>
       </c>
@@ -2343,11 +2346,11 @@
         <v>1</v>
       </c>
       <c r="C102" s="18"/>
-      <c r="D102" s="32" t="s">
+      <c r="D102" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="E102" s="33"/>
-      <c r="F102" s="34"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="38"/>
       <c r="G102" s="26"/>
       <c r="H102" s="19"/>
     </row>
@@ -2355,10 +2358,10 @@
       <c r="B105" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C105" s="31" t="s">
+      <c r="C105" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="D105" s="31"/>
+      <c r="D105" s="34"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
     </row>
@@ -2367,11 +2370,11 @@
         <v>1</v>
       </c>
       <c r="C106" s="21"/>
-      <c r="D106" s="41" t="s">
+      <c r="D106" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E106" s="41"/>
-      <c r="F106" s="41"/>
+      <c r="E106" s="35"/>
+      <c r="F106" s="35"/>
       <c r="G106" s="22" t="s">
         <v>3</v>
       </c>
@@ -2384,11 +2387,11 @@
         <v>1</v>
       </c>
       <c r="C107" s="18"/>
-      <c r="D107" s="32" t="s">
+      <c r="D107" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="E107" s="33"/>
-      <c r="F107" s="34"/>
+      <c r="E107" s="37"/>
+      <c r="F107" s="38"/>
       <c r="G107" s="26"/>
       <c r="H107" s="19"/>
     </row>
@@ -2396,10 +2399,10 @@
       <c r="B110" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C110" s="31" t="s">
+      <c r="C110" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="D110" s="31"/>
+      <c r="D110" s="34"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
     </row>
@@ -2408,11 +2411,11 @@
         <v>1</v>
       </c>
       <c r="C111" s="21"/>
-      <c r="D111" s="41" t="s">
+      <c r="D111" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E111" s="41"/>
-      <c r="F111" s="41"/>
+      <c r="E111" s="35"/>
+      <c r="F111" s="35"/>
       <c r="G111" s="22" t="s">
         <v>3</v>
       </c>
@@ -2425,9 +2428,9 @@
         <v>1</v>
       </c>
       <c r="C112" s="18"/>
-      <c r="D112" s="32"/>
-      <c r="E112" s="33"/>
-      <c r="F112" s="34"/>
+      <c r="D112" s="36"/>
+      <c r="E112" s="37"/>
+      <c r="F112" s="38"/>
       <c r="G112" s="30"/>
       <c r="H112" s="19"/>
     </row>
@@ -2435,10 +2438,10 @@
       <c r="B115" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C115" s="31" t="s">
+      <c r="C115" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="D115" s="31"/>
+      <c r="D115" s="34"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
     </row>
@@ -2447,11 +2450,11 @@
         <v>1</v>
       </c>
       <c r="C116" s="21"/>
-      <c r="D116" s="41" t="s">
+      <c r="D116" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E116" s="41"/>
-      <c r="F116" s="41"/>
+      <c r="E116" s="35"/>
+      <c r="F116" s="35"/>
       <c r="G116" s="22" t="s">
         <v>3</v>
       </c>
@@ -2464,11 +2467,11 @@
         <v>1</v>
       </c>
       <c r="C117" s="18"/>
-      <c r="D117" s="32" t="s">
+      <c r="D117" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="E117" s="33"/>
-      <c r="F117" s="34"/>
+      <c r="E117" s="37"/>
+      <c r="F117" s="38"/>
       <c r="G117" s="26"/>
       <c r="H117" s="19"/>
     </row>
@@ -2477,11 +2480,11 @@
         <v>2</v>
       </c>
       <c r="C118" s="4"/>
-      <c r="D118" s="35" t="s">
+      <c r="D118" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="E118" s="36"/>
-      <c r="F118" s="37"/>
+      <c r="E118" s="32"/>
+      <c r="F118" s="33"/>
       <c r="G118" s="27"/>
       <c r="H118" s="6"/>
     </row>
@@ -2490,11 +2493,11 @@
         <v>3</v>
       </c>
       <c r="C119" s="7"/>
-      <c r="D119" s="38" t="s">
+      <c r="D119" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="E119" s="39"/>
-      <c r="F119" s="40"/>
+      <c r="E119" s="40"/>
+      <c r="F119" s="41"/>
       <c r="G119" s="27"/>
       <c r="H119" s="14"/>
     </row>
@@ -2503,37 +2506,79 @@
         <v>4</v>
       </c>
       <c r="C120" s="4"/>
-      <c r="D120" s="35" t="s">
+      <c r="D120" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="E120" s="36"/>
-      <c r="F120" s="37"/>
+      <c r="E120" s="32"/>
+      <c r="F120" s="33"/>
       <c r="G120" s="27"/>
       <c r="H120" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="D102:F102"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D97:F97"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="D77:F77"/>
+    <mergeCell ref="D78:F78"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
     <mergeCell ref="D37:F37"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="D39:F39"/>
@@ -2550,69 +2595,27 @@
     <mergeCell ref="D28:F28"/>
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="D76:F76"/>
-    <mergeCell ref="D77:F77"/>
-    <mergeCell ref="D78:F78"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D102:F102"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D97:F97"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="D119:F119"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished up to ohne Sternpunkt
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02F9043-D669-445E-986C-424E48612020}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C0A03E-8E47-4C8A-9EE0-00D45F710FA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -361,7 +361,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,15 +400,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +438,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -683,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -745,12 +744,29 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -761,32 +777,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1104,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L88" sqref="L88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1123,13 +1118,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
       <c r="J2" s="11" t="s">
         <v>41</v>
       </c>
@@ -1144,10 +1139,10 @@
       <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="43"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="9"/>
@@ -1160,11 +1155,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="19"/>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="20" t="s">
         <v>3</v>
       </c>
@@ -1181,11 +1176,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="22"/>
       <c r="H6" s="17" t="s">
         <v>11</v>
@@ -1202,11 +1197,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="38"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="22"/>
       <c r="H7" s="6" t="s">
         <v>11</v>
@@ -1217,11 +1212,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="40" t="s">
+      <c r="D8" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="41"/>
-      <c r="F8" s="42"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="10"/>
       <c r="H8" s="14" t="s">
         <v>11</v>
@@ -1232,11 +1227,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="23"/>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -1247,11 +1242,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="42"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="22"/>
       <c r="H10" s="14" t="s">
         <v>45</v>
@@ -1262,11 +1257,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="10"/>
       <c r="H11" s="6"/>
     </row>
@@ -1275,11 +1270,11 @@
         <v>7</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="40" t="s">
+      <c r="D12" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="36"/>
       <c r="G12" s="23"/>
       <c r="H12" s="14"/>
     </row>
@@ -1288,11 +1283,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="38"/>
-      <c r="F13" s="39"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="23"/>
       <c r="H13" s="6"/>
     </row>
@@ -1301,11 +1296,11 @@
         <v>9</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="40" t="s">
+      <c r="D14" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="36"/>
       <c r="G14" s="23"/>
       <c r="H14" s="14"/>
     </row>
@@ -1314,11 +1309,11 @@
         <v>10</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
       <c r="G15" s="23"/>
       <c r="H15" s="6" t="s">
         <v>11</v>
@@ -1329,11 +1324,11 @@
         <v>11</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="41"/>
-      <c r="F16" s="42"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
       <c r="G16" s="23"/>
       <c r="H16" s="14"/>
     </row>
@@ -1342,11 +1337,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="38"/>
-      <c r="F17" s="39"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="23"/>
       <c r="H17" s="4"/>
     </row>
@@ -1355,11 +1350,11 @@
         <v>13</v>
       </c>
       <c r="C18" s="16"/>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="41"/>
       <c r="G18" s="23"/>
       <c r="H18" s="16"/>
     </row>
@@ -1368,11 +1363,11 @@
         <v>14</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="39"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
       <c r="G19" s="23"/>
       <c r="H19" s="4"/>
     </row>
@@ -1381,11 +1376,11 @@
         <v>15</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="41"/>
-      <c r="F20" s="42"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="36"/>
       <c r="G20" s="23"/>
       <c r="H20" s="7"/>
     </row>
@@ -1394,11 +1389,11 @@
         <v>16</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="39"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="23"/>
       <c r="H21" s="4"/>
     </row>
@@ -1407,11 +1402,11 @@
         <v>17</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="42"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="36"/>
       <c r="G22" s="23"/>
       <c r="H22" s="7"/>
     </row>
@@ -1420,11 +1415,11 @@
         <v>18</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="39"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="23"/>
       <c r="H23" s="4"/>
     </row>
@@ -1433,11 +1428,11 @@
         <v>19</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
       <c r="G24" s="23"/>
       <c r="H24" s="7"/>
     </row>
@@ -1446,11 +1441,11 @@
         <v>20</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="39"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="23"/>
       <c r="H25" s="4"/>
     </row>
@@ -1459,11 +1454,11 @@
         <v>21</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="42"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="23"/>
       <c r="H26" s="7"/>
     </row>
@@ -1472,11 +1467,11 @@
         <v>22</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="38"/>
-      <c r="F27" s="39"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
       <c r="G27" s="23"/>
       <c r="H27" s="4"/>
     </row>
@@ -1485,11 +1480,11 @@
         <v>23</v>
       </c>
       <c r="C28" s="16"/>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="23"/>
       <c r="H28" s="16"/>
     </row>
@@ -1498,11 +1493,11 @@
         <v>24</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="38"/>
-      <c r="F29" s="39"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
       <c r="G29" s="23"/>
       <c r="H29" s="4"/>
     </row>
@@ -1511,11 +1506,11 @@
         <v>25</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="41"/>
-      <c r="F30" s="42"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="36"/>
       <c r="G30" s="23"/>
       <c r="H30" s="7"/>
     </row>
@@ -1524,11 +1519,11 @@
         <v>26</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="38"/>
-      <c r="F31" s="39"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="23"/>
       <c r="H31" s="4" t="s">
         <v>44</v>
@@ -1539,11 +1534,11 @@
         <v>27</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="42"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="23"/>
       <c r="H32" s="29" t="s">
         <v>11</v>
@@ -1554,11 +1549,11 @@
         <v>28</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="37" t="s">
+      <c r="D33" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="39"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
       <c r="G33" s="23"/>
       <c r="H33" s="4"/>
     </row>
@@ -1567,11 +1562,11 @@
         <v>29</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="41"/>
-      <c r="F34" s="42"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="23"/>
       <c r="H34" s="7"/>
     </row>
@@ -1580,11 +1575,11 @@
         <v>30</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="38"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
       <c r="G35" s="23"/>
       <c r="H35" s="4"/>
     </row>
@@ -1593,11 +1588,11 @@
         <v>31</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="40" t="s">
+      <c r="D36" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="42"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="23"/>
       <c r="H36" s="7"/>
     </row>
@@ -1606,11 +1601,11 @@
         <v>32</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="37" t="s">
+      <c r="D37" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="23"/>
       <c r="H37" s="4"/>
     </row>
@@ -1619,11 +1614,11 @@
         <v>33</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="41"/>
       <c r="G38" s="23"/>
       <c r="H38" s="16"/>
     </row>
@@ -1632,11 +1627,11 @@
         <v>34</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="39"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
       <c r="G39" s="23"/>
       <c r="H39" s="4"/>
     </row>
@@ -1644,10 +1639,10 @@
       <c r="B42" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="43"/>
+      <c r="D42" s="38"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
@@ -1656,11 +1651,11 @@
         <v>1</v>
       </c>
       <c r="C43" s="19"/>
-      <c r="D43" s="44" t="s">
+      <c r="D43" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="44"/>
-      <c r="F43" s="44"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
       <c r="G43" s="20" t="s">
         <v>3</v>
       </c>
@@ -1673,11 +1668,11 @@
         <v>1</v>
       </c>
       <c r="C44" s="16"/>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="35"/>
-      <c r="F44" s="36"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="41"/>
       <c r="G44" s="23"/>
       <c r="H44" s="17"/>
     </row>
@@ -1686,11 +1681,11 @@
         <v>2</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="37" t="s">
+      <c r="D45" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="38"/>
-      <c r="F45" s="39"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
       <c r="G45" s="23"/>
       <c r="H45" s="6"/>
     </row>
@@ -1699,11 +1694,11 @@
         <v>3</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="41"/>
-      <c r="F46" s="42"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="36"/>
       <c r="G46" s="23"/>
       <c r="H46" s="14"/>
     </row>
@@ -1712,11 +1707,11 @@
         <v>4</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="37" t="s">
+      <c r="D47" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="38"/>
-      <c r="F47" s="39"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
       <c r="G47" s="23"/>
       <c r="H47" s="6" t="s">
         <v>90</v>
@@ -1727,11 +1722,11 @@
         <v>5</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="40" t="s">
+      <c r="D48" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="41"/>
-      <c r="F48" s="42"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="36"/>
       <c r="G48" s="23"/>
       <c r="H48" s="14"/>
     </row>
@@ -1740,11 +1735,11 @@
         <v>6</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="37" t="s">
+      <c r="D49" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="38"/>
-      <c r="F49" s="39"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
       <c r="G49" s="23"/>
       <c r="H49" s="6"/>
     </row>
@@ -1753,11 +1748,11 @@
         <v>7</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="40" t="s">
+      <c r="D50" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="41"/>
-      <c r="F50" s="42"/>
+      <c r="E50" s="35"/>
+      <c r="F50" s="36"/>
       <c r="G50" s="23"/>
       <c r="H50" s="14" t="s">
         <v>58</v>
@@ -1767,10 +1762,10 @@
       <c r="B53" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="43" t="s">
+      <c r="C53" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="43"/>
+      <c r="D53" s="38"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
@@ -1779,11 +1774,11 @@
         <v>1</v>
       </c>
       <c r="C54" s="19"/>
-      <c r="D54" s="44" t="s">
+      <c r="D54" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="44"/>
-      <c r="F54" s="44"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
       <c r="G54" s="20" t="s">
         <v>3</v>
       </c>
@@ -1796,11 +1791,11 @@
         <v>1</v>
       </c>
       <c r="C55" s="16"/>
-      <c r="D55" s="34" t="s">
+      <c r="D55" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="35"/>
-      <c r="F55" s="36"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="41"/>
       <c r="G55" s="23"/>
       <c r="H55" s="15"/>
     </row>
@@ -1809,11 +1804,11 @@
         <v>2</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="37" t="s">
+      <c r="D56" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="38"/>
-      <c r="F56" s="39"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="33"/>
       <c r="G56" s="23"/>
       <c r="H56" s="5"/>
     </row>
@@ -1822,11 +1817,11 @@
         <v>3</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="D57" s="40" t="s">
+      <c r="D57" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="41"/>
-      <c r="F57" s="42"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="36"/>
       <c r="G57" s="23"/>
       <c r="H57" s="13"/>
     </row>
@@ -1835,11 +1830,11 @@
         <v>4</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="37" t="s">
+      <c r="D58" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="38"/>
-      <c r="F58" s="39"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="33"/>
       <c r="G58" s="23"/>
       <c r="H58" s="5"/>
     </row>
@@ -1848,11 +1843,11 @@
         <v>5</v>
       </c>
       <c r="C59" s="7"/>
-      <c r="D59" s="40" t="s">
+      <c r="D59" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="41"/>
-      <c r="F59" s="42"/>
+      <c r="E59" s="35"/>
+      <c r="F59" s="36"/>
       <c r="G59" s="23"/>
       <c r="H59" s="13"/>
     </row>
@@ -1861,11 +1856,11 @@
         <v>6</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="37" t="s">
+      <c r="D60" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="38"/>
-      <c r="F60" s="39"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="33"/>
       <c r="G60" s="23"/>
       <c r="H60" s="5"/>
     </row>
@@ -1874,11 +1869,11 @@
         <v>7</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="40" t="s">
+      <c r="D61" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="41"/>
-      <c r="F61" s="42"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="36"/>
       <c r="G61" s="23"/>
       <c r="H61" s="13"/>
     </row>
@@ -1887,11 +1882,11 @@
         <v>8</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="37" t="s">
+      <c r="D62" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="38"/>
-      <c r="F62" s="39"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="33"/>
       <c r="G62" s="23"/>
       <c r="H62" s="5"/>
     </row>
@@ -1900,11 +1895,11 @@
         <v>9</v>
       </c>
       <c r="C63" s="7"/>
-      <c r="D63" s="40" t="s">
+      <c r="D63" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="41"/>
-      <c r="F63" s="42"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="36"/>
       <c r="G63" s="23"/>
       <c r="H63" s="13"/>
     </row>
@@ -1913,11 +1908,11 @@
         <v>10</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="37" t="s">
+      <c r="D64" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="38"/>
-      <c r="F64" s="39"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="33"/>
       <c r="G64" s="23"/>
       <c r="H64" s="5"/>
     </row>
@@ -1928,11 +1923,11 @@
       <c r="C65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="40" t="s">
+      <c r="D65" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="41"/>
-      <c r="F65" s="42"/>
+      <c r="E65" s="35"/>
+      <c r="F65" s="36"/>
       <c r="G65" s="25"/>
       <c r="H65" s="28" t="s">
         <v>91</v>
@@ -1942,10 +1937,10 @@
       <c r="B68" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="43" t="s">
+      <c r="C68" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="43"/>
+      <c r="D68" s="38"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
@@ -1954,11 +1949,11 @@
         <v>1</v>
       </c>
       <c r="C69" s="19"/>
-      <c r="D69" s="44" t="s">
+      <c r="D69" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="44"/>
-      <c r="F69" s="44"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
       <c r="G69" s="20" t="s">
         <v>3</v>
       </c>
@@ -1971,11 +1966,11 @@
         <v>1</v>
       </c>
       <c r="C70" s="16"/>
-      <c r="D70" s="34" t="s">
+      <c r="D70" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="E70" s="35"/>
-      <c r="F70" s="36"/>
+      <c r="E70" s="40"/>
+      <c r="F70" s="41"/>
       <c r="G70" s="23"/>
       <c r="H70" s="15"/>
     </row>
@@ -1984,11 +1979,11 @@
         <v>2</v>
       </c>
       <c r="C71" s="4"/>
-      <c r="D71" s="37" t="s">
+      <c r="D71" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="38"/>
-      <c r="F71" s="39"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="33"/>
       <c r="G71" s="23"/>
       <c r="H71" s="5"/>
     </row>
@@ -1997,11 +1992,11 @@
         <v>3</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="D72" s="40" t="s">
+      <c r="D72" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="E72" s="41"/>
-      <c r="F72" s="42"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="36"/>
       <c r="G72" s="23"/>
       <c r="H72" s="13"/>
     </row>
@@ -2010,11 +2005,11 @@
         <v>4</v>
       </c>
       <c r="C73" s="4"/>
-      <c r="D73" s="37" t="s">
+      <c r="D73" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="E73" s="38"/>
-      <c r="F73" s="39"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="33"/>
       <c r="G73" s="23"/>
       <c r="H73" s="5"/>
     </row>
@@ -2023,11 +2018,11 @@
         <v>5</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="D74" s="40" t="s">
+      <c r="D74" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="E74" s="41"/>
-      <c r="F74" s="42"/>
+      <c r="E74" s="35"/>
+      <c r="F74" s="36"/>
       <c r="G74" s="23"/>
       <c r="H74" s="13"/>
     </row>
@@ -2036,11 +2031,11 @@
         <v>6</v>
       </c>
       <c r="C75" s="4"/>
-      <c r="D75" s="37" t="s">
+      <c r="D75" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="E75" s="38"/>
-      <c r="F75" s="39"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="33"/>
       <c r="G75" s="23"/>
       <c r="H75" s="5"/>
     </row>
@@ -2048,10 +2043,10 @@
       <c r="B78" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="43" t="s">
+      <c r="C78" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D78" s="43"/>
+      <c r="D78" s="38"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
@@ -2060,11 +2055,11 @@
         <v>1</v>
       </c>
       <c r="C79" s="19"/>
-      <c r="D79" s="44" t="s">
+      <c r="D79" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="37"/>
       <c r="G79" s="20" t="s">
         <v>3</v>
       </c>
@@ -2077,12 +2072,12 @@
         <v>1</v>
       </c>
       <c r="C80" s="16"/>
-      <c r="D80" s="34" t="s">
+      <c r="D80" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="E80" s="35"/>
-      <c r="F80" s="36"/>
-      <c r="G80" s="32"/>
+      <c r="E80" s="40"/>
+      <c r="F80" s="41"/>
+      <c r="G80" s="23"/>
       <c r="H80" s="15"/>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.3">
@@ -2090,25 +2085,25 @@
         <v>2</v>
       </c>
       <c r="C81" s="4"/>
-      <c r="D81" s="37" t="s">
+      <c r="D81" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E81" s="38"/>
-      <c r="F81" s="39"/>
-      <c r="G81" s="33"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="23"/>
       <c r="H81" s="5"/>
     </row>
-    <row r="82" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B82" s="13">
         <v>3</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="D82" s="40" t="s">
+      <c r="D82" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="E82" s="41"/>
-      <c r="F82" s="42"/>
-      <c r="G82" s="32"/>
+      <c r="E82" s="35"/>
+      <c r="F82" s="36"/>
+      <c r="G82" s="23"/>
       <c r="H82" s="13"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.3">
@@ -2116,12 +2111,12 @@
         <v>4</v>
       </c>
       <c r="C83" s="4"/>
-      <c r="D83" s="37" t="s">
+      <c r="D83" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="E83" s="38"/>
-      <c r="F83" s="39"/>
-      <c r="G83" s="24"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="23"/>
       <c r="H83" s="5"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.3">
@@ -2129,12 +2124,12 @@
         <v>5</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="40" t="s">
+      <c r="D84" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="E84" s="41"/>
-      <c r="F84" s="42"/>
-      <c r="G84" s="25"/>
+      <c r="E84" s="35"/>
+      <c r="F84" s="36"/>
+      <c r="G84" s="23"/>
       <c r="H84" s="13"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.3">
@@ -2142,12 +2137,12 @@
         <v>6</v>
       </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="37" t="s">
+      <c r="D85" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="E85" s="38"/>
-      <c r="F85" s="39"/>
-      <c r="G85" s="31"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="23"/>
       <c r="H85" s="5"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.3">
@@ -2155,12 +2150,12 @@
         <v>7</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="40" t="s">
+      <c r="D86" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="E86" s="41"/>
-      <c r="F86" s="42"/>
-      <c r="G86" s="31"/>
+      <c r="E86" s="35"/>
+      <c r="F86" s="36"/>
+      <c r="G86" s="43"/>
       <c r="H86" s="13"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
@@ -2168,11 +2163,11 @@
         <v>8</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="D87" s="37" t="s">
+      <c r="D87" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E87" s="38"/>
-      <c r="F87" s="39"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="33"/>
       <c r="G87" s="25"/>
       <c r="H87" s="5"/>
     </row>
@@ -2181,11 +2176,11 @@
         <v>9</v>
       </c>
       <c r="C88" s="16"/>
-      <c r="D88" s="34" t="s">
+      <c r="D88" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="E88" s="35"/>
-      <c r="F88" s="36"/>
+      <c r="E88" s="40"/>
+      <c r="F88" s="41"/>
       <c r="G88" s="25"/>
       <c r="H88" s="13"/>
     </row>
@@ -2194,11 +2189,11 @@
         <v>10</v>
       </c>
       <c r="C89" s="4"/>
-      <c r="D89" s="37" t="s">
+      <c r="D89" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E89" s="38"/>
-      <c r="F89" s="39"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="33"/>
       <c r="G89" s="25"/>
       <c r="H89" s="5"/>
     </row>
@@ -2207,11 +2202,11 @@
         <v>11</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="40" t="s">
+      <c r="D90" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="E90" s="41"/>
-      <c r="F90" s="42"/>
+      <c r="E90" s="35"/>
+      <c r="F90" s="36"/>
       <c r="G90" s="25"/>
       <c r="H90" s="13"/>
     </row>
@@ -2220,11 +2215,11 @@
         <v>12</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="D91" s="37" t="s">
+      <c r="D91" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E91" s="38"/>
-      <c r="F91" s="39"/>
+      <c r="E91" s="32"/>
+      <c r="F91" s="33"/>
       <c r="G91" s="25"/>
       <c r="H91" s="5"/>
     </row>
@@ -2233,11 +2228,11 @@
         <v>13</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="40" t="s">
+      <c r="D92" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="E92" s="41"/>
-      <c r="F92" s="42"/>
+      <c r="E92" s="35"/>
+      <c r="F92" s="36"/>
       <c r="G92" s="25"/>
       <c r="H92" s="15"/>
     </row>
@@ -2246,11 +2241,11 @@
         <v>14</v>
       </c>
       <c r="C93" s="4"/>
-      <c r="D93" s="37" t="s">
+      <c r="D93" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E93" s="38"/>
-      <c r="F93" s="39"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="33"/>
       <c r="G93" s="25"/>
       <c r="H93" s="5"/>
     </row>
@@ -2259,11 +2254,11 @@
         <v>15</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="40" t="s">
+      <c r="D94" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="E94" s="41"/>
-      <c r="F94" s="42"/>
+      <c r="E94" s="35"/>
+      <c r="F94" s="36"/>
       <c r="G94" s="25"/>
       <c r="H94" s="13"/>
     </row>
@@ -2272,11 +2267,11 @@
         <v>16</v>
       </c>
       <c r="C95" s="4"/>
-      <c r="D95" s="37" t="s">
+      <c r="D95" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E95" s="38"/>
-      <c r="F95" s="39"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="33"/>
       <c r="G95" s="25"/>
       <c r="H95" s="5"/>
     </row>
@@ -2285,11 +2280,11 @@
         <v>17</v>
       </c>
       <c r="C96" s="16"/>
-      <c r="D96" s="34" t="s">
+      <c r="D96" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="E96" s="35"/>
-      <c r="F96" s="36"/>
+      <c r="E96" s="40"/>
+      <c r="F96" s="41"/>
       <c r="G96" s="30"/>
       <c r="H96" s="13"/>
     </row>
@@ -2297,10 +2292,10 @@
       <c r="B99" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C99" s="43" t="s">
+      <c r="C99" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="43"/>
+      <c r="D99" s="38"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
     </row>
@@ -2309,11 +2304,11 @@
         <v>1</v>
       </c>
       <c r="C100" s="19"/>
-      <c r="D100" s="44" t="s">
+      <c r="D100" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E100" s="44"/>
-      <c r="F100" s="44"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="37"/>
       <c r="G100" s="20" t="s">
         <v>3</v>
       </c>
@@ -2326,11 +2321,11 @@
         <v>1</v>
       </c>
       <c r="C101" s="16"/>
-      <c r="D101" s="34" t="s">
+      <c r="D101" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="E101" s="35"/>
-      <c r="F101" s="36"/>
+      <c r="E101" s="40"/>
+      <c r="F101" s="41"/>
       <c r="G101" s="24"/>
       <c r="H101" s="17"/>
     </row>
@@ -2338,10 +2333,10 @@
       <c r="B104" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C104" s="43" t="s">
+      <c r="C104" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="D104" s="43"/>
+      <c r="D104" s="38"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
@@ -2350,11 +2345,11 @@
         <v>1</v>
       </c>
       <c r="C105" s="19"/>
-      <c r="D105" s="44" t="s">
+      <c r="D105" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="44"/>
-      <c r="F105" s="44"/>
+      <c r="E105" s="37"/>
+      <c r="F105" s="37"/>
       <c r="G105" s="20" t="s">
         <v>3</v>
       </c>
@@ -2367,11 +2362,11 @@
         <v>1</v>
       </c>
       <c r="C106" s="16"/>
-      <c r="D106" s="34" t="s">
+      <c r="D106" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="E106" s="35"/>
-      <c r="F106" s="36"/>
+      <c r="E106" s="40"/>
+      <c r="F106" s="41"/>
       <c r="G106" s="24"/>
       <c r="H106" s="17"/>
     </row>
@@ -2379,10 +2374,10 @@
       <c r="B109" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C109" s="43" t="s">
+      <c r="C109" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="D109" s="43"/>
+      <c r="D109" s="38"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
     </row>
@@ -2391,11 +2386,11 @@
         <v>1</v>
       </c>
       <c r="C110" s="19"/>
-      <c r="D110" s="44" t="s">
+      <c r="D110" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E110" s="44"/>
-      <c r="F110" s="44"/>
+      <c r="E110" s="37"/>
+      <c r="F110" s="37"/>
       <c r="G110" s="20" t="s">
         <v>3</v>
       </c>
@@ -2408,11 +2403,11 @@
         <v>1</v>
       </c>
       <c r="C111" s="16"/>
-      <c r="D111" s="34" t="s">
+      <c r="D111" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="E111" s="35"/>
-      <c r="F111" s="36"/>
+      <c r="E111" s="40"/>
+      <c r="F111" s="41"/>
       <c r="G111" s="24"/>
       <c r="H111" s="17"/>
     </row>
@@ -2421,11 +2416,11 @@
         <v>2</v>
       </c>
       <c r="C112" s="4"/>
-      <c r="D112" s="37" t="s">
+      <c r="D112" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="E112" s="38"/>
-      <c r="F112" s="39"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="33"/>
       <c r="G112" s="25"/>
       <c r="H112" s="6"/>
     </row>
@@ -2434,11 +2429,11 @@
         <v>3</v>
       </c>
       <c r="C113" s="7"/>
-      <c r="D113" s="40" t="s">
+      <c r="D113" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E113" s="41"/>
-      <c r="F113" s="42"/>
+      <c r="E113" s="35"/>
+      <c r="F113" s="36"/>
       <c r="G113" s="25"/>
       <c r="H113" s="14"/>
     </row>
@@ -2447,73 +2442,41 @@
         <v>4</v>
       </c>
       <c r="C114" s="4"/>
-      <c r="D114" s="37" t="s">
+      <c r="D114" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E114" s="38"/>
-      <c r="F114" s="39"/>
+      <c r="E114" s="32"/>
+      <c r="F114" s="33"/>
       <c r="G114" s="25"/>
       <c r="H114" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="98">
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="D114:F114"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="D39:F39"/>
     <mergeCell ref="B2:F2"/>
@@ -2530,31 +2493,63 @@
     <mergeCell ref="D29:F29"/>
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="D114:F114"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="D111:F111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Up to Ströme ohne Sternpunkt
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C0A03E-8E47-4C8A-9EE0-00D45F710FA5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5ECE17-64E0-47FD-9417-2396FACDC26D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="110">
   <si>
     <t xml:space="preserve">Liste der zu zeichnenden Zeigerdiagramme </t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>Erzeugung Drehfeld III c)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serien vs. Parallelschwingkreis I </t>
+  </si>
+  <si>
+    <t>Clicker</t>
   </si>
 </sst>
 </file>
@@ -682,7 +688,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -744,6 +750,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -762,26 +780,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1097,10 +1106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
-  <dimension ref="B2:K114"/>
+  <dimension ref="B2:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L88" sqref="L88"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L93" sqref="L93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,13 +1127,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
       <c r="J2" s="11" t="s">
         <v>41</v>
       </c>
@@ -1139,10 +1148,10 @@
       <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="9"/>
@@ -1155,11 +1164,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="19"/>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="20" t="s">
         <v>3</v>
       </c>
@@ -1176,11 +1185,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="22"/>
       <c r="H6" s="17" t="s">
         <v>11</v>
@@ -1197,11 +1206,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="22"/>
       <c r="H7" s="6" t="s">
         <v>11</v>
@@ -1212,11 +1221,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="40"/>
       <c r="G8" s="10"/>
       <c r="H8" s="14" t="s">
         <v>11</v>
@@ -1227,11 +1236,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
       <c r="G9" s="23"/>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -1242,11 +1251,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="22"/>
       <c r="H10" s="14" t="s">
         <v>45</v>
@@ -1257,11 +1266,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="10"/>
       <c r="H11" s="6"/>
     </row>
@@ -1270,11 +1279,11 @@
         <v>7</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="36"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="23"/>
       <c r="H12" s="14"/>
     </row>
@@ -1283,11 +1292,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="23"/>
       <c r="H13" s="6"/>
     </row>
@@ -1296,11 +1305,11 @@
         <v>9</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="23"/>
       <c r="H14" s="14"/>
     </row>
@@ -1309,11 +1318,11 @@
         <v>10</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
       <c r="G15" s="23"/>
       <c r="H15" s="6" t="s">
         <v>11</v>
@@ -1324,11 +1333,11 @@
         <v>11</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
       <c r="G16" s="23"/>
       <c r="H16" s="14"/>
     </row>
@@ -1337,11 +1346,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
       <c r="G17" s="23"/>
       <c r="H17" s="4"/>
     </row>
@@ -1350,11 +1359,11 @@
         <v>13</v>
       </c>
       <c r="C18" s="16"/>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="41"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="23"/>
       <c r="H18" s="16"/>
     </row>
@@ -1363,11 +1372,11 @@
         <v>14</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="23"/>
       <c r="H19" s="4"/>
     </row>
@@ -1376,11 +1385,11 @@
         <v>15</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="36"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="40"/>
       <c r="G20" s="23"/>
       <c r="H20" s="7"/>
     </row>
@@ -1389,11 +1398,11 @@
         <v>16</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="23"/>
       <c r="H21" s="4"/>
     </row>
@@ -1402,11 +1411,11 @@
         <v>17</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="35"/>
-      <c r="F22" s="36"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="40"/>
       <c r="G22" s="23"/>
       <c r="H22" s="7"/>
     </row>
@@ -1415,11 +1424,11 @@
         <v>18</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="37"/>
       <c r="G23" s="23"/>
       <c r="H23" s="4"/>
     </row>
@@ -1428,11 +1437,11 @@
         <v>19</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="40"/>
       <c r="G24" s="23"/>
       <c r="H24" s="7"/>
     </row>
@@ -1441,11 +1450,11 @@
         <v>20</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="37"/>
       <c r="G25" s="23"/>
       <c r="H25" s="4"/>
     </row>
@@ -1454,11 +1463,11 @@
         <v>21</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="40"/>
       <c r="G26" s="23"/>
       <c r="H26" s="7"/>
     </row>
@@ -1467,11 +1476,11 @@
         <v>22</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="37"/>
       <c r="G27" s="23"/>
       <c r="H27" s="4"/>
     </row>
@@ -1480,11 +1489,11 @@
         <v>23</v>
       </c>
       <c r="C28" s="16"/>
-      <c r="D28" s="39" t="s">
+      <c r="D28" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="40"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="23"/>
       <c r="H28" s="16"/>
     </row>
@@ -1493,11 +1502,11 @@
         <v>24</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="37"/>
       <c r="G29" s="23"/>
       <c r="H29" s="4"/>
     </row>
@@ -1506,11 +1515,11 @@
         <v>25</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="36"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="40"/>
       <c r="G30" s="23"/>
       <c r="H30" s="7"/>
     </row>
@@ -1519,11 +1528,11 @@
         <v>26</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="37"/>
       <c r="G31" s="23"/>
       <c r="H31" s="4" t="s">
         <v>44</v>
@@ -1534,11 +1543,11 @@
         <v>27</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="35"/>
-      <c r="F32" s="36"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="40"/>
       <c r="G32" s="23"/>
       <c r="H32" s="29" t="s">
         <v>11</v>
@@ -1549,11 +1558,11 @@
         <v>28</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="37"/>
       <c r="G33" s="23"/>
       <c r="H33" s="4"/>
     </row>
@@ -1562,11 +1571,11 @@
         <v>29</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="35"/>
-      <c r="F34" s="36"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="40"/>
       <c r="G34" s="23"/>
       <c r="H34" s="7"/>
     </row>
@@ -1575,11 +1584,11 @@
         <v>30</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="37"/>
       <c r="G35" s="23"/>
       <c r="H35" s="4"/>
     </row>
@@ -1588,11 +1597,11 @@
         <v>31</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="35"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="23"/>
       <c r="H36" s="7"/>
     </row>
@@ -1601,11 +1610,11 @@
         <v>32</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="37"/>
       <c r="G37" s="23"/>
       <c r="H37" s="4"/>
     </row>
@@ -1614,11 +1623,11 @@
         <v>33</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="40"/>
-      <c r="F38" s="41"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="23"/>
       <c r="H38" s="16"/>
     </row>
@@ -1627,11 +1636,11 @@
         <v>34</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="37"/>
       <c r="G39" s="23"/>
       <c r="H39" s="4"/>
     </row>
@@ -1639,10 +1648,10 @@
       <c r="B42" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="38" t="s">
+      <c r="C42" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="38"/>
+      <c r="D42" s="41"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
@@ -1651,11 +1660,11 @@
         <v>1</v>
       </c>
       <c r="C43" s="19"/>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
       <c r="G43" s="20" t="s">
         <v>3</v>
       </c>
@@ -1668,11 +1677,11 @@
         <v>1</v>
       </c>
       <c r="C44" s="16"/>
-      <c r="D44" s="39" t="s">
+      <c r="D44" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="40"/>
-      <c r="F44" s="41"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="34"/>
       <c r="G44" s="23"/>
       <c r="H44" s="17"/>
     </row>
@@ -1681,11 +1690,11 @@
         <v>2</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="32"/>
-      <c r="F45" s="33"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="37"/>
       <c r="G45" s="23"/>
       <c r="H45" s="6"/>
     </row>
@@ -1694,11 +1703,11 @@
         <v>3</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="34" t="s">
+      <c r="D46" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="40"/>
       <c r="G46" s="23"/>
       <c r="H46" s="14"/>
     </row>
@@ -1707,11 +1716,11 @@
         <v>4</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="33"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="37"/>
       <c r="G47" s="23"/>
       <c r="H47" s="6" t="s">
         <v>90</v>
@@ -1722,11 +1731,11 @@
         <v>5</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="35"/>
-      <c r="F48" s="36"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="40"/>
       <c r="G48" s="23"/>
       <c r="H48" s="14"/>
     </row>
@@ -1735,11 +1744,11 @@
         <v>6</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="32"/>
-      <c r="F49" s="33"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="37"/>
       <c r="G49" s="23"/>
       <c r="H49" s="6"/>
     </row>
@@ -1748,24 +1757,37 @@
         <v>7</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="35"/>
-      <c r="F50" s="36"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="40"/>
       <c r="G50" s="23"/>
       <c r="H50" s="14" t="s">
         <v>58</v>
       </c>
     </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51" s="13">
+        <v>8</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="38" t="s">
+        <v>108</v>
+      </c>
+      <c r="E51" s="39"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="14"/>
+    </row>
     <row r="53" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="38" t="s">
+      <c r="C53" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="38"/>
+      <c r="D53" s="41"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
@@ -1774,11 +1796,11 @@
         <v>1</v>
       </c>
       <c r="C54" s="19"/>
-      <c r="D54" s="37" t="s">
+      <c r="D54" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
       <c r="G54" s="20" t="s">
         <v>3</v>
       </c>
@@ -1791,11 +1813,11 @@
         <v>1</v>
       </c>
       <c r="C55" s="16"/>
-      <c r="D55" s="39" t="s">
+      <c r="D55" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="40"/>
-      <c r="F55" s="41"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="34"/>
       <c r="G55" s="23"/>
       <c r="H55" s="15"/>
     </row>
@@ -1804,11 +1826,11 @@
         <v>2</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="31" t="s">
+      <c r="D56" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="32"/>
-      <c r="F56" s="33"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="37"/>
       <c r="G56" s="23"/>
       <c r="H56" s="5"/>
     </row>
@@ -1817,11 +1839,11 @@
         <v>3</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="D57" s="34" t="s">
+      <c r="D57" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="35"/>
-      <c r="F57" s="36"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="40"/>
       <c r="G57" s="23"/>
       <c r="H57" s="13"/>
     </row>
@@ -1830,11 +1852,11 @@
         <v>4</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="31" t="s">
+      <c r="D58" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="32"/>
-      <c r="F58" s="33"/>
+      <c r="E58" s="36"/>
+      <c r="F58" s="37"/>
       <c r="G58" s="23"/>
       <c r="H58" s="5"/>
     </row>
@@ -1843,11 +1865,11 @@
         <v>5</v>
       </c>
       <c r="C59" s="7"/>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="35"/>
-      <c r="F59" s="36"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="40"/>
       <c r="G59" s="23"/>
       <c r="H59" s="13"/>
     </row>
@@ -1856,11 +1878,11 @@
         <v>6</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="31" t="s">
+      <c r="D60" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="32"/>
-      <c r="F60" s="33"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="37"/>
       <c r="G60" s="23"/>
       <c r="H60" s="5"/>
     </row>
@@ -1869,11 +1891,11 @@
         <v>7</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="34" t="s">
+      <c r="D61" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="35"/>
-      <c r="F61" s="36"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="40"/>
       <c r="G61" s="23"/>
       <c r="H61" s="13"/>
     </row>
@@ -1882,11 +1904,11 @@
         <v>8</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="31" t="s">
+      <c r="D62" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="32"/>
-      <c r="F62" s="33"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="37"/>
       <c r="G62" s="23"/>
       <c r="H62" s="5"/>
     </row>
@@ -1895,11 +1917,11 @@
         <v>9</v>
       </c>
       <c r="C63" s="7"/>
-      <c r="D63" s="34" t="s">
+      <c r="D63" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="35"/>
-      <c r="F63" s="36"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="40"/>
       <c r="G63" s="23"/>
       <c r="H63" s="13"/>
     </row>
@@ -1908,11 +1930,11 @@
         <v>10</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="31" t="s">
+      <c r="D64" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="32"/>
-      <c r="F64" s="33"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="37"/>
       <c r="G64" s="23"/>
       <c r="H64" s="5"/>
     </row>
@@ -1923,11 +1945,11 @@
       <c r="C65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="34" t="s">
+      <c r="D65" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="35"/>
-      <c r="F65" s="36"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="40"/>
       <c r="G65" s="25"/>
       <c r="H65" s="28" t="s">
         <v>91</v>
@@ -1937,10 +1959,10 @@
       <c r="B68" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="38" t="s">
+      <c r="C68" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="38"/>
+      <c r="D68" s="41"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
@@ -1949,11 +1971,11 @@
         <v>1</v>
       </c>
       <c r="C69" s="19"/>
-      <c r="D69" s="37" t="s">
+      <c r="D69" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
       <c r="G69" s="20" t="s">
         <v>3</v>
       </c>
@@ -1966,11 +1988,11 @@
         <v>1</v>
       </c>
       <c r="C70" s="16"/>
-      <c r="D70" s="39" t="s">
+      <c r="D70" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="E70" s="40"/>
-      <c r="F70" s="41"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="34"/>
       <c r="G70" s="23"/>
       <c r="H70" s="15"/>
     </row>
@@ -1979,11 +2001,11 @@
         <v>2</v>
       </c>
       <c r="C71" s="4"/>
-      <c r="D71" s="31" t="s">
+      <c r="D71" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="32"/>
-      <c r="F71" s="33"/>
+      <c r="E71" s="36"/>
+      <c r="F71" s="37"/>
       <c r="G71" s="23"/>
       <c r="H71" s="5"/>
     </row>
@@ -1992,11 +2014,11 @@
         <v>3</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="D72" s="34" t="s">
+      <c r="D72" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="E72" s="35"/>
-      <c r="F72" s="36"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="40"/>
       <c r="G72" s="23"/>
       <c r="H72" s="13"/>
     </row>
@@ -2005,11 +2027,11 @@
         <v>4</v>
       </c>
       <c r="C73" s="4"/>
-      <c r="D73" s="31" t="s">
+      <c r="D73" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="E73" s="32"/>
-      <c r="F73" s="33"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="37"/>
       <c r="G73" s="23"/>
       <c r="H73" s="5"/>
     </row>
@@ -2018,11 +2040,11 @@
         <v>5</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="D74" s="34" t="s">
+      <c r="D74" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E74" s="35"/>
-      <c r="F74" s="36"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="40"/>
       <c r="G74" s="23"/>
       <c r="H74" s="13"/>
     </row>
@@ -2031,11 +2053,11 @@
         <v>6</v>
       </c>
       <c r="C75" s="4"/>
-      <c r="D75" s="31" t="s">
+      <c r="D75" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="E75" s="32"/>
-      <c r="F75" s="33"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="37"/>
       <c r="G75" s="23"/>
       <c r="H75" s="5"/>
     </row>
@@ -2043,10 +2065,10 @@
       <c r="B78" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="38" t="s">
+      <c r="C78" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="D78" s="38"/>
+      <c r="D78" s="41"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
@@ -2055,11 +2077,11 @@
         <v>1</v>
       </c>
       <c r="C79" s="19"/>
-      <c r="D79" s="37" t="s">
+      <c r="D79" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
+      <c r="E79" s="42"/>
+      <c r="F79" s="42"/>
       <c r="G79" s="20" t="s">
         <v>3</v>
       </c>
@@ -2072,11 +2094,11 @@
         <v>1</v>
       </c>
       <c r="C80" s="16"/>
-      <c r="D80" s="39" t="s">
+      <c r="D80" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="E80" s="40"/>
-      <c r="F80" s="41"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="34"/>
       <c r="G80" s="23"/>
       <c r="H80" s="15"/>
     </row>
@@ -2085,11 +2107,11 @@
         <v>2</v>
       </c>
       <c r="C81" s="4"/>
-      <c r="D81" s="31" t="s">
+      <c r="D81" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="E81" s="32"/>
-      <c r="F81" s="33"/>
+      <c r="E81" s="36"/>
+      <c r="F81" s="37"/>
       <c r="G81" s="23"/>
       <c r="H81" s="5"/>
     </row>
@@ -2098,11 +2120,11 @@
         <v>3</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="D82" s="34" t="s">
+      <c r="D82" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="E82" s="35"/>
-      <c r="F82" s="36"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="40"/>
       <c r="G82" s="23"/>
       <c r="H82" s="13"/>
     </row>
@@ -2111,11 +2133,11 @@
         <v>4</v>
       </c>
       <c r="C83" s="4"/>
-      <c r="D83" s="31" t="s">
+      <c r="D83" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="E83" s="32"/>
-      <c r="F83" s="33"/>
+      <c r="E83" s="36"/>
+      <c r="F83" s="37"/>
       <c r="G83" s="23"/>
       <c r="H83" s="5"/>
     </row>
@@ -2124,11 +2146,11 @@
         <v>5</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="34" t="s">
+      <c r="D84" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="E84" s="35"/>
-      <c r="F84" s="36"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="40"/>
       <c r="G84" s="23"/>
       <c r="H84" s="13"/>
     </row>
@@ -2137,11 +2159,11 @@
         <v>6</v>
       </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="31" t="s">
+      <c r="D85" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="E85" s="32"/>
-      <c r="F85" s="33"/>
+      <c r="E85" s="36"/>
+      <c r="F85" s="37"/>
       <c r="G85" s="23"/>
       <c r="H85" s="5"/>
     </row>
@@ -2150,12 +2172,12 @@
         <v>7</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="34" t="s">
+      <c r="D86" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="E86" s="35"/>
-      <c r="F86" s="36"/>
-      <c r="G86" s="43"/>
+      <c r="E86" s="39"/>
+      <c r="F86" s="40"/>
+      <c r="G86" s="23"/>
       <c r="H86" s="13"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
@@ -2163,12 +2185,12 @@
         <v>8</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="D87" s="31" t="s">
+      <c r="D87" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="E87" s="32"/>
-      <c r="F87" s="33"/>
-      <c r="G87" s="25"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="23"/>
       <c r="H87" s="5"/>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
@@ -2176,12 +2198,12 @@
         <v>9</v>
       </c>
       <c r="C88" s="16"/>
-      <c r="D88" s="39" t="s">
+      <c r="D88" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E88" s="40"/>
-      <c r="F88" s="41"/>
-      <c r="G88" s="25"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="34"/>
+      <c r="G88" s="23"/>
       <c r="H88" s="13"/>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.3">
@@ -2189,12 +2211,12 @@
         <v>10</v>
       </c>
       <c r="C89" s="4"/>
-      <c r="D89" s="31" t="s">
+      <c r="D89" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="E89" s="32"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="25"/>
+      <c r="E89" s="36"/>
+      <c r="F89" s="37"/>
+      <c r="G89" s="23"/>
       <c r="H89" s="5"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.3">
@@ -2202,12 +2224,12 @@
         <v>11</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="34" t="s">
+      <c r="D90" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="E90" s="35"/>
-      <c r="F90" s="36"/>
-      <c r="G90" s="25"/>
+      <c r="E90" s="39"/>
+      <c r="F90" s="40"/>
+      <c r="G90" s="23"/>
       <c r="H90" s="13"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.3">
@@ -2215,12 +2237,12 @@
         <v>12</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="D91" s="31" t="s">
+      <c r="D91" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="E91" s="32"/>
-      <c r="F91" s="33"/>
-      <c r="G91" s="25"/>
+      <c r="E91" s="36"/>
+      <c r="F91" s="37"/>
+      <c r="G91" s="31"/>
       <c r="H91" s="5"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.3">
@@ -2228,11 +2250,11 @@
         <v>13</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="34" t="s">
+      <c r="D92" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="E92" s="35"/>
-      <c r="F92" s="36"/>
+      <c r="E92" s="39"/>
+      <c r="F92" s="40"/>
       <c r="G92" s="25"/>
       <c r="H92" s="15"/>
     </row>
@@ -2241,11 +2263,11 @@
         <v>14</v>
       </c>
       <c r="C93" s="4"/>
-      <c r="D93" s="31" t="s">
+      <c r="D93" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="E93" s="32"/>
-      <c r="F93" s="33"/>
+      <c r="E93" s="36"/>
+      <c r="F93" s="37"/>
       <c r="G93" s="25"/>
       <c r="H93" s="5"/>
     </row>
@@ -2254,11 +2276,11 @@
         <v>15</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="34" t="s">
+      <c r="D94" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="E94" s="35"/>
-      <c r="F94" s="36"/>
+      <c r="E94" s="39"/>
+      <c r="F94" s="40"/>
       <c r="G94" s="25"/>
       <c r="H94" s="13"/>
     </row>
@@ -2267,11 +2289,11 @@
         <v>16</v>
       </c>
       <c r="C95" s="4"/>
-      <c r="D95" s="31" t="s">
+      <c r="D95" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="E95" s="32"/>
-      <c r="F95" s="33"/>
+      <c r="E95" s="36"/>
+      <c r="F95" s="37"/>
       <c r="G95" s="25"/>
       <c r="H95" s="5"/>
     </row>
@@ -2280,11 +2302,11 @@
         <v>17</v>
       </c>
       <c r="C96" s="16"/>
-      <c r="D96" s="39" t="s">
+      <c r="D96" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="E96" s="40"/>
-      <c r="F96" s="41"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="34"/>
       <c r="G96" s="30"/>
       <c r="H96" s="13"/>
     </row>
@@ -2292,10 +2314,10 @@
       <c r="B99" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C99" s="38" t="s">
+      <c r="C99" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="38"/>
+      <c r="D99" s="41"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
     </row>
@@ -2304,11 +2326,11 @@
         <v>1</v>
       </c>
       <c r="C100" s="19"/>
-      <c r="D100" s="37" t="s">
+      <c r="D100" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E100" s="37"/>
-      <c r="F100" s="37"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
       <c r="G100" s="20" t="s">
         <v>3</v>
       </c>
@@ -2321,11 +2343,11 @@
         <v>1</v>
       </c>
       <c r="C101" s="16"/>
-      <c r="D101" s="39" t="s">
+      <c r="D101" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="E101" s="40"/>
-      <c r="F101" s="41"/>
+      <c r="E101" s="33"/>
+      <c r="F101" s="34"/>
       <c r="G101" s="24"/>
       <c r="H101" s="17"/>
     </row>
@@ -2333,10 +2355,10 @@
       <c r="B104" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C104" s="38" t="s">
+      <c r="C104" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="D104" s="38"/>
+      <c r="D104" s="41"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
@@ -2345,11 +2367,11 @@
         <v>1</v>
       </c>
       <c r="C105" s="19"/>
-      <c r="D105" s="37" t="s">
+      <c r="D105" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="37"/>
-      <c r="F105" s="37"/>
+      <c r="E105" s="42"/>
+      <c r="F105" s="42"/>
       <c r="G105" s="20" t="s">
         <v>3</v>
       </c>
@@ -2362,11 +2384,11 @@
         <v>1</v>
       </c>
       <c r="C106" s="16"/>
-      <c r="D106" s="39" t="s">
+      <c r="D106" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E106" s="40"/>
-      <c r="F106" s="41"/>
+      <c r="E106" s="33"/>
+      <c r="F106" s="34"/>
       <c r="G106" s="24"/>
       <c r="H106" s="17"/>
     </row>
@@ -2374,10 +2396,10 @@
       <c r="B109" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C109" s="38" t="s">
+      <c r="C109" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="D109" s="38"/>
+      <c r="D109" s="41"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
     </row>
@@ -2386,11 +2408,11 @@
         <v>1</v>
       </c>
       <c r="C110" s="19"/>
-      <c r="D110" s="37" t="s">
+      <c r="D110" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E110" s="37"/>
-      <c r="F110" s="37"/>
+      <c r="E110" s="42"/>
+      <c r="F110" s="42"/>
       <c r="G110" s="20" t="s">
         <v>3</v>
       </c>
@@ -2403,11 +2425,11 @@
         <v>1</v>
       </c>
       <c r="C111" s="16"/>
-      <c r="D111" s="39" t="s">
+      <c r="D111" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="E111" s="40"/>
-      <c r="F111" s="41"/>
+      <c r="E111" s="33"/>
+      <c r="F111" s="34"/>
       <c r="G111" s="24"/>
       <c r="H111" s="17"/>
     </row>
@@ -2416,11 +2438,11 @@
         <v>2</v>
       </c>
       <c r="C112" s="4"/>
-      <c r="D112" s="31" t="s">
+      <c r="D112" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="E112" s="32"/>
-      <c r="F112" s="33"/>
+      <c r="E112" s="36"/>
+      <c r="F112" s="37"/>
       <c r="G112" s="25"/>
       <c r="H112" s="6"/>
     </row>
@@ -2429,11 +2451,11 @@
         <v>3</v>
       </c>
       <c r="C113" s="7"/>
-      <c r="D113" s="34" t="s">
+      <c r="D113" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="E113" s="35"/>
-      <c r="F113" s="36"/>
+      <c r="E113" s="39"/>
+      <c r="F113" s="40"/>
       <c r="G113" s="25"/>
       <c r="H113" s="14"/>
     </row>
@@ -2442,16 +2464,175 @@
         <v>4</v>
       </c>
       <c r="C114" s="4"/>
-      <c r="D114" s="31" t="s">
+      <c r="D114" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="E114" s="32"/>
-      <c r="F114" s="33"/>
+      <c r="E114" s="36"/>
+      <c r="F114" s="37"/>
       <c r="G114" s="25"/>
       <c r="H114" s="6"/>
     </row>
+    <row r="116" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B116" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C116" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="D116" s="44"/>
+    </row>
+    <row r="117" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B117" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" s="19"/>
+      <c r="D117" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="E117" s="42"/>
+      <c r="F117" s="42"/>
+      <c r="G117" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="H117" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B118" s="15">
+        <v>1</v>
+      </c>
+      <c r="C118" s="16"/>
+      <c r="D118" s="32"/>
+      <c r="E118" s="33"/>
+      <c r="F118" s="34"/>
+      <c r="G118" s="24"/>
+      <c r="H118" s="17"/>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B119" s="5">
+        <v>2</v>
+      </c>
+      <c r="C119" s="4"/>
+      <c r="D119" s="35"/>
+      <c r="E119" s="36"/>
+      <c r="F119" s="37"/>
+      <c r="G119" s="25"/>
+      <c r="H119" s="6"/>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B120" s="15">
+        <v>3</v>
+      </c>
+      <c r="C120" s="7"/>
+      <c r="D120" s="38"/>
+      <c r="E120" s="39"/>
+      <c r="F120" s="40"/>
+      <c r="G120" s="25"/>
+      <c r="H120" s="14"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B121" s="5">
+        <v>4</v>
+      </c>
+      <c r="C121" s="4"/>
+      <c r="D121" s="35"/>
+      <c r="E121" s="36"/>
+      <c r="F121" s="37"/>
+      <c r="G121" s="25"/>
+      <c r="H121" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="98">
+  <mergeCells count="105">
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="D114:F114"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="D70:F70"/>
     <mergeCell ref="D80:F80"/>
     <mergeCell ref="D81:F81"/>
@@ -2468,88 +2649,6 @@
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="D114:F114"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="D111:F111"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix color of writing
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B05C7F-2580-442B-AC40-05ACA37D4A17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECD8E02-5216-47B8-A067-18EA5CC7B85B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -733,6 +733,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -742,37 +761,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1089,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H108" sqref="H108"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H110" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,13 +1108,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
       <c r="J2" s="11" t="s">
         <v>41</v>
       </c>
@@ -1145,11 +1145,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="19"/>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="20" t="s">
         <v>3</v>
       </c>
@@ -1166,11 +1166,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="22"/>
       <c r="H6" s="17" t="s">
         <v>11</v>
@@ -1187,11 +1187,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="22"/>
       <c r="H7" s="6" t="s">
         <v>11</v>
@@ -1202,11 +1202,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="10"/>
       <c r="H8" s="14" t="s">
         <v>11</v>
@@ -1217,11 +1217,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="35"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="23"/>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -1232,11 +1232,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="22"/>
       <c r="H10" s="14" t="s">
         <v>45</v>
@@ -1247,11 +1247,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="10"/>
       <c r="H11" s="6"/>
     </row>
@@ -1260,11 +1260,11 @@
         <v>7</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="39"/>
       <c r="G12" s="23"/>
       <c r="H12" s="14"/>
     </row>
@@ -1273,11 +1273,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="35"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="23"/>
       <c r="H13" s="6"/>
     </row>
@@ -1286,11 +1286,11 @@
         <v>9</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
       <c r="G14" s="23"/>
       <c r="H14" s="14"/>
     </row>
@@ -1299,11 +1299,11 @@
         <v>10</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="35"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
       <c r="G15" s="23"/>
       <c r="H15" s="6" t="s">
         <v>11</v>
@@ -1314,11 +1314,11 @@
         <v>11</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="39"/>
       <c r="G16" s="23"/>
       <c r="H16" s="14"/>
     </row>
@@ -1327,11 +1327,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="23"/>
       <c r="H17" s="4"/>
     </row>
@@ -1340,11 +1340,11 @@
         <v>13</v>
       </c>
       <c r="C18" s="16"/>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
       <c r="G18" s="23"/>
       <c r="H18" s="16"/>
     </row>
@@ -1353,11 +1353,11 @@
         <v>14</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
       <c r="G19" s="23"/>
       <c r="H19" s="4"/>
     </row>
@@ -1366,11 +1366,11 @@
         <v>15</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="39"/>
       <c r="G20" s="23"/>
       <c r="H20" s="7"/>
     </row>
@@ -1379,11 +1379,11 @@
         <v>16</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="23"/>
       <c r="H21" s="4"/>
     </row>
@@ -1392,11 +1392,11 @@
         <v>17</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="39"/>
       <c r="G22" s="23"/>
       <c r="H22" s="7"/>
     </row>
@@ -1405,11 +1405,11 @@
         <v>18</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="35"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="23"/>
       <c r="H23" s="4"/>
     </row>
@@ -1418,11 +1418,11 @@
         <v>19</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="39"/>
       <c r="G24" s="23"/>
       <c r="H24" s="7"/>
     </row>
@@ -1431,11 +1431,11 @@
         <v>20</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="23"/>
       <c r="H25" s="4"/>
     </row>
@@ -1444,11 +1444,11 @@
         <v>21</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="23"/>
       <c r="H26" s="7"/>
     </row>
@@ -1457,11 +1457,11 @@
         <v>22</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
       <c r="G27" s="23"/>
       <c r="H27" s="4"/>
     </row>
@@ -1470,11 +1470,11 @@
         <v>23</v>
       </c>
       <c r="C28" s="16"/>
-      <c r="D28" s="38" t="s">
+      <c r="D28" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="40"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="23"/>
       <c r="H28" s="16"/>
     </row>
@@ -1483,11 +1483,11 @@
         <v>24</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="35"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
       <c r="G29" s="23"/>
       <c r="H29" s="4"/>
     </row>
@@ -1496,11 +1496,11 @@
         <v>25</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="32"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="39"/>
       <c r="G30" s="23"/>
       <c r="H30" s="7"/>
     </row>
@@ -1509,11 +1509,11 @@
         <v>26</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="35"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="23"/>
       <c r="H31" s="4" t="s">
         <v>44</v>
@@ -1524,11 +1524,11 @@
         <v>27</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="32"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="23"/>
       <c r="H32" s="29" t="s">
         <v>11</v>
@@ -1539,11 +1539,11 @@
         <v>28</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="35"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
       <c r="G33" s="23"/>
       <c r="H33" s="4"/>
     </row>
@@ -1552,11 +1552,11 @@
         <v>29</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="23"/>
       <c r="H34" s="7"/>
     </row>
@@ -1565,11 +1565,11 @@
         <v>30</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="35"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
       <c r="G35" s="23"/>
       <c r="H35" s="4"/>
     </row>
@@ -1578,11 +1578,11 @@
         <v>31</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="23"/>
       <c r="H36" s="7"/>
     </row>
@@ -1591,11 +1591,11 @@
         <v>32</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="23"/>
       <c r="H37" s="4"/>
     </row>
@@ -1604,11 +1604,11 @@
         <v>33</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="40"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="36"/>
       <c r="G38" s="23"/>
       <c r="H38" s="16"/>
     </row>
@@ -1617,11 +1617,11 @@
         <v>34</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="33" t="s">
+      <c r="D39" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="35"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
       <c r="G39" s="23"/>
       <c r="H39" s="4"/>
     </row>
@@ -1641,11 +1641,11 @@
         <v>1</v>
       </c>
       <c r="C43" s="19"/>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="E43" s="42"/>
+      <c r="F43" s="42"/>
       <c r="G43" s="20" t="s">
         <v>3</v>
       </c>
@@ -1658,11 +1658,11 @@
         <v>1</v>
       </c>
       <c r="C44" s="16"/>
-      <c r="D44" s="38" t="s">
+      <c r="D44" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="40"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="36"/>
       <c r="G44" s="23"/>
       <c r="H44" s="17"/>
     </row>
@@ -1671,11 +1671,11 @@
         <v>2</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="33" t="s">
+      <c r="D45" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="34"/>
-      <c r="F45" s="35"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
       <c r="G45" s="23"/>
       <c r="H45" s="6"/>
     </row>
@@ -1684,11 +1684,11 @@
         <v>3</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="32"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="39"/>
       <c r="G46" s="23"/>
       <c r="H46" s="14"/>
     </row>
@@ -1697,11 +1697,11 @@
         <v>4</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="34"/>
-      <c r="F47" s="35"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
       <c r="G47" s="23"/>
       <c r="H47" s="6" t="s">
         <v>90</v>
@@ -1712,11 +1712,11 @@
         <v>5</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="39"/>
       <c r="G48" s="23"/>
       <c r="H48" s="14"/>
     </row>
@@ -1725,11 +1725,11 @@
         <v>6</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="33" t="s">
+      <c r="D49" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="34"/>
-      <c r="F49" s="35"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
       <c r="G49" s="23"/>
       <c r="H49" s="6"/>
     </row>
@@ -1738,11 +1738,11 @@
         <v>7</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="32"/>
+      <c r="E50" s="38"/>
+      <c r="F50" s="39"/>
       <c r="G50" s="23"/>
       <c r="H50" s="14" t="s">
         <v>58</v>
@@ -1753,11 +1753,11 @@
         <v>8</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="30" t="s">
+      <c r="D51" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="E51" s="31"/>
-      <c r="F51" s="32"/>
+      <c r="E51" s="38"/>
+      <c r="F51" s="39"/>
       <c r="G51" s="25"/>
       <c r="H51" s="14"/>
     </row>
@@ -1777,11 +1777,11 @@
         <v>1</v>
       </c>
       <c r="C54" s="19"/>
-      <c r="D54" s="37" t="s">
+      <c r="D54" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
       <c r="G54" s="20" t="s">
         <v>3</v>
       </c>
@@ -1794,11 +1794,11 @@
         <v>1</v>
       </c>
       <c r="C55" s="16"/>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="39"/>
-      <c r="F55" s="40"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="36"/>
       <c r="G55" s="23"/>
       <c r="H55" s="15"/>
     </row>
@@ -1807,11 +1807,11 @@
         <v>2</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="33" t="s">
+      <c r="D56" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="34"/>
-      <c r="F56" s="35"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="33"/>
       <c r="G56" s="23"/>
       <c r="H56" s="5"/>
     </row>
@@ -1820,11 +1820,11 @@
         <v>3</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="31"/>
-      <c r="F57" s="32"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="39"/>
       <c r="G57" s="23"/>
       <c r="H57" s="13"/>
     </row>
@@ -1833,11 +1833,11 @@
         <v>4</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="33" t="s">
+      <c r="D58" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="34"/>
-      <c r="F58" s="35"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="33"/>
       <c r="G58" s="23"/>
       <c r="H58" s="5"/>
     </row>
@@ -1846,11 +1846,11 @@
         <v>5</v>
       </c>
       <c r="C59" s="7"/>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="31"/>
-      <c r="F59" s="32"/>
+      <c r="E59" s="38"/>
+      <c r="F59" s="39"/>
       <c r="G59" s="23"/>
       <c r="H59" s="13"/>
     </row>
@@ -1859,11 +1859,11 @@
         <v>6</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="33" t="s">
+      <c r="D60" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="34"/>
-      <c r="F60" s="35"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="33"/>
       <c r="G60" s="23"/>
       <c r="H60" s="5"/>
     </row>
@@ -1872,11 +1872,11 @@
         <v>7</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="30" t="s">
+      <c r="D61" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="31"/>
-      <c r="F61" s="32"/>
+      <c r="E61" s="38"/>
+      <c r="F61" s="39"/>
       <c r="G61" s="23"/>
       <c r="H61" s="13"/>
     </row>
@@ -1885,11 +1885,11 @@
         <v>8</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="33" t="s">
+      <c r="D62" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="34"/>
-      <c r="F62" s="35"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="33"/>
       <c r="G62" s="23"/>
       <c r="H62" s="5"/>
     </row>
@@ -1898,11 +1898,11 @@
         <v>9</v>
       </c>
       <c r="C63" s="7"/>
-      <c r="D63" s="30" t="s">
+      <c r="D63" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="31"/>
-      <c r="F63" s="32"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="39"/>
       <c r="G63" s="23"/>
       <c r="H63" s="13"/>
     </row>
@@ -1911,11 +1911,11 @@
         <v>10</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="33" t="s">
+      <c r="D64" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="34"/>
-      <c r="F64" s="35"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="33"/>
       <c r="G64" s="23"/>
       <c r="H64" s="5"/>
     </row>
@@ -1926,11 +1926,11 @@
       <c r="C65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="30" t="s">
+      <c r="D65" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="31"/>
-      <c r="F65" s="32"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="39"/>
       <c r="G65" s="25"/>
       <c r="H65" s="28" t="s">
         <v>91</v>
@@ -1952,11 +1952,11 @@
         <v>1</v>
       </c>
       <c r="C69" s="19"/>
-      <c r="D69" s="37" t="s">
+      <c r="D69" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
+      <c r="E69" s="42"/>
+      <c r="F69" s="42"/>
       <c r="G69" s="20" t="s">
         <v>3</v>
       </c>
@@ -1969,11 +1969,11 @@
         <v>1</v>
       </c>
       <c r="C70" s="16"/>
-      <c r="D70" s="38" t="s">
+      <c r="D70" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="E70" s="39"/>
-      <c r="F70" s="40"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="36"/>
       <c r="G70" s="23"/>
       <c r="H70" s="15"/>
     </row>
@@ -1982,11 +1982,11 @@
         <v>2</v>
       </c>
       <c r="C71" s="4"/>
-      <c r="D71" s="33" t="s">
+      <c r="D71" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="34"/>
-      <c r="F71" s="35"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="33"/>
       <c r="G71" s="23"/>
       <c r="H71" s="5"/>
     </row>
@@ -1995,11 +1995,11 @@
         <v>3</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="D72" s="30" t="s">
+      <c r="D72" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E72" s="31"/>
-      <c r="F72" s="32"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="39"/>
       <c r="G72" s="23"/>
       <c r="H72" s="13"/>
     </row>
@@ -2008,11 +2008,11 @@
         <v>4</v>
       </c>
       <c r="C73" s="4"/>
-      <c r="D73" s="33" t="s">
+      <c r="D73" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="E73" s="34"/>
-      <c r="F73" s="35"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="33"/>
       <c r="G73" s="23"/>
       <c r="H73" s="5"/>
     </row>
@@ -2021,11 +2021,11 @@
         <v>5</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="D74" s="30" t="s">
+      <c r="D74" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="E74" s="31"/>
-      <c r="F74" s="32"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="39"/>
       <c r="G74" s="23"/>
       <c r="H74" s="13"/>
     </row>
@@ -2034,11 +2034,11 @@
         <v>6</v>
       </c>
       <c r="C75" s="4"/>
-      <c r="D75" s="33" t="s">
+      <c r="D75" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="E75" s="34"/>
-      <c r="F75" s="35"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="33"/>
       <c r="G75" s="23"/>
       <c r="H75" s="5"/>
     </row>
@@ -2058,11 +2058,11 @@
         <v>1</v>
       </c>
       <c r="C79" s="19"/>
-      <c r="D79" s="37" t="s">
+      <c r="D79" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
+      <c r="E79" s="42"/>
+      <c r="F79" s="42"/>
       <c r="G79" s="20" t="s">
         <v>3</v>
       </c>
@@ -2075,11 +2075,11 @@
         <v>1</v>
       </c>
       <c r="C80" s="16"/>
-      <c r="D80" s="38" t="s">
+      <c r="D80" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="E80" s="39"/>
-      <c r="F80" s="40"/>
+      <c r="E80" s="35"/>
+      <c r="F80" s="36"/>
       <c r="G80" s="23"/>
       <c r="H80" s="15"/>
     </row>
@@ -2088,11 +2088,11 @@
         <v>2</v>
       </c>
       <c r="C81" s="4"/>
-      <c r="D81" s="33" t="s">
+      <c r="D81" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E81" s="34"/>
-      <c r="F81" s="35"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="33"/>
       <c r="G81" s="23"/>
       <c r="H81" s="5"/>
     </row>
@@ -2101,11 +2101,11 @@
         <v>3</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="D82" s="30" t="s">
+      <c r="D82" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="E82" s="31"/>
-      <c r="F82" s="32"/>
+      <c r="E82" s="38"/>
+      <c r="F82" s="39"/>
       <c r="G82" s="23"/>
       <c r="H82" s="13"/>
     </row>
@@ -2114,11 +2114,11 @@
         <v>4</v>
       </c>
       <c r="C83" s="4"/>
-      <c r="D83" s="33" t="s">
+      <c r="D83" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="E83" s="34"/>
-      <c r="F83" s="35"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="33"/>
       <c r="G83" s="23"/>
       <c r="H83" s="5"/>
     </row>
@@ -2127,11 +2127,11 @@
         <v>5</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="30" t="s">
+      <c r="D84" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="E84" s="31"/>
-      <c r="F84" s="32"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="39"/>
       <c r="G84" s="23"/>
       <c r="H84" s="13"/>
     </row>
@@ -2140,11 +2140,11 @@
         <v>6</v>
       </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="33" t="s">
+      <c r="D85" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="E85" s="34"/>
-      <c r="F85" s="35"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="33"/>
       <c r="G85" s="23"/>
       <c r="H85" s="5"/>
     </row>
@@ -2153,11 +2153,11 @@
         <v>7</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="30" t="s">
+      <c r="D86" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="E86" s="31"/>
-      <c r="F86" s="32"/>
+      <c r="E86" s="38"/>
+      <c r="F86" s="39"/>
       <c r="G86" s="23"/>
       <c r="H86" s="13"/>
     </row>
@@ -2166,11 +2166,11 @@
         <v>8</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="D87" s="33" t="s">
+      <c r="D87" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E87" s="34"/>
-      <c r="F87" s="35"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="33"/>
       <c r="G87" s="23"/>
       <c r="H87" s="5"/>
     </row>
@@ -2179,11 +2179,11 @@
         <v>9</v>
       </c>
       <c r="C88" s="16"/>
-      <c r="D88" s="38" t="s">
+      <c r="D88" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E88" s="39"/>
-      <c r="F88" s="40"/>
+      <c r="E88" s="35"/>
+      <c r="F88" s="36"/>
       <c r="G88" s="23"/>
       <c r="H88" s="13"/>
     </row>
@@ -2192,11 +2192,11 @@
         <v>10</v>
       </c>
       <c r="C89" s="4"/>
-      <c r="D89" s="33" t="s">
+      <c r="D89" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E89" s="34"/>
-      <c r="F89" s="35"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="33"/>
       <c r="G89" s="23"/>
       <c r="H89" s="5"/>
     </row>
@@ -2205,11 +2205,11 @@
         <v>11</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="30" t="s">
+      <c r="D90" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="E90" s="31"/>
-      <c r="F90" s="32"/>
+      <c r="E90" s="38"/>
+      <c r="F90" s="39"/>
       <c r="G90" s="23"/>
       <c r="H90" s="13"/>
     </row>
@@ -2218,11 +2218,11 @@
         <v>12</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="D91" s="33" t="s">
+      <c r="D91" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E91" s="34"/>
-      <c r="F91" s="35"/>
+      <c r="E91" s="32"/>
+      <c r="F91" s="33"/>
       <c r="G91" s="23"/>
       <c r="H91" s="5"/>
     </row>
@@ -2231,11 +2231,11 @@
         <v>13</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="30" t="s">
+      <c r="D92" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="E92" s="31"/>
-      <c r="F92" s="32"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="39"/>
       <c r="G92" s="23"/>
       <c r="H92" s="15"/>
     </row>
@@ -2244,11 +2244,11 @@
         <v>14</v>
       </c>
       <c r="C93" s="4"/>
-      <c r="D93" s="33" t="s">
+      <c r="D93" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E93" s="34"/>
-      <c r="F93" s="35"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="33"/>
       <c r="G93" s="23"/>
       <c r="H93" s="5"/>
     </row>
@@ -2257,11 +2257,11 @@
         <v>15</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="30" t="s">
+      <c r="D94" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="E94" s="31"/>
-      <c r="F94" s="32"/>
+      <c r="E94" s="38"/>
+      <c r="F94" s="39"/>
       <c r="G94" s="23"/>
       <c r="H94" s="13"/>
     </row>
@@ -2270,11 +2270,11 @@
         <v>16</v>
       </c>
       <c r="C95" s="4"/>
-      <c r="D95" s="33" t="s">
+      <c r="D95" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E95" s="34"/>
-      <c r="F95" s="35"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="33"/>
       <c r="G95" s="23"/>
       <c r="H95" s="5"/>
     </row>
@@ -2283,11 +2283,11 @@
         <v>17</v>
       </c>
       <c r="C96" s="16"/>
-      <c r="D96" s="38" t="s">
+      <c r="D96" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="E96" s="39"/>
-      <c r="F96" s="40"/>
+      <c r="E96" s="35"/>
+      <c r="F96" s="36"/>
       <c r="G96" s="23"/>
       <c r="H96" s="13"/>
     </row>
@@ -2307,11 +2307,11 @@
         <v>1</v>
       </c>
       <c r="C100" s="19"/>
-      <c r="D100" s="37" t="s">
+      <c r="D100" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E100" s="37"/>
-      <c r="F100" s="37"/>
+      <c r="E100" s="42"/>
+      <c r="F100" s="42"/>
       <c r="G100" s="20" t="s">
         <v>3</v>
       </c>
@@ -2324,11 +2324,11 @@
         <v>1</v>
       </c>
       <c r="C101" s="16"/>
-      <c r="D101" s="38" t="s">
+      <c r="D101" s="34" t="s">
         <v>82</v>
       </c>
-      <c r="E101" s="39"/>
-      <c r="F101" s="40"/>
+      <c r="E101" s="35"/>
+      <c r="F101" s="36"/>
       <c r="G101" s="23"/>
       <c r="H101" s="17"/>
     </row>
@@ -2337,11 +2337,11 @@
         <v>2</v>
       </c>
       <c r="C102" s="16"/>
-      <c r="D102" s="38" t="s">
+      <c r="D102" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="E102" s="39"/>
-      <c r="F102" s="40"/>
+      <c r="E102" s="35"/>
+      <c r="F102" s="36"/>
       <c r="G102" s="23"/>
       <c r="H102" s="17"/>
     </row>
@@ -2361,11 +2361,11 @@
         <v>1</v>
       </c>
       <c r="C105" s="19"/>
-      <c r="D105" s="37" t="s">
+      <c r="D105" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="37"/>
-      <c r="F105" s="37"/>
+      <c r="E105" s="42"/>
+      <c r="F105" s="42"/>
       <c r="G105" s="20" t="s">
         <v>3</v>
       </c>
@@ -2378,12 +2378,12 @@
         <v>1</v>
       </c>
       <c r="C106" s="16"/>
-      <c r="D106" s="38" t="s">
+      <c r="D106" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="E106" s="39"/>
-      <c r="F106" s="40"/>
-      <c r="G106" s="43"/>
+      <c r="E106" s="35"/>
+      <c r="F106" s="36"/>
+      <c r="G106" s="23"/>
       <c r="H106" s="17"/>
     </row>
     <row r="109" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -2402,11 +2402,11 @@
         <v>1</v>
       </c>
       <c r="C110" s="19"/>
-      <c r="D110" s="37" t="s">
+      <c r="D110" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E110" s="37"/>
-      <c r="F110" s="37"/>
+      <c r="E110" s="42"/>
+      <c r="F110" s="42"/>
       <c r="G110" s="20" t="s">
         <v>3</v>
       </c>
@@ -2419,12 +2419,12 @@
         <v>1</v>
       </c>
       <c r="C111" s="16"/>
-      <c r="D111" s="38" t="s">
+      <c r="D111" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="E111" s="39"/>
-      <c r="F111" s="40"/>
-      <c r="G111" s="24"/>
+      <c r="E111" s="35"/>
+      <c r="F111" s="36"/>
+      <c r="G111" s="30"/>
       <c r="H111" s="17"/>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.3">
@@ -2432,11 +2432,11 @@
         <v>2</v>
       </c>
       <c r="C112" s="4"/>
-      <c r="D112" s="33" t="s">
+      <c r="D112" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="E112" s="34"/>
-      <c r="F112" s="35"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="33"/>
       <c r="G112" s="25"/>
       <c r="H112" s="6"/>
     </row>
@@ -2445,11 +2445,11 @@
         <v>3</v>
       </c>
       <c r="C113" s="7"/>
-      <c r="D113" s="30" t="s">
+      <c r="D113" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="E113" s="31"/>
-      <c r="F113" s="32"/>
+      <c r="E113" s="38"/>
+      <c r="F113" s="39"/>
       <c r="G113" s="25"/>
       <c r="H113" s="14"/>
     </row>
@@ -2458,11 +2458,11 @@
         <v>4</v>
       </c>
       <c r="C114" s="4"/>
-      <c r="D114" s="33" t="s">
+      <c r="D114" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E114" s="34"/>
-      <c r="F114" s="35"/>
+      <c r="E114" s="32"/>
+      <c r="F114" s="33"/>
       <c r="G114" s="25"/>
       <c r="H114" s="6"/>
     </row>
@@ -2470,21 +2470,21 @@
       <c r="B116" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C116" s="36" t="s">
+      <c r="C116" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="D116" s="36"/>
+      <c r="D116" s="43"/>
     </row>
     <row r="117" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C117" s="19"/>
-      <c r="D117" s="37" t="s">
+      <c r="D117" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E117" s="37"/>
-      <c r="F117" s="37"/>
+      <c r="E117" s="42"/>
+      <c r="F117" s="42"/>
       <c r="G117" s="20" t="s">
         <v>3</v>
       </c>
@@ -2497,9 +2497,9 @@
         <v>1</v>
       </c>
       <c r="C118" s="16"/>
-      <c r="D118" s="38"/>
-      <c r="E118" s="39"/>
-      <c r="F118" s="40"/>
+      <c r="D118" s="34"/>
+      <c r="E118" s="35"/>
+      <c r="F118" s="36"/>
       <c r="G118" s="24"/>
       <c r="H118" s="17"/>
     </row>
@@ -2508,9 +2508,9 @@
         <v>2</v>
       </c>
       <c r="C119" s="4"/>
-      <c r="D119" s="33"/>
-      <c r="E119" s="34"/>
-      <c r="F119" s="35"/>
+      <c r="D119" s="31"/>
+      <c r="E119" s="32"/>
+      <c r="F119" s="33"/>
       <c r="G119" s="25"/>
       <c r="H119" s="6"/>
     </row>
@@ -2519,9 +2519,9 @@
         <v>3</v>
       </c>
       <c r="C120" s="7"/>
-      <c r="D120" s="30"/>
-      <c r="E120" s="31"/>
-      <c r="F120" s="32"/>
+      <c r="D120" s="37"/>
+      <c r="E120" s="38"/>
+      <c r="F120" s="39"/>
       <c r="G120" s="25"/>
       <c r="H120" s="14"/>
     </row>
@@ -2530,32 +2530,63 @@
         <v>4</v>
       </c>
       <c r="C121" s="4"/>
-      <c r="D121" s="33"/>
-      <c r="E121" s="34"/>
-      <c r="F121" s="35"/>
+      <c r="D121" s="31"/>
+      <c r="E121" s="32"/>
+      <c r="F121" s="33"/>
       <c r="G121" s="25"/>
       <c r="H121" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D102:F102"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="D114:F114"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D82:F82"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D31:F31"/>
     <mergeCell ref="D32:F32"/>
@@ -2580,6 +2611,24 @@
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D102:F102"/>
     <mergeCell ref="C42:D42"/>
     <mergeCell ref="D43:F43"/>
     <mergeCell ref="D44:F44"/>
@@ -2595,55 +2644,6 @@
     <mergeCell ref="D69:F69"/>
     <mergeCell ref="D62:F62"/>
     <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="D121:F121"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="D119:F119"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="D114:F114"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D90:F90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished last diagram, start now with missed
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CECD8E02-5216-47B8-A067-18EA5CC7B85B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0B85BB-D4AB-430F-84A0-BE138F548C0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="111">
   <si>
     <t xml:space="preserve">Liste der zu zeichnenden Zeigerdiagramme </t>
   </si>
@@ -410,7 +410,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,6 +447,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -733,7 +739,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -743,6 +757,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -752,27 +772,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1089,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1108,13 +1114,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
       <c r="J2" s="11" t="s">
         <v>41</v>
       </c>
@@ -1145,11 +1151,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="19"/>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="20" t="s">
         <v>3</v>
       </c>
@@ -1166,11 +1172,11 @@
         <v>1</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40"/>
       <c r="G6" s="22"/>
       <c r="H6" s="17" t="s">
         <v>11</v>
@@ -1187,11 +1193,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="22"/>
       <c r="H7" s="6" t="s">
         <v>11</v>
@@ -1202,11 +1208,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="38"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="10"/>
       <c r="H8" s="14" t="s">
         <v>11</v>
@@ -1217,11 +1223,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="33"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="23"/>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -1232,11 +1238,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="22"/>
       <c r="H10" s="14" t="s">
         <v>45</v>
@@ -1247,11 +1253,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="35"/>
       <c r="G11" s="10"/>
       <c r="H11" s="6"/>
     </row>
@@ -1260,11 +1266,11 @@
         <v>7</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="39"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="32"/>
       <c r="G12" s="23"/>
       <c r="H12" s="14"/>
     </row>
@@ -1273,11 +1279,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="33"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="35"/>
       <c r="G13" s="23"/>
       <c r="H13" s="6"/>
     </row>
@@ -1286,11 +1292,11 @@
         <v>9</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="38"/>
-      <c r="F14" s="39"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="32"/>
       <c r="G14" s="23"/>
       <c r="H14" s="14"/>
     </row>
@@ -1299,11 +1305,11 @@
         <v>10</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="33"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="35"/>
       <c r="G15" s="23"/>
       <c r="H15" s="6" t="s">
         <v>11</v>
@@ -1314,11 +1320,11 @@
         <v>11</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="38"/>
-      <c r="F16" s="39"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
       <c r="G16" s="23"/>
       <c r="H16" s="14"/>
     </row>
@@ -1327,11 +1333,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="33"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35"/>
       <c r="G17" s="23"/>
       <c r="H17" s="4"/>
     </row>
@@ -1340,11 +1346,11 @@
         <v>13</v>
       </c>
       <c r="C18" s="16"/>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="36"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="40"/>
       <c r="G18" s="23"/>
       <c r="H18" s="16"/>
     </row>
@@ -1353,11 +1359,11 @@
         <v>14</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="31" t="s">
+      <c r="D19" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="33"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="35"/>
       <c r="G19" s="23"/>
       <c r="H19" s="4"/>
     </row>
@@ -1366,11 +1372,11 @@
         <v>15</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="39"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="23"/>
       <c r="H20" s="7"/>
     </row>
@@ -1379,11 +1385,11 @@
         <v>16</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="35"/>
       <c r="G21" s="23"/>
       <c r="H21" s="4"/>
     </row>
@@ -1392,11 +1398,11 @@
         <v>17</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="38"/>
-      <c r="F22" s="39"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
       <c r="G22" s="23"/>
       <c r="H22" s="7"/>
     </row>
@@ -1405,11 +1411,11 @@
         <v>18</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="23"/>
       <c r="H23" s="4"/>
     </row>
@@ -1418,11 +1424,11 @@
         <v>19</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="38"/>
-      <c r="F24" s="39"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
       <c r="G24" s="23"/>
       <c r="H24" s="7"/>
     </row>
@@ -1431,11 +1437,11 @@
         <v>20</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="31" t="s">
+      <c r="D25" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="35"/>
       <c r="G25" s="23"/>
       <c r="H25" s="4"/>
     </row>
@@ -1444,11 +1450,11 @@
         <v>21</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
       <c r="G26" s="23"/>
       <c r="H26" s="7"/>
     </row>
@@ -1457,11 +1463,11 @@
         <v>22</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="31" t="s">
+      <c r="D27" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="35"/>
       <c r="G27" s="23"/>
       <c r="H27" s="4"/>
     </row>
@@ -1470,11 +1476,11 @@
         <v>23</v>
       </c>
       <c r="C28" s="16"/>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="35"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="40"/>
       <c r="G28" s="23"/>
       <c r="H28" s="16"/>
     </row>
@@ -1483,11 +1489,11 @@
         <v>24</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="31" t="s">
+      <c r="D29" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="35"/>
       <c r="G29" s="23"/>
       <c r="H29" s="4"/>
     </row>
@@ -1496,11 +1502,11 @@
         <v>25</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="38"/>
-      <c r="F30" s="39"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
       <c r="G30" s="23"/>
       <c r="H30" s="7"/>
     </row>
@@ -1509,11 +1515,11 @@
         <v>26</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="23"/>
       <c r="H31" s="4" t="s">
         <v>44</v>
@@ -1524,11 +1530,11 @@
         <v>27</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="39"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="23"/>
       <c r="H32" s="29" t="s">
         <v>11</v>
@@ -1539,11 +1545,11 @@
         <v>28</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="35"/>
       <c r="G33" s="23"/>
       <c r="H33" s="4"/>
     </row>
@@ -1552,11 +1558,11 @@
         <v>29</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="37" t="s">
+      <c r="D34" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="38"/>
-      <c r="F34" s="39"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="23"/>
       <c r="H34" s="7"/>
     </row>
@@ -1565,11 +1571,11 @@
         <v>30</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="31" t="s">
+      <c r="D35" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="35"/>
       <c r="G35" s="23"/>
       <c r="H35" s="4"/>
     </row>
@@ -1578,11 +1584,11 @@
         <v>31</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="37" t="s">
+      <c r="D36" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="38"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="23"/>
       <c r="H36" s="7"/>
     </row>
@@ -1591,11 +1597,11 @@
         <v>32</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="31" t="s">
+      <c r="D37" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="35"/>
       <c r="G37" s="23"/>
       <c r="H37" s="4"/>
     </row>
@@ -1604,11 +1610,11 @@
         <v>33</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="36"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="40"/>
       <c r="G38" s="23"/>
       <c r="H38" s="16"/>
     </row>
@@ -1617,11 +1623,11 @@
         <v>34</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="35"/>
       <c r="G39" s="23"/>
       <c r="H39" s="4"/>
     </row>
@@ -1641,11 +1647,11 @@
         <v>1</v>
       </c>
       <c r="C43" s="19"/>
-      <c r="D43" s="42" t="s">
+      <c r="D43" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="42"/>
-      <c r="F43" s="42"/>
+      <c r="E43" s="37"/>
+      <c r="F43" s="37"/>
       <c r="G43" s="20" t="s">
         <v>3</v>
       </c>
@@ -1658,11 +1664,11 @@
         <v>1</v>
       </c>
       <c r="C44" s="16"/>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="35"/>
-      <c r="F44" s="36"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="40"/>
       <c r="G44" s="23"/>
       <c r="H44" s="17"/>
     </row>
@@ -1671,11 +1677,11 @@
         <v>2</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="32"/>
-      <c r="F45" s="33"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="35"/>
       <c r="G45" s="23"/>
       <c r="H45" s="6"/>
     </row>
@@ -1684,11 +1690,11 @@
         <v>3</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="37" t="s">
+      <c r="D46" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="38"/>
-      <c r="F46" s="39"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="32"/>
       <c r="G46" s="23"/>
       <c r="H46" s="14"/>
     </row>
@@ -1697,11 +1703,11 @@
         <v>4</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="33"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="35"/>
       <c r="G47" s="23"/>
       <c r="H47" s="6" t="s">
         <v>90</v>
@@ -1712,11 +1718,11 @@
         <v>5</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="38"/>
-      <c r="F48" s="39"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="32"/>
       <c r="G48" s="23"/>
       <c r="H48" s="14"/>
     </row>
@@ -1725,11 +1731,11 @@
         <v>6</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="32"/>
-      <c r="F49" s="33"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="35"/>
       <c r="G49" s="23"/>
       <c r="H49" s="6"/>
     </row>
@@ -1738,11 +1744,11 @@
         <v>7</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="37" t="s">
+      <c r="D50" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="38"/>
-      <c r="F50" s="39"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="32"/>
       <c r="G50" s="23"/>
       <c r="H50" s="14" t="s">
         <v>58</v>
@@ -1753,12 +1759,12 @@
         <v>8</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="37" t="s">
+      <c r="D51" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="E51" s="38"/>
-      <c r="F51" s="39"/>
-      <c r="G51" s="25"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="43"/>
       <c r="H51" s="14"/>
     </row>
     <row r="53" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1777,11 +1783,11 @@
         <v>1</v>
       </c>
       <c r="C54" s="19"/>
-      <c r="D54" s="42" t="s">
+      <c r="D54" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
       <c r="G54" s="20" t="s">
         <v>3</v>
       </c>
@@ -1794,11 +1800,11 @@
         <v>1</v>
       </c>
       <c r="C55" s="16"/>
-      <c r="D55" s="34" t="s">
+      <c r="D55" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="35"/>
-      <c r="F55" s="36"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="40"/>
       <c r="G55" s="23"/>
       <c r="H55" s="15"/>
     </row>
@@ -1807,11 +1813,11 @@
         <v>2</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="31" t="s">
+      <c r="D56" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="32"/>
-      <c r="F56" s="33"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="35"/>
       <c r="G56" s="23"/>
       <c r="H56" s="5"/>
     </row>
@@ -1820,11 +1826,11 @@
         <v>3</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="D57" s="37" t="s">
+      <c r="D57" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="38"/>
-      <c r="F57" s="39"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="32"/>
       <c r="G57" s="23"/>
       <c r="H57" s="13"/>
     </row>
@@ -1833,11 +1839,11 @@
         <v>4</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="31" t="s">
+      <c r="D58" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="32"/>
-      <c r="F58" s="33"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="35"/>
       <c r="G58" s="23"/>
       <c r="H58" s="5"/>
     </row>
@@ -1846,11 +1852,11 @@
         <v>5</v>
       </c>
       <c r="C59" s="7"/>
-      <c r="D59" s="37" t="s">
+      <c r="D59" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="38"/>
-      <c r="F59" s="39"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="32"/>
       <c r="G59" s="23"/>
       <c r="H59" s="13"/>
     </row>
@@ -1859,11 +1865,11 @@
         <v>6</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="31" t="s">
+      <c r="D60" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="32"/>
-      <c r="F60" s="33"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="35"/>
       <c r="G60" s="23"/>
       <c r="H60" s="5"/>
     </row>
@@ -1872,11 +1878,11 @@
         <v>7</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="37" t="s">
+      <c r="D61" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="38"/>
-      <c r="F61" s="39"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="32"/>
       <c r="G61" s="23"/>
       <c r="H61" s="13"/>
     </row>
@@ -1885,11 +1891,11 @@
         <v>8</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="31" t="s">
+      <c r="D62" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="32"/>
-      <c r="F62" s="33"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="35"/>
       <c r="G62" s="23"/>
       <c r="H62" s="5"/>
     </row>
@@ -1898,11 +1904,11 @@
         <v>9</v>
       </c>
       <c r="C63" s="7"/>
-      <c r="D63" s="37" t="s">
+      <c r="D63" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="38"/>
-      <c r="F63" s="39"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="32"/>
       <c r="G63" s="23"/>
       <c r="H63" s="13"/>
     </row>
@@ -1911,11 +1917,11 @@
         <v>10</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="31" t="s">
+      <c r="D64" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="32"/>
-      <c r="F64" s="33"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="35"/>
       <c r="G64" s="23"/>
       <c r="H64" s="5"/>
     </row>
@@ -1926,11 +1932,11 @@
       <c r="C65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="37" t="s">
+      <c r="D65" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="38"/>
-      <c r="F65" s="39"/>
+      <c r="E65" s="31"/>
+      <c r="F65" s="32"/>
       <c r="G65" s="25"/>
       <c r="H65" s="28" t="s">
         <v>91</v>
@@ -1952,11 +1958,11 @@
         <v>1</v>
       </c>
       <c r="C69" s="19"/>
-      <c r="D69" s="42" t="s">
+      <c r="D69" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="42"/>
-      <c r="F69" s="42"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
       <c r="G69" s="20" t="s">
         <v>3</v>
       </c>
@@ -1969,11 +1975,11 @@
         <v>1</v>
       </c>
       <c r="C70" s="16"/>
-      <c r="D70" s="34" t="s">
+      <c r="D70" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="E70" s="35"/>
-      <c r="F70" s="36"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="40"/>
       <c r="G70" s="23"/>
       <c r="H70" s="15"/>
     </row>
@@ -1982,11 +1988,11 @@
         <v>2</v>
       </c>
       <c r="C71" s="4"/>
-      <c r="D71" s="31" t="s">
+      <c r="D71" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="32"/>
-      <c r="F71" s="33"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="35"/>
       <c r="G71" s="23"/>
       <c r="H71" s="5"/>
     </row>
@@ -1995,11 +2001,11 @@
         <v>3</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="D72" s="37" t="s">
+      <c r="D72" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="E72" s="38"/>
-      <c r="F72" s="39"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="32"/>
       <c r="G72" s="23"/>
       <c r="H72" s="13"/>
     </row>
@@ -2008,11 +2014,11 @@
         <v>4</v>
       </c>
       <c r="C73" s="4"/>
-      <c r="D73" s="31" t="s">
+      <c r="D73" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="E73" s="32"/>
-      <c r="F73" s="33"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="35"/>
       <c r="G73" s="23"/>
       <c r="H73" s="5"/>
     </row>
@@ -2021,11 +2027,11 @@
         <v>5</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="D74" s="37" t="s">
+      <c r="D74" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="E74" s="38"/>
-      <c r="F74" s="39"/>
+      <c r="E74" s="31"/>
+      <c r="F74" s="32"/>
       <c r="G74" s="23"/>
       <c r="H74" s="13"/>
     </row>
@@ -2034,11 +2040,11 @@
         <v>6</v>
       </c>
       <c r="C75" s="4"/>
-      <c r="D75" s="31" t="s">
+      <c r="D75" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="E75" s="32"/>
-      <c r="F75" s="33"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="35"/>
       <c r="G75" s="23"/>
       <c r="H75" s="5"/>
     </row>
@@ -2058,11 +2064,11 @@
         <v>1</v>
       </c>
       <c r="C79" s="19"/>
-      <c r="D79" s="42" t="s">
+      <c r="D79" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="42"/>
-      <c r="F79" s="42"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="37"/>
       <c r="G79" s="20" t="s">
         <v>3</v>
       </c>
@@ -2075,11 +2081,11 @@
         <v>1</v>
       </c>
       <c r="C80" s="16"/>
-      <c r="D80" s="34" t="s">
+      <c r="D80" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="E80" s="35"/>
-      <c r="F80" s="36"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="40"/>
       <c r="G80" s="23"/>
       <c r="H80" s="15"/>
     </row>
@@ -2088,11 +2094,11 @@
         <v>2</v>
       </c>
       <c r="C81" s="4"/>
-      <c r="D81" s="31" t="s">
+      <c r="D81" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="E81" s="32"/>
-      <c r="F81" s="33"/>
+      <c r="E81" s="34"/>
+      <c r="F81" s="35"/>
       <c r="G81" s="23"/>
       <c r="H81" s="5"/>
     </row>
@@ -2101,11 +2107,11 @@
         <v>3</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="D82" s="37" t="s">
+      <c r="D82" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="E82" s="38"/>
-      <c r="F82" s="39"/>
+      <c r="E82" s="31"/>
+      <c r="F82" s="32"/>
       <c r="G82" s="23"/>
       <c r="H82" s="13"/>
     </row>
@@ -2114,11 +2120,11 @@
         <v>4</v>
       </c>
       <c r="C83" s="4"/>
-      <c r="D83" s="31" t="s">
+      <c r="D83" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="E83" s="32"/>
-      <c r="F83" s="33"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="35"/>
       <c r="G83" s="23"/>
       <c r="H83" s="5"/>
     </row>
@@ -2127,11 +2133,11 @@
         <v>5</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="37" t="s">
+      <c r="D84" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="E84" s="38"/>
-      <c r="F84" s="39"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="32"/>
       <c r="G84" s="23"/>
       <c r="H84" s="13"/>
     </row>
@@ -2140,11 +2146,11 @@
         <v>6</v>
       </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="31" t="s">
+      <c r="D85" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="E85" s="32"/>
-      <c r="F85" s="33"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="35"/>
       <c r="G85" s="23"/>
       <c r="H85" s="5"/>
     </row>
@@ -2153,11 +2159,11 @@
         <v>7</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="37" t="s">
+      <c r="D86" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E86" s="38"/>
-      <c r="F86" s="39"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="32"/>
       <c r="G86" s="23"/>
       <c r="H86" s="13"/>
     </row>
@@ -2166,11 +2172,11 @@
         <v>8</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="D87" s="31" t="s">
+      <c r="D87" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="E87" s="32"/>
-      <c r="F87" s="33"/>
+      <c r="E87" s="34"/>
+      <c r="F87" s="35"/>
       <c r="G87" s="23"/>
       <c r="H87" s="5"/>
     </row>
@@ -2179,11 +2185,11 @@
         <v>9</v>
       </c>
       <c r="C88" s="16"/>
-      <c r="D88" s="34" t="s">
+      <c r="D88" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="E88" s="35"/>
-      <c r="F88" s="36"/>
+      <c r="E88" s="39"/>
+      <c r="F88" s="40"/>
       <c r="G88" s="23"/>
       <c r="H88" s="13"/>
     </row>
@@ -2192,11 +2198,11 @@
         <v>10</v>
       </c>
       <c r="C89" s="4"/>
-      <c r="D89" s="31" t="s">
+      <c r="D89" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="E89" s="32"/>
-      <c r="F89" s="33"/>
+      <c r="E89" s="34"/>
+      <c r="F89" s="35"/>
       <c r="G89" s="23"/>
       <c r="H89" s="5"/>
     </row>
@@ -2205,11 +2211,11 @@
         <v>11</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="37" t="s">
+      <c r="D90" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="E90" s="38"/>
-      <c r="F90" s="39"/>
+      <c r="E90" s="31"/>
+      <c r="F90" s="32"/>
       <c r="G90" s="23"/>
       <c r="H90" s="13"/>
     </row>
@@ -2218,11 +2224,11 @@
         <v>12</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="D91" s="31" t="s">
+      <c r="D91" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="E91" s="32"/>
-      <c r="F91" s="33"/>
+      <c r="E91" s="34"/>
+      <c r="F91" s="35"/>
       <c r="G91" s="23"/>
       <c r="H91" s="5"/>
     </row>
@@ -2231,11 +2237,11 @@
         <v>13</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="37" t="s">
+      <c r="D92" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="E92" s="38"/>
-      <c r="F92" s="39"/>
+      <c r="E92" s="31"/>
+      <c r="F92" s="32"/>
       <c r="G92" s="23"/>
       <c r="H92" s="15"/>
     </row>
@@ -2244,11 +2250,11 @@
         <v>14</v>
       </c>
       <c r="C93" s="4"/>
-      <c r="D93" s="31" t="s">
+      <c r="D93" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="E93" s="32"/>
-      <c r="F93" s="33"/>
+      <c r="E93" s="34"/>
+      <c r="F93" s="35"/>
       <c r="G93" s="23"/>
       <c r="H93" s="5"/>
     </row>
@@ -2257,11 +2263,11 @@
         <v>15</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="37" t="s">
+      <c r="D94" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="E94" s="38"/>
-      <c r="F94" s="39"/>
+      <c r="E94" s="31"/>
+      <c r="F94" s="32"/>
       <c r="G94" s="23"/>
       <c r="H94" s="13"/>
     </row>
@@ -2270,11 +2276,11 @@
         <v>16</v>
       </c>
       <c r="C95" s="4"/>
-      <c r="D95" s="31" t="s">
+      <c r="D95" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="E95" s="32"/>
-      <c r="F95" s="33"/>
+      <c r="E95" s="34"/>
+      <c r="F95" s="35"/>
       <c r="G95" s="23"/>
       <c r="H95" s="5"/>
     </row>
@@ -2283,11 +2289,11 @@
         <v>17</v>
       </c>
       <c r="C96" s="16"/>
-      <c r="D96" s="34" t="s">
+      <c r="D96" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="E96" s="35"/>
-      <c r="F96" s="36"/>
+      <c r="E96" s="39"/>
+      <c r="F96" s="40"/>
       <c r="G96" s="23"/>
       <c r="H96" s="13"/>
     </row>
@@ -2307,11 +2313,11 @@
         <v>1</v>
       </c>
       <c r="C100" s="19"/>
-      <c r="D100" s="42" t="s">
+      <c r="D100" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E100" s="42"/>
-      <c r="F100" s="42"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="37"/>
       <c r="G100" s="20" t="s">
         <v>3</v>
       </c>
@@ -2324,11 +2330,11 @@
         <v>1</v>
       </c>
       <c r="C101" s="16"/>
-      <c r="D101" s="34" t="s">
+      <c r="D101" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="E101" s="35"/>
-      <c r="F101" s="36"/>
+      <c r="E101" s="39"/>
+      <c r="F101" s="40"/>
       <c r="G101" s="23"/>
       <c r="H101" s="17"/>
     </row>
@@ -2337,11 +2343,11 @@
         <v>2</v>
       </c>
       <c r="C102" s="16"/>
-      <c r="D102" s="34" t="s">
+      <c r="D102" s="38" t="s">
         <v>110</v>
       </c>
-      <c r="E102" s="35"/>
-      <c r="F102" s="36"/>
+      <c r="E102" s="39"/>
+      <c r="F102" s="40"/>
       <c r="G102" s="23"/>
       <c r="H102" s="17"/>
     </row>
@@ -2361,11 +2367,11 @@
         <v>1</v>
       </c>
       <c r="C105" s="19"/>
-      <c r="D105" s="42" t="s">
+      <c r="D105" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="42"/>
-      <c r="F105" s="42"/>
+      <c r="E105" s="37"/>
+      <c r="F105" s="37"/>
       <c r="G105" s="20" t="s">
         <v>3</v>
       </c>
@@ -2378,11 +2384,11 @@
         <v>1</v>
       </c>
       <c r="C106" s="16"/>
-      <c r="D106" s="34" t="s">
+      <c r="D106" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="E106" s="35"/>
-      <c r="F106" s="36"/>
+      <c r="E106" s="39"/>
+      <c r="F106" s="40"/>
       <c r="G106" s="23"/>
       <c r="H106" s="17"/>
     </row>
@@ -2402,11 +2408,11 @@
         <v>1</v>
       </c>
       <c r="C110" s="19"/>
-      <c r="D110" s="42" t="s">
+      <c r="D110" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E110" s="42"/>
-      <c r="F110" s="42"/>
+      <c r="E110" s="37"/>
+      <c r="F110" s="37"/>
       <c r="G110" s="20" t="s">
         <v>3</v>
       </c>
@@ -2419,12 +2425,12 @@
         <v>1</v>
       </c>
       <c r="C111" s="16"/>
-      <c r="D111" s="34" t="s">
+      <c r="D111" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="E111" s="35"/>
-      <c r="F111" s="36"/>
-      <c r="G111" s="30"/>
+      <c r="E111" s="39"/>
+      <c r="F111" s="40"/>
+      <c r="G111" s="23"/>
       <c r="H111" s="17"/>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.3">
@@ -2432,12 +2438,12 @@
         <v>2</v>
       </c>
       <c r="C112" s="4"/>
-      <c r="D112" s="31" t="s">
+      <c r="D112" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="E112" s="32"/>
-      <c r="F112" s="33"/>
-      <c r="G112" s="25"/>
+      <c r="E112" s="34"/>
+      <c r="F112" s="35"/>
+      <c r="G112" s="23"/>
       <c r="H112" s="6"/>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.3">
@@ -2445,12 +2451,12 @@
         <v>3</v>
       </c>
       <c r="C113" s="7"/>
-      <c r="D113" s="37" t="s">
+      <c r="D113" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="E113" s="38"/>
-      <c r="F113" s="39"/>
-      <c r="G113" s="25"/>
+      <c r="E113" s="31"/>
+      <c r="F113" s="32"/>
+      <c r="G113" s="23"/>
       <c r="H113" s="14"/>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.3">
@@ -2458,33 +2464,33 @@
         <v>4</v>
       </c>
       <c r="C114" s="4"/>
-      <c r="D114" s="31" t="s">
+      <c r="D114" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="E114" s="32"/>
-      <c r="F114" s="33"/>
-      <c r="G114" s="25"/>
+      <c r="E114" s="34"/>
+      <c r="F114" s="35"/>
+      <c r="G114" s="23"/>
       <c r="H114" s="6"/>
     </row>
     <row r="116" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C116" s="43" t="s">
+      <c r="C116" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="D116" s="43"/>
+      <c r="D116" s="36"/>
     </row>
     <row r="117" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C117" s="19"/>
-      <c r="D117" s="42" t="s">
+      <c r="D117" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E117" s="42"/>
-      <c r="F117" s="42"/>
+      <c r="E117" s="37"/>
+      <c r="F117" s="37"/>
       <c r="G117" s="20" t="s">
         <v>3</v>
       </c>
@@ -2497,9 +2503,9 @@
         <v>1</v>
       </c>
       <c r="C118" s="16"/>
-      <c r="D118" s="34"/>
-      <c r="E118" s="35"/>
-      <c r="F118" s="36"/>
+      <c r="D118" s="38"/>
+      <c r="E118" s="39"/>
+      <c r="F118" s="40"/>
       <c r="G118" s="24"/>
       <c r="H118" s="17"/>
     </row>
@@ -2508,9 +2514,9 @@
         <v>2</v>
       </c>
       <c r="C119" s="4"/>
-      <c r="D119" s="31"/>
-      <c r="E119" s="32"/>
-      <c r="F119" s="33"/>
+      <c r="D119" s="33"/>
+      <c r="E119" s="34"/>
+      <c r="F119" s="35"/>
       <c r="G119" s="25"/>
       <c r="H119" s="6"/>
     </row>
@@ -2519,9 +2525,9 @@
         <v>3</v>
       </c>
       <c r="C120" s="7"/>
-      <c r="D120" s="37"/>
-      <c r="E120" s="38"/>
-      <c r="F120" s="39"/>
+      <c r="D120" s="30"/>
+      <c r="E120" s="31"/>
+      <c r="F120" s="32"/>
       <c r="G120" s="25"/>
       <c r="H120" s="14"/>
     </row>
@@ -2530,14 +2536,96 @@
         <v>4</v>
       </c>
       <c r="C121" s="4"/>
-      <c r="D121" s="31"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="33"/>
+      <c r="D121" s="33"/>
+      <c r="E121" s="34"/>
+      <c r="F121" s="35"/>
       <c r="G121" s="25"/>
       <c r="H121" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="106">
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D102:F102"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
     <mergeCell ref="D120:F120"/>
     <mergeCell ref="D121:F121"/>
     <mergeCell ref="D51:F51"/>
@@ -2562,88 +2650,6 @@
     <mergeCell ref="D88:F88"/>
     <mergeCell ref="D89:F89"/>
     <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D102:F102"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D57:F57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add label to clicker, make spacing bigger
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0B85BB-D4AB-430F-84A0-BE138F548C0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4114DAA2-FAFD-4702-B0A7-2E17F26C7437}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="114">
   <si>
     <t xml:space="preserve">Liste der zu zeichnenden Zeigerdiagramme </t>
   </si>
@@ -364,6 +364,15 @@
   </si>
   <si>
     <t xml:space="preserve">Parasitäre Effekte bei Spulen I b) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeigerdiagramm Strom Spannung </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zeigerdiagramm einfach </t>
+  </si>
+  <si>
+    <t xml:space="preserve">RLC Serienschwingkreis Zeiger a b c </t>
   </si>
 </sst>
 </file>
@@ -410,7 +419,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,14 +456,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -659,26 +662,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -725,7 +713,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -739,6 +726,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -748,37 +753,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1095,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118:F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1114,13 +1100,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
       <c r="J2" s="11" t="s">
         <v>41</v>
       </c>
@@ -1135,10 +1121,10 @@
       <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="9"/>
@@ -1151,11 +1137,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="19"/>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="20" t="s">
         <v>3</v>
       </c>
@@ -1172,16 +1158,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="22"/>
       <c r="H6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="25" t="s">
         <v>7</v>
       </c>
       <c r="K6" t="s">
@@ -1193,11 +1179,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
       <c r="G7" s="22"/>
       <c r="H7" s="6" t="s">
         <v>11</v>
@@ -1208,11 +1194,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="10"/>
       <c r="H8" s="14" t="s">
         <v>11</v>
@@ -1223,11 +1209,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="33" t="s">
+      <c r="D9" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="35"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="31"/>
       <c r="G9" s="23"/>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -1238,11 +1224,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="22"/>
       <c r="H10" s="14" t="s">
         <v>45</v>
@@ -1253,11 +1239,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="35"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="10"/>
       <c r="H11" s="6"/>
     </row>
@@ -1266,11 +1252,11 @@
         <v>7</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="23"/>
       <c r="H12" s="14"/>
     </row>
@@ -1279,11 +1265,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="35"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
       <c r="G13" s="23"/>
       <c r="H13" s="6"/>
     </row>
@@ -1292,11 +1278,11 @@
         <v>9</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
       <c r="G14" s="23"/>
       <c r="H14" s="14"/>
     </row>
@@ -1305,11 +1291,11 @@
         <v>10</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="34"/>
-      <c r="F15" s="35"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="31"/>
       <c r="G15" s="23"/>
       <c r="H15" s="6" t="s">
         <v>11</v>
@@ -1320,11 +1306,11 @@
         <v>11</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
       <c r="G16" s="23"/>
       <c r="H16" s="14"/>
     </row>
@@ -1333,11 +1319,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="35"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
       <c r="G17" s="23"/>
       <c r="H17" s="4"/>
     </row>
@@ -1346,11 +1332,11 @@
         <v>13</v>
       </c>
       <c r="C18" s="16"/>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="40"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="23"/>
       <c r="H18" s="16"/>
     </row>
@@ -1359,11 +1345,11 @@
         <v>14</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="31"/>
       <c r="G19" s="23"/>
       <c r="H19" s="4"/>
     </row>
@@ -1372,11 +1358,11 @@
         <v>15</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="23"/>
       <c r="H20" s="7"/>
     </row>
@@ -1385,11 +1371,11 @@
         <v>16</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="34"/>
-      <c r="F21" s="35"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="23"/>
       <c r="H21" s="4"/>
     </row>
@@ -1398,11 +1384,11 @@
         <v>17</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
       <c r="G22" s="23"/>
       <c r="H22" s="7"/>
     </row>
@@ -1411,11 +1397,11 @@
         <v>18</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="34"/>
-      <c r="F23" s="35"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="23"/>
       <c r="H23" s="4"/>
     </row>
@@ -1424,11 +1410,11 @@
         <v>19</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
       <c r="G24" s="23"/>
       <c r="H24" s="7"/>
     </row>
@@ -1437,11 +1423,11 @@
         <v>20</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="34"/>
-      <c r="F25" s="35"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="23"/>
       <c r="H25" s="4"/>
     </row>
@@ -1450,11 +1436,11 @@
         <v>21</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="32"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="37"/>
       <c r="G26" s="23"/>
       <c r="H26" s="7"/>
     </row>
@@ -1463,11 +1449,11 @@
         <v>22</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="34"/>
-      <c r="F27" s="35"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="31"/>
       <c r="G27" s="23"/>
       <c r="H27" s="4"/>
     </row>
@@ -1476,11 +1462,11 @@
         <v>23</v>
       </c>
       <c r="C28" s="16"/>
-      <c r="D28" s="38" t="s">
+      <c r="D28" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="40"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="23"/>
       <c r="H28" s="16"/>
     </row>
@@ -1489,11 +1475,11 @@
         <v>24</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="33" t="s">
+      <c r="D29" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="35"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
       <c r="G29" s="23"/>
       <c r="H29" s="4"/>
     </row>
@@ -1502,11 +1488,11 @@
         <v>25</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="32"/>
+      <c r="E30" s="36"/>
+      <c r="F30" s="37"/>
       <c r="G30" s="23"/>
       <c r="H30" s="7"/>
     </row>
@@ -1515,11 +1501,11 @@
         <v>26</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="33" t="s">
+      <c r="D31" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="34"/>
-      <c r="F31" s="35"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="31"/>
       <c r="G31" s="23"/>
       <c r="H31" s="4" t="s">
         <v>44</v>
@@ -1530,13 +1516,13 @@
         <v>27</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="32"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="37"/>
       <c r="G32" s="23"/>
-      <c r="H32" s="29" t="s">
+      <c r="H32" s="28" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1545,11 +1531,11 @@
         <v>28</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="35"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="23"/>
       <c r="H33" s="4"/>
     </row>
@@ -1558,11 +1544,11 @@
         <v>29</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="37"/>
       <c r="G34" s="23"/>
       <c r="H34" s="7"/>
     </row>
@@ -1571,11 +1557,11 @@
         <v>30</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="33" t="s">
+      <c r="D35" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="35"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="23"/>
       <c r="H35" s="4"/>
     </row>
@@ -1584,11 +1570,11 @@
         <v>31</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="37"/>
       <c r="G36" s="23"/>
       <c r="H36" s="7"/>
     </row>
@@ -1597,24 +1583,24 @@
         <v>32</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="33" t="s">
+      <c r="D37" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="35"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="23"/>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="27">
+      <c r="B38" s="26">
         <v>33</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="39"/>
-      <c r="F38" s="40"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="23"/>
       <c r="H38" s="16"/>
     </row>
@@ -1623,11 +1609,11 @@
         <v>34</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="33" t="s">
+      <c r="D39" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="34"/>
-      <c r="F39" s="35"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="31"/>
       <c r="G39" s="23"/>
       <c r="H39" s="4"/>
     </row>
@@ -1635,10 +1621,10 @@
       <c r="B42" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="41"/>
+      <c r="D42" s="38"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
@@ -1647,11 +1633,11 @@
         <v>1</v>
       </c>
       <c r="C43" s="19"/>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="37"/>
-      <c r="F43" s="37"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
       <c r="G43" s="20" t="s">
         <v>3</v>
       </c>
@@ -1664,11 +1650,11 @@
         <v>1</v>
       </c>
       <c r="C44" s="16"/>
-      <c r="D44" s="38" t="s">
+      <c r="D44" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="39"/>
-      <c r="F44" s="40"/>
+      <c r="E44" s="33"/>
+      <c r="F44" s="34"/>
       <c r="G44" s="23"/>
       <c r="H44" s="17"/>
     </row>
@@ -1677,11 +1663,11 @@
         <v>2</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="33" t="s">
+      <c r="D45" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="34"/>
-      <c r="F45" s="35"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="31"/>
       <c r="G45" s="23"/>
       <c r="H45" s="6"/>
     </row>
@@ -1690,11 +1676,11 @@
         <v>3</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="32"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="37"/>
       <c r="G46" s="23"/>
       <c r="H46" s="14"/>
     </row>
@@ -1703,11 +1689,11 @@
         <v>4</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="33" t="s">
+      <c r="D47" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="34"/>
-      <c r="F47" s="35"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="31"/>
       <c r="G47" s="23"/>
       <c r="H47" s="6" t="s">
         <v>90</v>
@@ -1718,11 +1704,11 @@
         <v>5</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="37"/>
       <c r="G48" s="23"/>
       <c r="H48" s="14"/>
     </row>
@@ -1731,11 +1717,11 @@
         <v>6</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="33" t="s">
+      <c r="D49" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="34"/>
-      <c r="F49" s="35"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="31"/>
       <c r="G49" s="23"/>
       <c r="H49" s="6"/>
     </row>
@@ -1744,11 +1730,11 @@
         <v>7</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="32"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="37"/>
       <c r="G50" s="23"/>
       <c r="H50" s="14" t="s">
         <v>58</v>
@@ -1759,22 +1745,22 @@
         <v>8</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="30" t="s">
+      <c r="D51" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E51" s="31"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="43"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="23"/>
       <c r="H51" s="14"/>
     </row>
     <row r="53" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B53" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="41"/>
+      <c r="D53" s="38"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
@@ -1783,11 +1769,11 @@
         <v>1</v>
       </c>
       <c r="C54" s="19"/>
-      <c r="D54" s="37" t="s">
+      <c r="D54" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
       <c r="G54" s="20" t="s">
         <v>3</v>
       </c>
@@ -1800,11 +1786,11 @@
         <v>1</v>
       </c>
       <c r="C55" s="16"/>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="39"/>
-      <c r="F55" s="40"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="34"/>
       <c r="G55" s="23"/>
       <c r="H55" s="15"/>
     </row>
@@ -1813,11 +1799,11 @@
         <v>2</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="33" t="s">
+      <c r="D56" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="34"/>
-      <c r="F56" s="35"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="31"/>
       <c r="G56" s="23"/>
       <c r="H56" s="5"/>
     </row>
@@ -1826,11 +1812,11 @@
         <v>3</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="31"/>
-      <c r="F57" s="32"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="37"/>
       <c r="G57" s="23"/>
       <c r="H57" s="13"/>
     </row>
@@ -1839,11 +1825,11 @@
         <v>4</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="33" t="s">
+      <c r="D58" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="34"/>
-      <c r="F58" s="35"/>
+      <c r="E58" s="30"/>
+      <c r="F58" s="31"/>
       <c r="G58" s="23"/>
       <c r="H58" s="5"/>
     </row>
@@ -1852,11 +1838,11 @@
         <v>5</v>
       </c>
       <c r="C59" s="7"/>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="31"/>
-      <c r="F59" s="32"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="37"/>
       <c r="G59" s="23"/>
       <c r="H59" s="13"/>
     </row>
@@ -1865,11 +1851,11 @@
         <v>6</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="33" t="s">
+      <c r="D60" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="34"/>
-      <c r="F60" s="35"/>
+      <c r="E60" s="30"/>
+      <c r="F60" s="31"/>
       <c r="G60" s="23"/>
       <c r="H60" s="5"/>
     </row>
@@ -1878,11 +1864,11 @@
         <v>7</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="30" t="s">
+      <c r="D61" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="31"/>
-      <c r="F61" s="32"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="37"/>
       <c r="G61" s="23"/>
       <c r="H61" s="13"/>
     </row>
@@ -1891,11 +1877,11 @@
         <v>8</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="33" t="s">
+      <c r="D62" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="34"/>
-      <c r="F62" s="35"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="31"/>
       <c r="G62" s="23"/>
       <c r="H62" s="5"/>
     </row>
@@ -1904,11 +1890,11 @@
         <v>9</v>
       </c>
       <c r="C63" s="7"/>
-      <c r="D63" s="30" t="s">
+      <c r="D63" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="31"/>
-      <c r="F63" s="32"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="37"/>
       <c r="G63" s="23"/>
       <c r="H63" s="13"/>
     </row>
@@ -1917,11 +1903,11 @@
         <v>10</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="33" t="s">
+      <c r="D64" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="34"/>
-      <c r="F64" s="35"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="31"/>
       <c r="G64" s="23"/>
       <c r="H64" s="5"/>
     </row>
@@ -1932,13 +1918,13 @@
       <c r="C65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="30" t="s">
+      <c r="D65" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="31"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="25"/>
-      <c r="H65" s="28" t="s">
+      <c r="E65" s="36"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="24"/>
+      <c r="H65" s="27" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1946,10 +1932,10 @@
       <c r="B68" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="41" t="s">
+      <c r="C68" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="41"/>
+      <c r="D68" s="38"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
@@ -1958,11 +1944,11 @@
         <v>1</v>
       </c>
       <c r="C69" s="19"/>
-      <c r="D69" s="37" t="s">
+      <c r="D69" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="37"/>
-      <c r="F69" s="37"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
       <c r="G69" s="20" t="s">
         <v>3</v>
       </c>
@@ -1975,11 +1961,11 @@
         <v>1</v>
       </c>
       <c r="C70" s="16"/>
-      <c r="D70" s="38" t="s">
+      <c r="D70" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="E70" s="39"/>
-      <c r="F70" s="40"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="34"/>
       <c r="G70" s="23"/>
       <c r="H70" s="15"/>
     </row>
@@ -1988,11 +1974,11 @@
         <v>2</v>
       </c>
       <c r="C71" s="4"/>
-      <c r="D71" s="33" t="s">
+      <c r="D71" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="34"/>
-      <c r="F71" s="35"/>
+      <c r="E71" s="30"/>
+      <c r="F71" s="31"/>
       <c r="G71" s="23"/>
       <c r="H71" s="5"/>
     </row>
@@ -2001,11 +1987,11 @@
         <v>3</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="D72" s="30" t="s">
+      <c r="D72" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="E72" s="31"/>
-      <c r="F72" s="32"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="37"/>
       <c r="G72" s="23"/>
       <c r="H72" s="13"/>
     </row>
@@ -2014,11 +2000,11 @@
         <v>4</v>
       </c>
       <c r="C73" s="4"/>
-      <c r="D73" s="33" t="s">
+      <c r="D73" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="E73" s="34"/>
-      <c r="F73" s="35"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="31"/>
       <c r="G73" s="23"/>
       <c r="H73" s="5"/>
     </row>
@@ -2027,11 +2013,11 @@
         <v>5</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="D74" s="30" t="s">
+      <c r="D74" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="E74" s="31"/>
-      <c r="F74" s="32"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="37"/>
       <c r="G74" s="23"/>
       <c r="H74" s="13"/>
     </row>
@@ -2040,11 +2026,11 @@
         <v>6</v>
       </c>
       <c r="C75" s="4"/>
-      <c r="D75" s="33" t="s">
+      <c r="D75" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="E75" s="34"/>
-      <c r="F75" s="35"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="31"/>
       <c r="G75" s="23"/>
       <c r="H75" s="5"/>
     </row>
@@ -2052,10 +2038,10 @@
       <c r="B78" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="41" t="s">
+      <c r="C78" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="D78" s="41"/>
+      <c r="D78" s="38"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
@@ -2064,11 +2050,11 @@
         <v>1</v>
       </c>
       <c r="C79" s="19"/>
-      <c r="D79" s="37" t="s">
+      <c r="D79" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="37"/>
-      <c r="F79" s="37"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39"/>
       <c r="G79" s="20" t="s">
         <v>3</v>
       </c>
@@ -2081,11 +2067,11 @@
         <v>1</v>
       </c>
       <c r="C80" s="16"/>
-      <c r="D80" s="38" t="s">
+      <c r="D80" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="E80" s="39"/>
-      <c r="F80" s="40"/>
+      <c r="E80" s="33"/>
+      <c r="F80" s="34"/>
       <c r="G80" s="23"/>
       <c r="H80" s="15"/>
     </row>
@@ -2094,11 +2080,11 @@
         <v>2</v>
       </c>
       <c r="C81" s="4"/>
-      <c r="D81" s="33" t="s">
+      <c r="D81" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="E81" s="34"/>
-      <c r="F81" s="35"/>
+      <c r="E81" s="30"/>
+      <c r="F81" s="31"/>
       <c r="G81" s="23"/>
       <c r="H81" s="5"/>
     </row>
@@ -2107,11 +2093,11 @@
         <v>3</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="D82" s="30" t="s">
+      <c r="D82" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="E82" s="31"/>
-      <c r="F82" s="32"/>
+      <c r="E82" s="36"/>
+      <c r="F82" s="37"/>
       <c r="G82" s="23"/>
       <c r="H82" s="13"/>
     </row>
@@ -2120,11 +2106,11 @@
         <v>4</v>
       </c>
       <c r="C83" s="4"/>
-      <c r="D83" s="33" t="s">
+      <c r="D83" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="E83" s="34"/>
-      <c r="F83" s="35"/>
+      <c r="E83" s="30"/>
+      <c r="F83" s="31"/>
       <c r="G83" s="23"/>
       <c r="H83" s="5"/>
     </row>
@@ -2133,11 +2119,11 @@
         <v>5</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="30" t="s">
+      <c r="D84" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="E84" s="31"/>
-      <c r="F84" s="32"/>
+      <c r="E84" s="36"/>
+      <c r="F84" s="37"/>
       <c r="G84" s="23"/>
       <c r="H84" s="13"/>
     </row>
@@ -2146,11 +2132,11 @@
         <v>6</v>
       </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="33" t="s">
+      <c r="D85" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E85" s="34"/>
-      <c r="F85" s="35"/>
+      <c r="E85" s="30"/>
+      <c r="F85" s="31"/>
       <c r="G85" s="23"/>
       <c r="H85" s="5"/>
     </row>
@@ -2159,11 +2145,11 @@
         <v>7</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="30" t="s">
+      <c r="D86" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="E86" s="31"/>
-      <c r="F86" s="32"/>
+      <c r="E86" s="36"/>
+      <c r="F86" s="37"/>
       <c r="G86" s="23"/>
       <c r="H86" s="13"/>
     </row>
@@ -2172,11 +2158,11 @@
         <v>8</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="D87" s="33" t="s">
+      <c r="D87" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="E87" s="34"/>
-      <c r="F87" s="35"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="31"/>
       <c r="G87" s="23"/>
       <c r="H87" s="5"/>
     </row>
@@ -2185,11 +2171,11 @@
         <v>9</v>
       </c>
       <c r="C88" s="16"/>
-      <c r="D88" s="38" t="s">
+      <c r="D88" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E88" s="39"/>
-      <c r="F88" s="40"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="34"/>
       <c r="G88" s="23"/>
       <c r="H88" s="13"/>
     </row>
@@ -2198,11 +2184,11 @@
         <v>10</v>
       </c>
       <c r="C89" s="4"/>
-      <c r="D89" s="33" t="s">
+      <c r="D89" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="E89" s="34"/>
-      <c r="F89" s="35"/>
+      <c r="E89" s="30"/>
+      <c r="F89" s="31"/>
       <c r="G89" s="23"/>
       <c r="H89" s="5"/>
     </row>
@@ -2211,11 +2197,11 @@
         <v>11</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="30" t="s">
+      <c r="D90" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="E90" s="31"/>
-      <c r="F90" s="32"/>
+      <c r="E90" s="36"/>
+      <c r="F90" s="37"/>
       <c r="G90" s="23"/>
       <c r="H90" s="13"/>
     </row>
@@ -2224,11 +2210,11 @@
         <v>12</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="D91" s="33" t="s">
+      <c r="D91" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="E91" s="34"/>
-      <c r="F91" s="35"/>
+      <c r="E91" s="30"/>
+      <c r="F91" s="31"/>
       <c r="G91" s="23"/>
       <c r="H91" s="5"/>
     </row>
@@ -2237,11 +2223,11 @@
         <v>13</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="30" t="s">
+      <c r="D92" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="E92" s="31"/>
-      <c r="F92" s="32"/>
+      <c r="E92" s="36"/>
+      <c r="F92" s="37"/>
       <c r="G92" s="23"/>
       <c r="H92" s="15"/>
     </row>
@@ -2250,11 +2236,11 @@
         <v>14</v>
       </c>
       <c r="C93" s="4"/>
-      <c r="D93" s="33" t="s">
+      <c r="D93" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="E93" s="34"/>
-      <c r="F93" s="35"/>
+      <c r="E93" s="30"/>
+      <c r="F93" s="31"/>
       <c r="G93" s="23"/>
       <c r="H93" s="5"/>
     </row>
@@ -2263,11 +2249,11 @@
         <v>15</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="30" t="s">
+      <c r="D94" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="E94" s="31"/>
-      <c r="F94" s="32"/>
+      <c r="E94" s="36"/>
+      <c r="F94" s="37"/>
       <c r="G94" s="23"/>
       <c r="H94" s="13"/>
     </row>
@@ -2276,11 +2262,11 @@
         <v>16</v>
       </c>
       <c r="C95" s="4"/>
-      <c r="D95" s="33" t="s">
+      <c r="D95" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="E95" s="34"/>
-      <c r="F95" s="35"/>
+      <c r="E95" s="30"/>
+      <c r="F95" s="31"/>
       <c r="G95" s="23"/>
       <c r="H95" s="5"/>
     </row>
@@ -2289,11 +2275,11 @@
         <v>17</v>
       </c>
       <c r="C96" s="16"/>
-      <c r="D96" s="38" t="s">
+      <c r="D96" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="E96" s="39"/>
-      <c r="F96" s="40"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="34"/>
       <c r="G96" s="23"/>
       <c r="H96" s="13"/>
     </row>
@@ -2301,10 +2287,10 @@
       <c r="B99" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C99" s="41" t="s">
+      <c r="C99" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="41"/>
+      <c r="D99" s="38"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
     </row>
@@ -2313,11 +2299,11 @@
         <v>1</v>
       </c>
       <c r="C100" s="19"/>
-      <c r="D100" s="37" t="s">
+      <c r="D100" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E100" s="37"/>
-      <c r="F100" s="37"/>
+      <c r="E100" s="39"/>
+      <c r="F100" s="39"/>
       <c r="G100" s="20" t="s">
         <v>3</v>
       </c>
@@ -2330,11 +2316,11 @@
         <v>1</v>
       </c>
       <c r="C101" s="16"/>
-      <c r="D101" s="38" t="s">
+      <c r="D101" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="E101" s="39"/>
-      <c r="F101" s="40"/>
+      <c r="E101" s="33"/>
+      <c r="F101" s="34"/>
       <c r="G101" s="23"/>
       <c r="H101" s="17"/>
     </row>
@@ -2343,11 +2329,11 @@
         <v>2</v>
       </c>
       <c r="C102" s="16"/>
-      <c r="D102" s="38" t="s">
+      <c r="D102" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="E102" s="39"/>
-      <c r="F102" s="40"/>
+      <c r="E102" s="33"/>
+      <c r="F102" s="34"/>
       <c r="G102" s="23"/>
       <c r="H102" s="17"/>
     </row>
@@ -2355,10 +2341,10 @@
       <c r="B104" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C104" s="41" t="s">
+      <c r="C104" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="D104" s="41"/>
+      <c r="D104" s="38"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
@@ -2367,11 +2353,11 @@
         <v>1</v>
       </c>
       <c r="C105" s="19"/>
-      <c r="D105" s="37" t="s">
+      <c r="D105" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="37"/>
-      <c r="F105" s="37"/>
+      <c r="E105" s="39"/>
+      <c r="F105" s="39"/>
       <c r="G105" s="20" t="s">
         <v>3</v>
       </c>
@@ -2384,11 +2370,11 @@
         <v>1</v>
       </c>
       <c r="C106" s="16"/>
-      <c r="D106" s="38" t="s">
+      <c r="D106" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E106" s="39"/>
-      <c r="F106" s="40"/>
+      <c r="E106" s="33"/>
+      <c r="F106" s="34"/>
       <c r="G106" s="23"/>
       <c r="H106" s="17"/>
     </row>
@@ -2396,10 +2382,10 @@
       <c r="B109" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C109" s="41" t="s">
+      <c r="C109" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="D109" s="41"/>
+      <c r="D109" s="38"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
     </row>
@@ -2408,11 +2394,11 @@
         <v>1</v>
       </c>
       <c r="C110" s="19"/>
-      <c r="D110" s="37" t="s">
+      <c r="D110" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E110" s="37"/>
-      <c r="F110" s="37"/>
+      <c r="E110" s="39"/>
+      <c r="F110" s="39"/>
       <c r="G110" s="20" t="s">
         <v>3</v>
       </c>
@@ -2425,11 +2411,11 @@
         <v>1</v>
       </c>
       <c r="C111" s="16"/>
-      <c r="D111" s="38" t="s">
+      <c r="D111" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="E111" s="39"/>
-      <c r="F111" s="40"/>
+      <c r="E111" s="33"/>
+      <c r="F111" s="34"/>
       <c r="G111" s="23"/>
       <c r="H111" s="17"/>
     </row>
@@ -2438,11 +2424,11 @@
         <v>2</v>
       </c>
       <c r="C112" s="4"/>
-      <c r="D112" s="33" t="s">
+      <c r="D112" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="E112" s="34"/>
-      <c r="F112" s="35"/>
+      <c r="E112" s="30"/>
+      <c r="F112" s="31"/>
       <c r="G112" s="23"/>
       <c r="H112" s="6"/>
     </row>
@@ -2451,11 +2437,11 @@
         <v>3</v>
       </c>
       <c r="C113" s="7"/>
-      <c r="D113" s="30" t="s">
+      <c r="D113" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="E113" s="31"/>
-      <c r="F113" s="32"/>
+      <c r="E113" s="36"/>
+      <c r="F113" s="37"/>
       <c r="G113" s="23"/>
       <c r="H113" s="14"/>
     </row>
@@ -2464,11 +2450,11 @@
         <v>4</v>
       </c>
       <c r="C114" s="4"/>
-      <c r="D114" s="33" t="s">
+      <c r="D114" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="E114" s="34"/>
-      <c r="F114" s="35"/>
+      <c r="E114" s="30"/>
+      <c r="F114" s="31"/>
       <c r="G114" s="23"/>
       <c r="H114" s="6"/>
     </row>
@@ -2476,21 +2462,21 @@
       <c r="B116" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C116" s="36" t="s">
+      <c r="C116" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="D116" s="36"/>
+      <c r="D116" s="41"/>
     </row>
     <row r="117" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C117" s="19"/>
-      <c r="D117" s="37" t="s">
+      <c r="D117" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E117" s="37"/>
-      <c r="F117" s="37"/>
+      <c r="E117" s="39"/>
+      <c r="F117" s="39"/>
       <c r="G117" s="20" t="s">
         <v>3</v>
       </c>
@@ -2503,10 +2489,12 @@
         <v>1</v>
       </c>
       <c r="C118" s="16"/>
-      <c r="D118" s="38"/>
-      <c r="E118" s="39"/>
-      <c r="F118" s="40"/>
-      <c r="G118" s="24"/>
+      <c r="D118" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="E118" s="33"/>
+      <c r="F118" s="34"/>
+      <c r="G118" s="9"/>
       <c r="H118" s="17"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.3">
@@ -2514,10 +2502,12 @@
         <v>2</v>
       </c>
       <c r="C119" s="4"/>
-      <c r="D119" s="33"/>
-      <c r="E119" s="34"/>
-      <c r="F119" s="35"/>
-      <c r="G119" s="25"/>
+      <c r="D119" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="E119" s="30"/>
+      <c r="F119" s="31"/>
+      <c r="G119" s="24"/>
       <c r="H119" s="6"/>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.3">
@@ -2525,10 +2515,12 @@
         <v>3</v>
       </c>
       <c r="C120" s="7"/>
-      <c r="D120" s="30"/>
-      <c r="E120" s="31"/>
-      <c r="F120" s="32"/>
-      <c r="G120" s="25"/>
+      <c r="D120" s="35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E120" s="36"/>
+      <c r="F120" s="37"/>
+      <c r="G120" s="24"/>
       <c r="H120" s="14"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.3">
@@ -2536,14 +2528,96 @@
         <v>4</v>
       </c>
       <c r="C121" s="4"/>
-      <c r="D121" s="33"/>
-      <c r="E121" s="34"/>
-      <c r="F121" s="35"/>
-      <c r="G121" s="25"/>
+      <c r="D121" s="29"/>
+      <c r="E121" s="30"/>
+      <c r="F121" s="31"/>
+      <c r="G121" s="24"/>
       <c r="H121" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="106">
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="D51:F51"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="D112:F112"/>
+    <mergeCell ref="D113:F113"/>
+    <mergeCell ref="D114:F114"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="D111:F111"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="D100:F100"/>
+    <mergeCell ref="D101:F101"/>
+    <mergeCell ref="D88:F88"/>
+    <mergeCell ref="D89:F89"/>
+    <mergeCell ref="D90:F90"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D38:F38"/>
     <mergeCell ref="D39:F39"/>
@@ -2568,88 +2642,6 @@
     <mergeCell ref="D69:F69"/>
     <mergeCell ref="D62:F62"/>
     <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="D121:F121"/>
-    <mergeCell ref="D51:F51"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="D119:F119"/>
-    <mergeCell ref="D112:F112"/>
-    <mergeCell ref="D113:F113"/>
-    <mergeCell ref="D114:F114"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="D111:F111"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="D100:F100"/>
-    <mergeCell ref="D101:F101"/>
-    <mergeCell ref="D88:F88"/>
-    <mergeCell ref="D89:F89"/>
-    <mergeCell ref="D90:F90"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished Clicker; started Ossanna
</commit_message>
<xml_diff>
--- a/Liste_Zeigerdiagramme.xlsx
+++ b/Liste_Zeigerdiagramme.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Marco\Git\Zeigerdiagramme_NusII\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4114DAA2-FAFD-4702-B0A7-2E17F26C7437}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE8D375-B5CF-489C-8884-9F756F707C3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{E43A5F62-9FE2-4985-9B9F-B24F7056F595}"/>
   </bookViews>
@@ -366,13 +366,13 @@
     <t xml:space="preserve">Parasitäre Effekte bei Spulen I b) </t>
   </si>
   <si>
-    <t xml:space="preserve">Zeigerdiagramm Strom Spannung </t>
-  </si>
-  <si>
     <t xml:space="preserve">Zeigerdiagramm einfach </t>
   </si>
   <si>
     <t xml:space="preserve">RLC Serienschwingkreis Zeiger a b c </t>
+  </si>
+  <si>
+    <t>Zeigerdiagramm L/C</t>
   </si>
 </sst>
 </file>
@@ -666,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -713,7 +713,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -726,6 +725,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -735,6 +743,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -744,27 +758,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1081,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D35F59-E36D-4CC4-97A3-9F1D0EFDD603}">
   <dimension ref="B2:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118:F118"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1121,10 +1122,10 @@
       <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="J4" s="9"/>
@@ -1137,11 +1138,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="19"/>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="20" t="s">
         <v>3</v>
       </c>
@@ -1158,16 +1159,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="38"/>
       <c r="G6" s="22"/>
       <c r="H6" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="25" t="s">
+      <c r="J6" s="24" t="s">
         <v>7</v>
       </c>
       <c r="K6" t="s">
@@ -1179,11 +1180,11 @@
         <v>2</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
       <c r="G7" s="22"/>
       <c r="H7" s="6" t="s">
         <v>11</v>
@@ -1194,11 +1195,11 @@
         <v>3</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="37"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="10"/>
       <c r="H8" s="14" t="s">
         <v>11</v>
@@ -1209,11 +1210,11 @@
         <v>4</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
       <c r="G9" s="23"/>
       <c r="H9" s="6" t="s">
         <v>46</v>
@@ -1224,11 +1225,11 @@
         <v>5</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="22"/>
       <c r="H10" s="14" t="s">
         <v>45</v>
@@ -1239,11 +1240,11 @@
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="31"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
       <c r="G11" s="10"/>
       <c r="H11" s="6"/>
     </row>
@@ -1252,11 +1253,11 @@
         <v>7</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="37"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
       <c r="G12" s="23"/>
       <c r="H12" s="14"/>
     </row>
@@ -1265,11 +1266,11 @@
         <v>8</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
       <c r="G13" s="23"/>
       <c r="H13" s="6"/>
     </row>
@@ -1278,11 +1279,11 @@
         <v>9</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="37"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="23"/>
       <c r="H14" s="14"/>
     </row>
@@ -1291,11 +1292,11 @@
         <v>10</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
       <c r="G15" s="23"/>
       <c r="H15" s="6" t="s">
         <v>11</v>
@@ -1306,11 +1307,11 @@
         <v>11</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="37"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="23"/>
       <c r="H16" s="14"/>
     </row>
@@ -1319,11 +1320,11 @@
         <v>12</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
       <c r="G17" s="23"/>
       <c r="H17" s="4"/>
     </row>
@@ -1332,11 +1333,11 @@
         <v>13</v>
       </c>
       <c r="C18" s="16"/>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="34"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="38"/>
       <c r="G18" s="23"/>
       <c r="H18" s="16"/>
     </row>
@@ -1345,11 +1346,11 @@
         <v>14</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
       <c r="G19" s="23"/>
       <c r="H19" s="4"/>
     </row>
@@ -1358,11 +1359,11 @@
         <v>15</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="36"/>
-      <c r="F20" s="37"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
       <c r="G20" s="23"/>
       <c r="H20" s="7"/>
     </row>
@@ -1371,11 +1372,11 @@
         <v>16</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="29" t="s">
+      <c r="D21" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="31"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
       <c r="G21" s="23"/>
       <c r="H21" s="4"/>
     </row>
@@ -1384,11 +1385,11 @@
         <v>17</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="37"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
       <c r="G22" s="23"/>
       <c r="H22" s="7"/>
     </row>
@@ -1397,11 +1398,11 @@
         <v>18</v>
       </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="30"/>
-      <c r="F23" s="31"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="23"/>
       <c r="H23" s="4"/>
     </row>
@@ -1410,11 +1411,11 @@
         <v>19</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="30"/>
       <c r="G24" s="23"/>
       <c r="H24" s="7"/>
     </row>
@@ -1423,11 +1424,11 @@
         <v>20</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="23"/>
       <c r="H25" s="4"/>
     </row>
@@ -1436,11 +1437,11 @@
         <v>21</v>
       </c>
       <c r="C26" s="7"/>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="37"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
       <c r="G26" s="23"/>
       <c r="H26" s="7"/>
     </row>
@@ -1449,11 +1450,11 @@
         <v>22</v>
       </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="33"/>
       <c r="G27" s="23"/>
       <c r="H27" s="4"/>
     </row>
@@ -1462,11 +1463,11 @@
         <v>23</v>
       </c>
       <c r="C28" s="16"/>
-      <c r="D28" s="32" t="s">
+      <c r="D28" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="38"/>
       <c r="G28" s="23"/>
       <c r="H28" s="16"/>
     </row>
@@ -1475,11 +1476,11 @@
         <v>24</v>
       </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
       <c r="G29" s="23"/>
       <c r="H29" s="4"/>
     </row>
@@ -1488,11 +1489,11 @@
         <v>25</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="36"/>
-      <c r="F30" s="37"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
       <c r="G30" s="23"/>
       <c r="H30" s="7"/>
     </row>
@@ -1501,11 +1502,11 @@
         <v>26</v>
       </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="29" t="s">
+      <c r="D31" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="30"/>
-      <c r="F31" s="31"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="23"/>
       <c r="H31" s="4" t="s">
         <v>44</v>
@@ -1516,13 +1517,13 @@
         <v>27</v>
       </c>
       <c r="C32" s="7"/>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="E32" s="36"/>
-      <c r="F32" s="37"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30"/>
       <c r="G32" s="23"/>
-      <c r="H32" s="28" t="s">
+      <c r="H32" s="27" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1531,11 +1532,11 @@
         <v>28</v>
       </c>
       <c r="C33" s="4"/>
-      <c r="D33" s="29" t="s">
+      <c r="D33" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="33"/>
       <c r="G33" s="23"/>
       <c r="H33" s="4"/>
     </row>
@@ -1544,11 +1545,11 @@
         <v>29</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="37"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="30"/>
       <c r="G34" s="23"/>
       <c r="H34" s="7"/>
     </row>
@@ -1557,11 +1558,11 @@
         <v>30</v>
       </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="29" t="s">
+      <c r="D35" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="30"/>
-      <c r="F35" s="31"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
       <c r="G35" s="23"/>
       <c r="H35" s="4"/>
     </row>
@@ -1570,11 +1571,11 @@
         <v>31</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="37"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
       <c r="G36" s="23"/>
       <c r="H36" s="7"/>
     </row>
@@ -1583,24 +1584,24 @@
         <v>32</v>
       </c>
       <c r="C37" s="4"/>
-      <c r="D37" s="29" t="s">
+      <c r="D37" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
       <c r="G37" s="23"/>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="26">
+      <c r="B38" s="25">
         <v>33</v>
       </c>
       <c r="C38" s="16"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="E38" s="33"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="38"/>
       <c r="G38" s="23"/>
       <c r="H38" s="16"/>
     </row>
@@ -1609,11 +1610,11 @@
         <v>34</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
+      <c r="E39" s="32"/>
+      <c r="F39" s="33"/>
       <c r="G39" s="23"/>
       <c r="H39" s="4"/>
     </row>
@@ -1621,10 +1622,10 @@
       <c r="B42" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="38" t="s">
+      <c r="C42" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="38"/>
+      <c r="D42" s="39"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
     </row>
@@ -1633,11 +1634,11 @@
         <v>1</v>
       </c>
       <c r="C43" s="19"/>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
       <c r="G43" s="20" t="s">
         <v>3</v>
       </c>
@@ -1650,11 +1651,11 @@
         <v>1</v>
       </c>
       <c r="C44" s="16"/>
-      <c r="D44" s="32" t="s">
+      <c r="D44" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="33"/>
-      <c r="F44" s="34"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="38"/>
       <c r="G44" s="23"/>
       <c r="H44" s="17"/>
     </row>
@@ -1663,11 +1664,11 @@
         <v>2</v>
       </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="29" t="s">
+      <c r="D45" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="30"/>
-      <c r="F45" s="31"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
       <c r="G45" s="23"/>
       <c r="H45" s="6"/>
     </row>
@@ -1676,11 +1677,11 @@
         <v>3</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="35" t="s">
+      <c r="D46" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="36"/>
-      <c r="F46" s="37"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="30"/>
       <c r="G46" s="23"/>
       <c r="H46" s="14"/>
     </row>
@@ -1689,11 +1690,11 @@
         <v>4</v>
       </c>
       <c r="C47" s="4"/>
-      <c r="D47" s="29" t="s">
+      <c r="D47" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="30"/>
-      <c r="F47" s="31"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
       <c r="G47" s="23"/>
       <c r="H47" s="6" t="s">
         <v>90</v>
@@ -1704,11 +1705,11 @@
         <v>5</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="35" t="s">
+      <c r="D48" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E48" s="36"/>
-      <c r="F48" s="37"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="30"/>
       <c r="G48" s="23"/>
       <c r="H48" s="14"/>
     </row>
@@ -1717,11 +1718,11 @@
         <v>6</v>
       </c>
       <c r="C49" s="4"/>
-      <c r="D49" s="29" t="s">
+      <c r="D49" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="30"/>
-      <c r="F49" s="31"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
       <c r="G49" s="23"/>
       <c r="H49" s="6"/>
     </row>
@@ -1730,11 +1731,11 @@
         <v>7</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="35" t="s">
+      <c r="D50" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E50" s="36"/>
-      <c r="F50" s="37"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="30"/>
       <c r="G50" s="23"/>
       <c r="H50" s="14" t="s">
         <v>58</v>
@@ -1745,11 +1746,11 @@
         <v>8</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="35" t="s">
+      <c r="D51" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="E51" s="36"/>
-      <c r="F51" s="37"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="30"/>
       <c r="G51" s="23"/>
       <c r="H51" s="14"/>
     </row>
@@ -1757,10 +1758,10 @@
       <c r="B53" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C53" s="38" t="s">
+      <c r="C53" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="38"/>
+      <c r="D53" s="39"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
     </row>
@@ -1769,11 +1770,11 @@
         <v>1</v>
       </c>
       <c r="C54" s="19"/>
-      <c r="D54" s="39" t="s">
+      <c r="D54" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="39"/>
-      <c r="F54" s="39"/>
+      <c r="E54" s="35"/>
+      <c r="F54" s="35"/>
       <c r="G54" s="20" t="s">
         <v>3</v>
       </c>
@@ -1786,11 +1787,11 @@
         <v>1</v>
       </c>
       <c r="C55" s="16"/>
-      <c r="D55" s="32" t="s">
+      <c r="D55" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="E55" s="33"/>
-      <c r="F55" s="34"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="38"/>
       <c r="G55" s="23"/>
       <c r="H55" s="15"/>
     </row>
@@ -1799,11 +1800,11 @@
         <v>2</v>
       </c>
       <c r="C56" s="4"/>
-      <c r="D56" s="29" t="s">
+      <c r="D56" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="E56" s="30"/>
-      <c r="F56" s="31"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="33"/>
       <c r="G56" s="23"/>
       <c r="H56" s="5"/>
     </row>
@@ -1812,11 +1813,11 @@
         <v>3</v>
       </c>
       <c r="C57" s="7"/>
-      <c r="D57" s="35" t="s">
+      <c r="D57" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="E57" s="36"/>
-      <c r="F57" s="37"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="30"/>
       <c r="G57" s="23"/>
       <c r="H57" s="13"/>
     </row>
@@ -1825,11 +1826,11 @@
         <v>4</v>
       </c>
       <c r="C58" s="4"/>
-      <c r="D58" s="29" t="s">
+      <c r="D58" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="30"/>
-      <c r="F58" s="31"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="33"/>
       <c r="G58" s="23"/>
       <c r="H58" s="5"/>
     </row>
@@ -1838,11 +1839,11 @@
         <v>5</v>
       </c>
       <c r="C59" s="7"/>
-      <c r="D59" s="35" t="s">
+      <c r="D59" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="36"/>
-      <c r="F59" s="37"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="30"/>
       <c r="G59" s="23"/>
       <c r="H59" s="13"/>
     </row>
@@ -1851,11 +1852,11 @@
         <v>6</v>
       </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="29" t="s">
+      <c r="D60" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="E60" s="30"/>
-      <c r="F60" s="31"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="33"/>
       <c r="G60" s="23"/>
       <c r="H60" s="5"/>
     </row>
@@ -1864,11 +1865,11 @@
         <v>7</v>
       </c>
       <c r="C61" s="7"/>
-      <c r="D61" s="35" t="s">
+      <c r="D61" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="E61" s="36"/>
-      <c r="F61" s="37"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="30"/>
       <c r="G61" s="23"/>
       <c r="H61" s="13"/>
     </row>
@@ -1877,11 +1878,11 @@
         <v>8</v>
       </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="29" t="s">
+      <c r="D62" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="30"/>
-      <c r="F62" s="31"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="33"/>
       <c r="G62" s="23"/>
       <c r="H62" s="5"/>
     </row>
@@ -1890,11 +1891,11 @@
         <v>9</v>
       </c>
       <c r="C63" s="7"/>
-      <c r="D63" s="35" t="s">
+      <c r="D63" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="E63" s="36"/>
-      <c r="F63" s="37"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="30"/>
       <c r="G63" s="23"/>
       <c r="H63" s="13"/>
     </row>
@@ -1903,11 +1904,11 @@
         <v>10</v>
       </c>
       <c r="C64" s="4"/>
-      <c r="D64" s="29" t="s">
+      <c r="D64" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="30"/>
-      <c r="F64" s="31"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="33"/>
       <c r="G64" s="23"/>
       <c r="H64" s="5"/>
     </row>
@@ -1918,13 +1919,13 @@
       <c r="C65" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="35" t="s">
+      <c r="D65" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="36"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="27" t="s">
+      <c r="E65" s="29"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="42"/>
+      <c r="H65" s="26" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1932,10 +1933,10 @@
       <c r="B68" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C68" s="38" t="s">
+      <c r="C68" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="D68" s="38"/>
+      <c r="D68" s="39"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
     </row>
@@ -1944,11 +1945,11 @@
         <v>1</v>
       </c>
       <c r="C69" s="19"/>
-      <c r="D69" s="39" t="s">
+      <c r="D69" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E69" s="39"/>
-      <c r="F69" s="39"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="35"/>
       <c r="G69" s="20" t="s">
         <v>3</v>
       </c>
@@ -1961,11 +1962,11 @@
         <v>1</v>
       </c>
       <c r="C70" s="16"/>
-      <c r="D70" s="32" t="s">
+      <c r="D70" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="E70" s="33"/>
-      <c r="F70" s="34"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="38"/>
       <c r="G70" s="23"/>
       <c r="H70" s="15"/>
     </row>
@@ -1974,11 +1975,11 @@
         <v>2</v>
       </c>
       <c r="C71" s="4"/>
-      <c r="D71" s="29" t="s">
+      <c r="D71" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E71" s="30"/>
-      <c r="F71" s="31"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="33"/>
       <c r="G71" s="23"/>
       <c r="H71" s="5"/>
     </row>
@@ -1987,11 +1988,11 @@
         <v>3</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="D72" s="35" t="s">
+      <c r="D72" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E72" s="36"/>
-      <c r="F72" s="37"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="30"/>
       <c r="G72" s="23"/>
       <c r="H72" s="13"/>
     </row>
@@ -2000,11 +2001,11 @@
         <v>4</v>
       </c>
       <c r="C73" s="4"/>
-      <c r="D73" s="29" t="s">
+      <c r="D73" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="E73" s="30"/>
-      <c r="F73" s="31"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="33"/>
       <c r="G73" s="23"/>
       <c r="H73" s="5"/>
     </row>
@@ -2013,11 +2014,11 @@
         <v>5</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="D74" s="35" t="s">
+      <c r="D74" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="E74" s="36"/>
-      <c r="F74" s="37"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="30"/>
       <c r="G74" s="23"/>
       <c r="H74" s="13"/>
     </row>
@@ -2026,11 +2027,11 @@
         <v>6</v>
       </c>
       <c r="C75" s="4"/>
-      <c r="D75" s="29" t="s">
+      <c r="D75" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="E75" s="30"/>
-      <c r="F75" s="31"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="33"/>
       <c r="G75" s="23"/>
       <c r="H75" s="5"/>
     </row>
@@ -2038,10 +2039,10 @@
       <c r="B78" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C78" s="38" t="s">
+      <c r="C78" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="D78" s="38"/>
+      <c r="D78" s="39"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
     </row>
@@ -2050,11 +2051,11 @@
         <v>1</v>
       </c>
       <c r="C79" s="19"/>
-      <c r="D79" s="39" t="s">
+      <c r="D79" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E79" s="39"/>
-      <c r="F79" s="39"/>
+      <c r="E79" s="35"/>
+      <c r="F79" s="35"/>
       <c r="G79" s="20" t="s">
         <v>3</v>
       </c>
@@ -2067,11 +2068,11 @@
         <v>1</v>
       </c>
       <c r="C80" s="16"/>
-      <c r="D80" s="32" t="s">
+      <c r="D80" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="E80" s="33"/>
-      <c r="F80" s="34"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="38"/>
       <c r="G80" s="23"/>
       <c r="H80" s="15"/>
     </row>
@@ -2080,11 +2081,11 @@
         <v>2</v>
       </c>
       <c r="C81" s="4"/>
-      <c r="D81" s="29" t="s">
+      <c r="D81" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="E81" s="30"/>
-      <c r="F81" s="31"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="33"/>
       <c r="G81" s="23"/>
       <c r="H81" s="5"/>
     </row>
@@ -2093,11 +2094,11 @@
         <v>3</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="D82" s="35" t="s">
+      <c r="D82" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="E82" s="36"/>
-      <c r="F82" s="37"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="30"/>
       <c r="G82" s="23"/>
       <c r="H82" s="13"/>
     </row>
@@ -2106,11 +2107,11 @@
         <v>4</v>
       </c>
       <c r="C83" s="4"/>
-      <c r="D83" s="29" t="s">
+      <c r="D83" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="E83" s="30"/>
-      <c r="F83" s="31"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="33"/>
       <c r="G83" s="23"/>
       <c r="H83" s="5"/>
     </row>
@@ -2119,11 +2120,11 @@
         <v>5</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="35" t="s">
+      <c r="D84" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="E84" s="36"/>
-      <c r="F84" s="37"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="30"/>
       <c r="G84" s="23"/>
       <c r="H84" s="13"/>
     </row>
@@ -2132,11 +2133,11 @@
         <v>6</v>
       </c>
       <c r="C85" s="4"/>
-      <c r="D85" s="29" t="s">
+      <c r="D85" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="E85" s="30"/>
-      <c r="F85" s="31"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="33"/>
       <c r="G85" s="23"/>
       <c r="H85" s="5"/>
     </row>
@@ -2145,11 +2146,11 @@
         <v>7</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="35" t="s">
+      <c r="D86" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="E86" s="36"/>
-      <c r="F86" s="37"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="30"/>
       <c r="G86" s="23"/>
       <c r="H86" s="13"/>
     </row>
@@ -2158,11 +2159,11 @@
         <v>8</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="D87" s="29" t="s">
+      <c r="D87" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E87" s="30"/>
-      <c r="F87" s="31"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="33"/>
       <c r="G87" s="23"/>
       <c r="H87" s="5"/>
     </row>
@@ -2171,11 +2172,11 @@
         <v>9</v>
       </c>
       <c r="C88" s="16"/>
-      <c r="D88" s="32" t="s">
+      <c r="D88" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="E88" s="33"/>
-      <c r="F88" s="34"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="38"/>
       <c r="G88" s="23"/>
       <c r="H88" s="13"/>
     </row>
@@ -2184,11 +2185,11 @@
         <v>10</v>
       </c>
       <c r="C89" s="4"/>
-      <c r="D89" s="29" t="s">
+      <c r="D89" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E89" s="30"/>
-      <c r="F89" s="31"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="33"/>
       <c r="G89" s="23"/>
       <c r="H89" s="5"/>
     </row>
@@ -2197,11 +2198,11 @@
         <v>11</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="35" t="s">
+      <c r="D90" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="E90" s="36"/>
-      <c r="F90" s="37"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="30"/>
       <c r="G90" s="23"/>
       <c r="H90" s="13"/>
     </row>
@@ -2210,11 +2211,11 @@
         <v>12</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="D91" s="29" t="s">
+      <c r="D91" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E91" s="30"/>
-      <c r="F91" s="31"/>
+      <c r="E91" s="32"/>
+      <c r="F91" s="33"/>
       <c r="G91" s="23"/>
       <c r="H91" s="5"/>
     </row>
@@ -2223,11 +2224,11 @@
         <v>13</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="35" t="s">
+      <c r="D92" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="E92" s="36"/>
-      <c r="F92" s="37"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="30"/>
       <c r="G92" s="23"/>
       <c r="H92" s="15"/>
     </row>
@@ -2236,11 +2237,11 @@
         <v>14</v>
       </c>
       <c r="C93" s="4"/>
-      <c r="D93" s="29" t="s">
+      <c r="D93" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E93" s="30"/>
-      <c r="F93" s="31"/>
+      <c r="E93" s="32"/>
+      <c r="F93" s="33"/>
       <c r="G93" s="23"/>
       <c r="H93" s="5"/>
     </row>
@@ -2249,11 +2250,11 @@
         <v>15</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="35" t="s">
+      <c r="D94" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="E94" s="36"/>
-      <c r="F94" s="37"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="30"/>
       <c r="G94" s="23"/>
       <c r="H94" s="13"/>
     </row>
@@ -2262,11 +2263,11 @@
         <v>16</v>
       </c>
       <c r="C95" s="4"/>
-      <c r="D95" s="29" t="s">
+      <c r="D95" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E95" s="30"/>
-      <c r="F95" s="31"/>
+      <c r="E95" s="32"/>
+      <c r="F95" s="33"/>
       <c r="G95" s="23"/>
       <c r="H95" s="5"/>
     </row>
@@ -2275,11 +2276,11 @@
         <v>17</v>
       </c>
       <c r="C96" s="16"/>
-      <c r="D96" s="32" t="s">
+      <c r="D96" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="E96" s="33"/>
-      <c r="F96" s="34"/>
+      <c r="E96" s="37"/>
+      <c r="F96" s="38"/>
       <c r="G96" s="23"/>
       <c r="H96" s="13"/>
     </row>
@@ -2287,10 +2288,10 @@
       <c r="B99" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C99" s="38" t="s">
+      <c r="C99" s="39" t="s">
         <v>81</v>
       </c>
-      <c r="D99" s="38"/>
+      <c r="D99" s="39"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
     </row>
@@ -2299,11 +2300,11 @@
         <v>1</v>
       </c>
       <c r="C100" s="19"/>
-      <c r="D100" s="39" t="s">
+      <c r="D100" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E100" s="39"/>
-      <c r="F100" s="39"/>
+      <c r="E100" s="35"/>
+      <c r="F100" s="35"/>
       <c r="G100" s="20" t="s">
         <v>3</v>
       </c>
@@ -2316,11 +2317,11 @@
         <v>1</v>
       </c>
       <c r="C101" s="16"/>
-      <c r="D101" s="32" t="s">
+      <c r="D101" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="E101" s="33"/>
-      <c r="F101" s="34"/>
+      <c r="E101" s="37"/>
+      <c r="F101" s="38"/>
       <c r="G101" s="23"/>
       <c r="H101" s="17"/>
     </row>
@@ -2329,11 +2330,11 @@
         <v>2</v>
       </c>
       <c r="C102" s="16"/>
-      <c r="D102" s="32" t="s">
+      <c r="D102" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="E102" s="33"/>
-      <c r="F102" s="34"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="38"/>
       <c r="G102" s="23"/>
       <c r="H102" s="17"/>
     </row>
@@ -2341,10 +2342,10 @@
       <c r="B104" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C104" s="38" t="s">
+      <c r="C104" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="D104" s="38"/>
+      <c r="D104" s="39"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
@@ -2353,11 +2354,11 @@
         <v>1</v>
       </c>
       <c r="C105" s="19"/>
-      <c r="D105" s="39" t="s">
+      <c r="D105" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E105" s="39"/>
-      <c r="F105" s="39"/>
+      <c r="E105" s="35"/>
+      <c r="F105" s="35"/>
       <c r="G105" s="20" t="s">
         <v>3</v>
       </c>
@@ -2370,11 +2371,11 @@
         <v>1</v>
       </c>
       <c r="C106" s="16"/>
-      <c r="D106" s="32" t="s">
+      <c r="D106" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="E106" s="33"/>
-      <c r="F106" s="34"/>
+      <c r="E106" s="37"/>
+      <c r="F106" s="38"/>
       <c r="G106" s="23"/>
       <c r="H106" s="17"/>
     </row>
@@ -2382,10 +2383,10 @@
       <c r="B109" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C109" s="38" t="s">
+      <c r="C109" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="D109" s="38"/>
+      <c r="D109" s="39"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
     </row>
@@ -2394,11 +2395,11 @@
         <v>1</v>
       </c>
       <c r="C110" s="19"/>
-      <c r="D110" s="39" t="s">
+      <c r="D110" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E110" s="39"/>
-      <c r="F110" s="39"/>
+      <c r="E110" s="35"/>
+      <c r="F110" s="35"/>
       <c r="G110" s="20" t="s">
         <v>3</v>
       </c>
@@ -2411,11 +2412,11 @@
         <v>1</v>
       </c>
       <c r="C111" s="16"/>
-      <c r="D111" s="32" t="s">
+      <c r="D111" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="E111" s="33"/>
-      <c r="F111" s="34"/>
+      <c r="E111" s="37"/>
+      <c r="F111" s="38"/>
       <c r="G111" s="23"/>
       <c r="H111" s="17"/>
     </row>
@@ -2424,11 +2425,11 @@
         <v>2</v>
       </c>
       <c r="C112" s="4"/>
-      <c r="D112" s="29" t="s">
+      <c r="D112" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="E112" s="30"/>
-      <c r="F112" s="31"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="33"/>
       <c r="G112" s="23"/>
       <c r="H112" s="6"/>
     </row>
@@ -2437,11 +2438,11 @@
         <v>3</v>
       </c>
       <c r="C113" s="7"/>
-      <c r="D113" s="35" t="s">
+      <c r="D113" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="E113" s="36"/>
-      <c r="F113" s="37"/>
+      <c r="E113" s="29"/>
+      <c r="F113" s="30"/>
       <c r="G113" s="23"/>
       <c r="H113" s="14"/>
     </row>
@@ -2450,11 +2451,11 @@
         <v>4</v>
       </c>
       <c r="C114" s="4"/>
-      <c r="D114" s="29" t="s">
+      <c r="D114" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E114" s="30"/>
-      <c r="F114" s="31"/>
+      <c r="E114" s="32"/>
+      <c r="F114" s="33"/>
       <c r="G114" s="23"/>
       <c r="H114" s="6"/>
     </row>
@@ -2462,21 +2463,21 @@
       <c r="B116" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C116" s="41" t="s">
+      <c r="C116" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="D116" s="41"/>
+      <c r="D116" s="34"/>
     </row>
     <row r="117" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C117" s="19"/>
-      <c r="D117" s="39" t="s">
+      <c r="D117" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E117" s="39"/>
-      <c r="F117" s="39"/>
+      <c r="E117" s="35"/>
+      <c r="F117" s="35"/>
       <c r="G117" s="20" t="s">
         <v>3</v>
       </c>
@@ -2489,12 +2490,12 @@
         <v>1</v>
       </c>
       <c r="C118" s="16"/>
-      <c r="D118" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="E118" s="33"/>
-      <c r="F118" s="34"/>
-      <c r="G118" s="9"/>
+      <c r="D118" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E118" s="37"/>
+      <c r="F118" s="38"/>
+      <c r="G118" s="23"/>
       <c r="H118" s="17"/>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.3">
@@ -2502,12 +2503,12 @@
         <v>2</v>
       </c>
       <c r="C119" s="4"/>
-      <c r="D119" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="E119" s="30"/>
-      <c r="F119" s="31"/>
-      <c r="G119" s="24"/>
+      <c r="D119" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="E119" s="32"/>
+      <c r="F119" s="33"/>
+      <c r="G119" s="23"/>
       <c r="H119" s="6"/>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.3">
@@ -2515,27 +2516,107 @@
         <v>3</v>
       </c>
       <c r="C120" s="7"/>
-      <c r="D120" s="35" t="s">
-        <v>112</v>
-      </c>
-      <c r="E120" s="36"/>
-      <c r="F120" s="37"/>
-      <c r="G120" s="24"/>
+      <c r="D120" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E120" s="29"/>
+      <c r="F120" s="30"/>
+      <c r="G120" s="23"/>
       <c r="H120" s="14"/>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B121" s="5">
-        <v>4</v>
-      </c>
+      <c r="B121" s="5"/>
       <c r="C121" s="4"/>
-      <c r="D121" s="29"/>
-      <c r="E121" s="30"/>
-      <c r="F121" s="31"/>
-      <c r="G121" s="24"/>
+      <c r="D121" s="31"/>
+      <c r="E121" s="32"/>
+      <c r="F121" s="33"/>
+      <c r="G121" s="41"/>
       <c r="H121" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="106">
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D39:F39"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D48:F48"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D102:F102"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="D63:F63"/>
+    <mergeCell ref="D64:F64"/>
+    <mergeCell ref="D65:F65"/>
+    <mergeCell ref="D54:F54"/>
+    <mergeCell ref="D55:F55"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="D31:F31"/>
+    <mergeCell ref="D32:F32"/>
+    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D70:F70"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D71:F71"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="D87:F87"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D72:F72"/>
+    <mergeCell ref="D73:F73"/>
+    <mergeCell ref="D74:F74"/>
+    <mergeCell ref="D75:F75"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D86:F86"/>
     <mergeCell ref="D120:F120"/>
     <mergeCell ref="D121:F121"/>
     <mergeCell ref="D51:F51"/>
@@ -2560,88 +2641,6 @@
     <mergeCell ref="D88:F88"/>
     <mergeCell ref="D89:F89"/>
     <mergeCell ref="D90:F90"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D71:F71"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="D87:F87"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D31:F31"/>
-    <mergeCell ref="D32:F32"/>
-    <mergeCell ref="D33:F33"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="D36:F36"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="D26:F26"/>
-    <mergeCell ref="D27:F27"/>
-    <mergeCell ref="D28:F28"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D39:F39"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D48:F48"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D102:F102"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="D63:F63"/>
-    <mergeCell ref="D64:F64"/>
-    <mergeCell ref="D65:F65"/>
-    <mergeCell ref="D54:F54"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D57:F57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>